<commit_message>
Added batteries and other new and updated recipes. Batteries do not work yet properly as fuel.
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="54375" yWindow="495" windowWidth="19200" windowHeight="19455" tabRatio="877"/>
+    <workbookView xWindow="57495" yWindow="495" windowWidth="19200" windowHeight="19455" tabRatio="877"/>
   </bookViews>
   <sheets>
     <sheet name="Custom Objects" sheetId="41" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2092" uniqueCount="2066">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2187" uniqueCount="2161">
   <si>
     <t>Ore</t>
   </si>
@@ -6239,6 +6239,291 @@
   </si>
   <si>
     <t>Internal Object</t>
+  </si>
+  <si>
+    <t>11u</t>
+  </si>
+  <si>
+    <t>11t</t>
+  </si>
+  <si>
+    <t>11s</t>
+  </si>
+  <si>
+    <t>11r</t>
+  </si>
+  <si>
+    <t>11y</t>
+  </si>
+  <si>
+    <t>11x</t>
+  </si>
+  <si>
+    <t>11w</t>
+  </si>
+  <si>
+    <t>11v</t>
+  </si>
+  <si>
+    <t>11C</t>
+  </si>
+  <si>
+    <t>11B</t>
+  </si>
+  <si>
+    <t>11A</t>
+  </si>
+  <si>
+    <t>11z</t>
+  </si>
+  <si>
+    <t>11G</t>
+  </si>
+  <si>
+    <t>11F</t>
+  </si>
+  <si>
+    <t>11E</t>
+  </si>
+  <si>
+    <t>11D</t>
+  </si>
+  <si>
+    <t>11W</t>
+  </si>
+  <si>
+    <t>11V</t>
+  </si>
+  <si>
+    <t>11U</t>
+  </si>
+  <si>
+    <t>11T</t>
+  </si>
+  <si>
+    <t>11S</t>
+  </si>
+  <si>
+    <t>11R</t>
+  </si>
+  <si>
+    <t>11Q</t>
+  </si>
+  <si>
+    <t>11P</t>
+  </si>
+  <si>
+    <t>11O</t>
+  </si>
+  <si>
+    <t>11N</t>
+  </si>
+  <si>
+    <t>11M</t>
+  </si>
+  <si>
+    <t>11L</t>
+  </si>
+  <si>
+    <t>11K</t>
+  </si>
+  <si>
+    <t>11J</t>
+  </si>
+  <si>
+    <t>11I</t>
+  </si>
+  <si>
+    <t>11H</t>
+  </si>
+  <si>
+    <t>12c</t>
+  </si>
+  <si>
+    <t>12b</t>
+  </si>
+  <si>
+    <t>12a</t>
+  </si>
+  <si>
+    <t>129</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>11Z</t>
+  </si>
+  <si>
+    <t>11Y</t>
+  </si>
+  <si>
+    <t>11X</t>
+  </si>
+  <si>
+    <t>12s</t>
+  </si>
+  <si>
+    <t>12r</t>
+  </si>
+  <si>
+    <t>12q</t>
+  </si>
+  <si>
+    <t>12p</t>
+  </si>
+  <si>
+    <t>12o</t>
+  </si>
+  <si>
+    <t>12n</t>
+  </si>
+  <si>
+    <t>12m</t>
+  </si>
+  <si>
+    <t>12l</t>
+  </si>
+  <si>
+    <t>12k</t>
+  </si>
+  <si>
+    <t>12j</t>
+  </si>
+  <si>
+    <t>12i</t>
+  </si>
+  <si>
+    <t>12h</t>
+  </si>
+  <si>
+    <t>12g</t>
+  </si>
+  <si>
+    <t>12f</t>
+  </si>
+  <si>
+    <t>12e</t>
+  </si>
+  <si>
+    <t>12d</t>
+  </si>
+  <si>
+    <t>12I</t>
+  </si>
+  <si>
+    <t>12H</t>
+  </si>
+  <si>
+    <t>12G</t>
+  </si>
+  <si>
+    <t>12F</t>
+  </si>
+  <si>
+    <t>12E</t>
+  </si>
+  <si>
+    <t>12D</t>
+  </si>
+  <si>
+    <t>12C</t>
+  </si>
+  <si>
+    <t>12B</t>
+  </si>
+  <si>
+    <t>12A</t>
+  </si>
+  <si>
+    <t>12z</t>
+  </si>
+  <si>
+    <t>12y</t>
+  </si>
+  <si>
+    <t>12x</t>
+  </si>
+  <si>
+    <t>12w</t>
+  </si>
+  <si>
+    <t>12v</t>
+  </si>
+  <si>
+    <t>12u</t>
+  </si>
+  <si>
+    <t>12t</t>
+  </si>
+  <si>
+    <t>12J</t>
+  </si>
+  <si>
+    <t>12K</t>
+  </si>
+  <si>
+    <t>Lead-Acid Battery (1-Cell)</t>
+  </si>
+  <si>
+    <t>Lead-Acid Battery (9-Cell)</t>
+  </si>
+  <si>
+    <t>Lithium Ion Battery (1-Cell)</t>
+  </si>
+  <si>
+    <t>Lithium Ion Battery (9-Cell)</t>
+  </si>
+  <si>
+    <t>Nickel Metal Hydride Battery (1-Cell)</t>
+  </si>
+  <si>
+    <t>12S</t>
+  </si>
+  <si>
+    <t>12R</t>
+  </si>
+  <si>
+    <t>12Q</t>
+  </si>
+  <si>
+    <t>12P</t>
+  </si>
+  <si>
+    <t>12O</t>
+  </si>
+  <si>
+    <t>12N</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>Nickel Metal Hydride Battery (9-Cell)</t>
   </si>
 </sst>
 </file>
@@ -11751,6 +12036,97 @@
             <v>Liquid</v>
           </cell>
         </row>
+        <row r="342">
+          <cell r="B342" t="str">
+            <v>Lactide</v>
+          </cell>
+          <cell r="D342" t="str">
+            <v>Liquid</v>
+          </cell>
+        </row>
+        <row r="343">
+          <cell r="B343" t="str">
+            <v>Cyclodextrin</v>
+          </cell>
+          <cell r="D343" t="str">
+            <v>Solid</v>
+          </cell>
+        </row>
+        <row r="344">
+          <cell r="B344" t="str">
+            <v>Alpha-cyclodextrin</v>
+          </cell>
+          <cell r="D344" t="str">
+            <v>Solid</v>
+          </cell>
+        </row>
+        <row r="345">
+          <cell r="B345" t="str">
+            <v>Beta-cyclodextrin</v>
+          </cell>
+          <cell r="D345" t="str">
+            <v>Solid</v>
+          </cell>
+        </row>
+        <row r="346">
+          <cell r="B346" t="str">
+            <v>Gamma-cyclodextrin</v>
+          </cell>
+          <cell r="D346" t="str">
+            <v>Solid</v>
+          </cell>
+        </row>
+        <row r="347">
+          <cell r="B347" t="str">
+            <v>MOF-5</v>
+          </cell>
+          <cell r="D347" t="str">
+            <v>Solid</v>
+          </cell>
+        </row>
+        <row r="348">
+          <cell r="B348" t="str">
+            <v>CD-MOF</v>
+          </cell>
+          <cell r="D348" t="str">
+            <v>Solid</v>
+          </cell>
+        </row>
+        <row r="349">
+          <cell r="B349" t="str">
+            <v>Bucky Balls (C60)</v>
+          </cell>
+          <cell r="D349" t="str">
+            <v>Solid</v>
+          </cell>
+        </row>
+        <row r="350">
+          <cell r="B350" t="str">
+            <v>Zinc Nitrate</v>
+          </cell>
+          <cell r="D350" t="str">
+            <v>Solid</v>
+          </cell>
+        </row>
+        <row r="351">
+          <cell r="B351" t="str">
+            <v>Lead Oxide</v>
+          </cell>
+          <cell r="D351" t="str">
+            <v>Solid</v>
+          </cell>
+        </row>
+        <row r="352">
+          <cell r="B352" t="str">
+            <v>Lithium Hexafluorophosphate</v>
+          </cell>
+          <cell r="C352" t="str">
+            <v>LiPF6</v>
+          </cell>
+          <cell r="D352" t="str">
+            <v>Solid</v>
+          </cell>
+        </row>
       </sheetData>
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
@@ -12052,14 +12428,14 @@
   <dimension ref="A1:R66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="27"/>
     <col min="2" max="2" width="8.85546875" style="26"/>
-    <col min="3" max="3" width="33.42578125" style="26" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" style="26" customWidth="1"/>
     <col min="4" max="4" width="12.140625" style="26" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" style="26"/>
     <col min="6" max="6" width="17.42578125" style="26" customWidth="1"/>
@@ -12998,35 +13374,142 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="29"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="27"/>
+      <c r="A36" s="29" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>2158</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D36" s="28" t="str">
+        <f>[1]Enums!$A$40</f>
+        <v>PC Item</v>
+      </c>
+      <c r="E36" s="26">
+        <v>8</v>
+      </c>
       <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
+      <c r="H36" s="28">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="29"/>
-      <c r="C37" s="28"/>
+      <c r="A37" s="29" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>2157</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>2149</v>
+      </c>
+      <c r="D37" s="28" t="str">
+        <f>[1]Enums!$A$40</f>
+        <v>PC Item</v>
+      </c>
+      <c r="E37" s="26">
+        <v>8</v>
+      </c>
       <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
+      <c r="H37" s="28">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="29"/>
-      <c r="C38" s="28"/>
+      <c r="A38" s="29" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>2156</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>2150</v>
+      </c>
+      <c r="D38" s="28" t="str">
+        <f>[1]Enums!$A$40</f>
+        <v>PC Item</v>
+      </c>
+      <c r="E38" s="26">
+        <v>8</v>
+      </c>
       <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
+      <c r="H38" s="28">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A39" s="29" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>2155</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>2151</v>
+      </c>
+      <c r="D39" s="28" t="str">
+        <f>[1]Enums!$A$40</f>
+        <v>PC Item</v>
+      </c>
+      <c r="E39" s="26">
+        <v>8</v>
+      </c>
       <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
+      <c r="H39" s="28">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A40" s="29" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>2154</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>2152</v>
+      </c>
+      <c r="D40" s="28" t="str">
+        <f>[1]Enums!$A$40</f>
+        <v>PC Item</v>
+      </c>
+      <c r="E40" s="26">
+        <v>8</v>
+      </c>
       <c r="G40" s="28"/>
-      <c r="H40" s="28"/>
+      <c r="H40" s="28">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="29" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C41" s="26" t="s">
+        <v>2160</v>
+      </c>
+      <c r="D41" s="28" t="str">
+        <f>[1]Enums!$A$40</f>
+        <v>PC Item</v>
+      </c>
+      <c r="E41" s="26">
+        <v>8</v>
+      </c>
       <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
+      <c r="H41" s="28">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="G42" s="28"/>
@@ -13149,7 +13632,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13290,7 +13773,7 @@
   <dimension ref="A1:R120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13975,10 +14458,10 @@
         <v>5</v>
       </c>
       <c r="J12" s="8">
+        <v>2</v>
+      </c>
+      <c r="K12" s="8">
         <v>5</v>
-      </c>
-      <c r="K12" s="8">
-        <v>7</v>
       </c>
       <c r="L12" s="8">
         <v>10</v>
@@ -14194,7 +14677,7 @@
         <v>11</v>
       </c>
       <c r="L16" s="8">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M16" s="8">
         <v>60</v>
@@ -16344,10 +16827,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16550,7 +17033,7 @@
         <v>74</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" ref="C10:C30" si="1">E10&amp;" "&amp;$C$1</f>
+        <f t="shared" ref="C10:C32" si="1">E10&amp;" "&amp;$C$1</f>
         <v>Antimony Trioxide Catalyst</v>
       </c>
       <c r="D10" t="str">
@@ -16944,6 +17427,69 @@
       <c r="E30" t="str">
         <f>[1]Compounds!$B$337</f>
         <v>Chromia Alumina</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>2147</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="1"/>
+        <v>Tin Catalyst</v>
+      </c>
+      <c r="D31" t="str">
+        <f>[1]Elements!$B$1</f>
+        <v>Element</v>
+      </c>
+      <c r="E31" t="str">
+        <f>[1]Elements!$B$51</f>
+        <v>Tin</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>2146</v>
+      </c>
+      <c r="C32" t="str">
+        <f>E32&amp;" "&amp;$C$1</f>
+        <v>Zinc Nitrate Catalyst</v>
+      </c>
+      <c r="D32" t="str">
+        <f>[1]Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="E32" t="str">
+        <f>[1]Compounds!$B$350</f>
+        <v>Zinc Nitrate</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>2159</v>
+      </c>
+      <c r="C33" t="str">
+        <f>E33&amp;" "&amp;$C$1</f>
+        <v>Lead Oxide Catalyst</v>
+      </c>
+      <c r="D33" t="str">
+        <f>[1]Compounds!$B$1</f>
+        <v>Compound</v>
+      </c>
+      <c r="E33" t="str">
+        <f>[1]Compounds!$B$351</f>
+        <v>Lead Oxide</v>
       </c>
     </row>
   </sheetData>
@@ -24363,10 +24909,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:O334"/>
+  <dimension ref="A1:O353"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="A304" workbookViewId="0">
+      <selection activeCell="B341" sqref="B341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -43156,7 +43702,10 @@
       </c>
     </row>
     <row r="333" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A333" s="4"/>
+      <c r="A333" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
       <c r="B333" s="13" t="s">
         <v>607</v>
       </c>
@@ -43171,47 +43720,758 @@
       </c>
       <c r="F333" s="16" t="str">
         <f t="shared" si="24"/>
-        <v>Bag (0)</v>
+        <v>Vial (Lactide)</v>
       </c>
       <c r="G333" s="16" t="str">
         <f t="shared" si="25"/>
-        <v>Sack (0)</v>
+        <v>Beaker (Lactide)</v>
       </c>
       <c r="H333" s="16" t="str">
         <f t="shared" si="26"/>
-        <v>Powder Keg (0)</v>
+        <v>Drum (Lactide)</v>
       </c>
       <c r="I333" s="16" t="str">
         <f t="shared" si="27"/>
-        <v>Chemical Silo (0)</v>
-      </c>
-      <c r="J333" s="16">
+        <v>Chemical Vat (Lactide)</v>
+      </c>
+      <c r="J333" s="16" t="str">
         <f>[1]Compounds!$B342</f>
-        <v>0</v>
-      </c>
-      <c r="K333">
+        <v>Lactide</v>
+      </c>
+      <c r="K333" t="str">
         <f>[1]Compounds!$D342</f>
-        <v>0</v>
+        <v>Liquid</v>
       </c>
       <c r="L333" s="4" t="str">
         <f>IF(K333=[1]Enums!$A$18, [1]Enums!$A$23, IF(K333=[1]Enums!$B$22, [1]Enums!$A$22, [1]Enums!$A$21))</f>
-        <v>Bag</v>
+        <v>Vial</v>
       </c>
       <c r="M333" s="4" t="str">
         <f>IF(K333=[1]Enums!$A$18, [1]Enums!$A$26, IF(K333=[1]Enums!$B$25, [1]Enums!$A$25, [1]Enums!$A$24))</f>
-        <v>Sack</v>
+        <v>Beaker</v>
       </c>
       <c r="N333" s="4" t="str">
         <f>IF(K333=[1]Enums!$A$18, [1]Enums!$A$29, IF(K333=[1]Enums!$B$22, [1]Enums!$A$28, [1]Enums!$A$27))</f>
-        <v>Powder Keg</v>
+        <v>Drum</v>
       </c>
       <c r="O333" s="4" t="str">
         <f>IF(K333=[1]Enums!$A$18, [1]Enums!$A$32, IF(K333=[1]Enums!$B$22, [1]Enums!$A$31, [1]Enums!$A$30))</f>
+        <v>Chemical Vat</v>
+      </c>
+    </row>
+    <row r="334" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A334" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B334" s="13" t="s">
+        <v>2069</v>
+      </c>
+      <c r="C334" s="13" t="s">
+        <v>2073</v>
+      </c>
+      <c r="D334" s="13" t="s">
+        <v>2077</v>
+      </c>
+      <c r="E334" s="13" t="s">
+        <v>2081</v>
+      </c>
+      <c r="F334" s="16" t="str">
+        <f t="shared" ref="F334" si="28">L334&amp;" ("&amp;$J334&amp;")"</f>
+        <v>Bag (Cyclodextrin)</v>
+      </c>
+      <c r="G334" s="16" t="str">
+        <f t="shared" ref="G334" si="29">M334&amp;" ("&amp;$J334&amp;")"</f>
+        <v>Sack (Cyclodextrin)</v>
+      </c>
+      <c r="H334" s="16" t="str">
+        <f t="shared" ref="H334" si="30">N334&amp;" ("&amp;$J334&amp;")"</f>
+        <v>Powder Keg (Cyclodextrin)</v>
+      </c>
+      <c r="I334" s="16" t="str">
+        <f t="shared" ref="I334" si="31">O334&amp;" ("&amp;$J334&amp;")"</f>
+        <v>Chemical Silo (Cyclodextrin)</v>
+      </c>
+      <c r="J334" s="16" t="str">
+        <f>[1]Compounds!$B343</f>
+        <v>Cyclodextrin</v>
+      </c>
+      <c r="K334" t="str">
+        <f>[1]Compounds!$D343</f>
+        <v>Solid</v>
+      </c>
+      <c r="L334" s="4" t="str">
+        <f>IF(K334=[1]Enums!$A$18, [1]Enums!$A$23, IF(K334=[1]Enums!$B$22, [1]Enums!$A$22, [1]Enums!$A$21))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M334" s="4" t="str">
+        <f>IF(K334=[1]Enums!$A$18, [1]Enums!$A$26, IF(K334=[1]Enums!$B$25, [1]Enums!$A$25, [1]Enums!$A$24))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N334" s="4" t="str">
+        <f>IF(K334=[1]Enums!$A$18, [1]Enums!$A$29, IF(K334=[1]Enums!$B$22, [1]Enums!$A$28, [1]Enums!$A$27))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O334" s="4" t="str">
+        <f>IF(K334=[1]Enums!$A$18, [1]Enums!$A$32, IF(K334=[1]Enums!$B$22, [1]Enums!$A$31, [1]Enums!$A$30))</f>
         <v>Chemical Silo</v>
       </c>
     </row>
-    <row r="334" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B334" s="13"/>
+    <row r="335" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A335" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B335" s="13" t="s">
+        <v>2068</v>
+      </c>
+      <c r="C335" s="13" t="s">
+        <v>2072</v>
+      </c>
+      <c r="D335" s="13" t="s">
+        <v>2076</v>
+      </c>
+      <c r="E335" s="13" t="s">
+        <v>2080</v>
+      </c>
+      <c r="F335" s="16" t="str">
+        <f t="shared" ref="F335:F337" si="32">L335&amp;" ("&amp;$J335&amp;")"</f>
+        <v>Bag (Alpha-cyclodextrin)</v>
+      </c>
+      <c r="G335" s="16" t="str">
+        <f t="shared" ref="G335:G337" si="33">M335&amp;" ("&amp;$J335&amp;")"</f>
+        <v>Sack (Alpha-cyclodextrin)</v>
+      </c>
+      <c r="H335" s="16" t="str">
+        <f t="shared" ref="H335:H337" si="34">N335&amp;" ("&amp;$J335&amp;")"</f>
+        <v>Powder Keg (Alpha-cyclodextrin)</v>
+      </c>
+      <c r="I335" s="16" t="str">
+        <f t="shared" ref="I335:I337" si="35">O335&amp;" ("&amp;$J335&amp;")"</f>
+        <v>Chemical Silo (Alpha-cyclodextrin)</v>
+      </c>
+      <c r="J335" s="16" t="str">
+        <f>[1]Compounds!$B344</f>
+        <v>Alpha-cyclodextrin</v>
+      </c>
+      <c r="K335" t="str">
+        <f>[1]Compounds!$D344</f>
+        <v>Solid</v>
+      </c>
+      <c r="L335" s="4" t="str">
+        <f>IF(K335=[1]Enums!$A$18, [1]Enums!$A$23, IF(K335=[1]Enums!$B$22, [1]Enums!$A$22, [1]Enums!$A$21))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M335" s="4" t="str">
+        <f>IF(K335=[1]Enums!$A$18, [1]Enums!$A$26, IF(K335=[1]Enums!$B$25, [1]Enums!$A$25, [1]Enums!$A$24))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N335" s="4" t="str">
+        <f>IF(K335=[1]Enums!$A$18, [1]Enums!$A$29, IF(K335=[1]Enums!$B$22, [1]Enums!$A$28, [1]Enums!$A$27))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O335" s="4" t="str">
+        <f>IF(K335=[1]Enums!$A$18, [1]Enums!$A$32, IF(K335=[1]Enums!$B$22, [1]Enums!$A$31, [1]Enums!$A$30))</f>
+        <v>Chemical Silo</v>
+      </c>
+    </row>
+    <row r="336" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A336" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B336" s="13" t="s">
+        <v>2067</v>
+      </c>
+      <c r="C336" s="13" t="s">
+        <v>2071</v>
+      </c>
+      <c r="D336" s="13" t="s">
+        <v>2075</v>
+      </c>
+      <c r="E336" s="13" t="s">
+        <v>2079</v>
+      </c>
+      <c r="F336" s="16" t="str">
+        <f t="shared" si="32"/>
+        <v>Bag (Beta-cyclodextrin)</v>
+      </c>
+      <c r="G336" s="16" t="str">
+        <f t="shared" si="33"/>
+        <v>Sack (Beta-cyclodextrin)</v>
+      </c>
+      <c r="H336" s="16" t="str">
+        <f t="shared" si="34"/>
+        <v>Powder Keg (Beta-cyclodextrin)</v>
+      </c>
+      <c r="I336" s="16" t="str">
+        <f t="shared" si="35"/>
+        <v>Chemical Silo (Beta-cyclodextrin)</v>
+      </c>
+      <c r="J336" s="16" t="str">
+        <f>[1]Compounds!$B345</f>
+        <v>Beta-cyclodextrin</v>
+      </c>
+      <c r="K336" t="str">
+        <f>[1]Compounds!$D345</f>
+        <v>Solid</v>
+      </c>
+      <c r="L336" s="4" t="str">
+        <f>IF(K336=[1]Enums!$A$18, [1]Enums!$A$23, IF(K336=[1]Enums!$B$22, [1]Enums!$A$22, [1]Enums!$A$21))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M336" s="4" t="str">
+        <f>IF(K336=[1]Enums!$A$18, [1]Enums!$A$26, IF(K336=[1]Enums!$B$25, [1]Enums!$A$25, [1]Enums!$A$24))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N336" s="4" t="str">
+        <f>IF(K336=[1]Enums!$A$18, [1]Enums!$A$29, IF(K336=[1]Enums!$B$22, [1]Enums!$A$28, [1]Enums!$A$27))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O336" s="4" t="str">
+        <f>IF(K336=[1]Enums!$A$18, [1]Enums!$A$32, IF(K336=[1]Enums!$B$22, [1]Enums!$A$31, [1]Enums!$A$30))</f>
+        <v>Chemical Silo</v>
+      </c>
+    </row>
+    <row r="337" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A337" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B337" s="13" t="s">
+        <v>2066</v>
+      </c>
+      <c r="C337" s="13" t="s">
+        <v>2070</v>
+      </c>
+      <c r="D337" s="13" t="s">
+        <v>2074</v>
+      </c>
+      <c r="E337" s="13" t="s">
+        <v>2078</v>
+      </c>
+      <c r="F337" s="16" t="str">
+        <f t="shared" si="32"/>
+        <v>Bag (Gamma-cyclodextrin)</v>
+      </c>
+      <c r="G337" s="16" t="str">
+        <f t="shared" si="33"/>
+        <v>Sack (Gamma-cyclodextrin)</v>
+      </c>
+      <c r="H337" s="16" t="str">
+        <f t="shared" si="34"/>
+        <v>Powder Keg (Gamma-cyclodextrin)</v>
+      </c>
+      <c r="I337" s="16" t="str">
+        <f t="shared" si="35"/>
+        <v>Chemical Silo (Gamma-cyclodextrin)</v>
+      </c>
+      <c r="J337" s="16" t="str">
+        <f>[1]Compounds!$B346</f>
+        <v>Gamma-cyclodextrin</v>
+      </c>
+      <c r="K337" t="str">
+        <f>[1]Compounds!$D346</f>
+        <v>Solid</v>
+      </c>
+      <c r="L337" s="4" t="str">
+        <f>IF(K337=[1]Enums!$A$18, [1]Enums!$A$23, IF(K337=[1]Enums!$B$22, [1]Enums!$A$22, [1]Enums!$A$21))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M337" s="4" t="str">
+        <f>IF(K337=[1]Enums!$A$18, [1]Enums!$A$26, IF(K337=[1]Enums!$B$25, [1]Enums!$A$25, [1]Enums!$A$24))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N337" s="4" t="str">
+        <f>IF(K337=[1]Enums!$A$18, [1]Enums!$A$29, IF(K337=[1]Enums!$B$22, [1]Enums!$A$28, [1]Enums!$A$27))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O337" s="4" t="str">
+        <f>IF(K337=[1]Enums!$A$18, [1]Enums!$A$32, IF(K337=[1]Enums!$B$22, [1]Enums!$A$31, [1]Enums!$A$30))</f>
+        <v>Chemical Silo</v>
+      </c>
+    </row>
+    <row r="338" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A338" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B338" s="13" t="s">
+        <v>2097</v>
+      </c>
+      <c r="C338" s="13" t="s">
+        <v>2113</v>
+      </c>
+      <c r="D338" s="13" t="s">
+        <v>2129</v>
+      </c>
+      <c r="E338" s="13" t="s">
+        <v>2145</v>
+      </c>
+      <c r="F338" s="16" t="str">
+        <f t="shared" ref="F338:F340" si="36">L338&amp;" ("&amp;$J338&amp;")"</f>
+        <v>Bag (MOF-5)</v>
+      </c>
+      <c r="G338" s="16" t="str">
+        <f t="shared" ref="G338:G340" si="37">M338&amp;" ("&amp;$J338&amp;")"</f>
+        <v>Sack (MOF-5)</v>
+      </c>
+      <c r="H338" s="16" t="str">
+        <f t="shared" ref="H338:H340" si="38">N338&amp;" ("&amp;$J338&amp;")"</f>
+        <v>Powder Keg (MOF-5)</v>
+      </c>
+      <c r="I338" s="16" t="str">
+        <f t="shared" ref="I338:I340" si="39">O338&amp;" ("&amp;$J338&amp;")"</f>
+        <v>Chemical Silo (MOF-5)</v>
+      </c>
+      <c r="J338" s="16" t="str">
+        <f>[1]Compounds!$B347</f>
+        <v>MOF-5</v>
+      </c>
+      <c r="K338" t="str">
+        <f>[1]Compounds!$D347</f>
+        <v>Solid</v>
+      </c>
+      <c r="L338" s="4" t="str">
+        <f>IF(K338=[1]Enums!$A$18, [1]Enums!$A$23, IF(K338=[1]Enums!$B$22, [1]Enums!$A$22, [1]Enums!$A$21))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M338" s="4" t="str">
+        <f>IF(K338=[1]Enums!$A$18, [1]Enums!$A$26, IF(K338=[1]Enums!$B$25, [1]Enums!$A$25, [1]Enums!$A$24))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N338" s="4" t="str">
+        <f>IF(K338=[1]Enums!$A$18, [1]Enums!$A$29, IF(K338=[1]Enums!$B$22, [1]Enums!$A$28, [1]Enums!$A$27))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O338" s="4" t="str">
+        <f>IF(K338=[1]Enums!$A$18, [1]Enums!$A$32, IF(K338=[1]Enums!$B$22, [1]Enums!$A$31, [1]Enums!$A$30))</f>
+        <v>Chemical Silo</v>
+      </c>
+    </row>
+    <row r="339" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A339" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B339" s="13" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C339" s="13" t="s">
+        <v>2112</v>
+      </c>
+      <c r="D339" s="13" t="s">
+        <v>2128</v>
+      </c>
+      <c r="E339" s="13" t="s">
+        <v>2144</v>
+      </c>
+      <c r="F339" s="16" t="str">
+        <f t="shared" si="36"/>
+        <v>Bag (CD-MOF)</v>
+      </c>
+      <c r="G339" s="16" t="str">
+        <f t="shared" si="37"/>
+        <v>Sack (CD-MOF)</v>
+      </c>
+      <c r="H339" s="16" t="str">
+        <f t="shared" si="38"/>
+        <v>Powder Keg (CD-MOF)</v>
+      </c>
+      <c r="I339" s="16" t="str">
+        <f t="shared" si="39"/>
+        <v>Chemical Silo (CD-MOF)</v>
+      </c>
+      <c r="J339" s="16" t="str">
+        <f>[1]Compounds!$B348</f>
+        <v>CD-MOF</v>
+      </c>
+      <c r="K339" t="str">
+        <f>[1]Compounds!$D348</f>
+        <v>Solid</v>
+      </c>
+      <c r="L339" s="4" t="str">
+        <f>IF(K339=[1]Enums!$A$18, [1]Enums!$A$23, IF(K339=[1]Enums!$B$22, [1]Enums!$A$22, [1]Enums!$A$21))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M339" s="4" t="str">
+        <f>IF(K339=[1]Enums!$A$18, [1]Enums!$A$26, IF(K339=[1]Enums!$B$25, [1]Enums!$A$25, [1]Enums!$A$24))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N339" s="4" t="str">
+        <f>IF(K339=[1]Enums!$A$18, [1]Enums!$A$29, IF(K339=[1]Enums!$B$22, [1]Enums!$A$28, [1]Enums!$A$27))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O339" s="4" t="str">
+        <f>IF(K339=[1]Enums!$A$18, [1]Enums!$A$32, IF(K339=[1]Enums!$B$22, [1]Enums!$A$31, [1]Enums!$A$30))</f>
+        <v>Chemical Silo</v>
+      </c>
+    </row>
+    <row r="340" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A340" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B340" s="13" t="s">
+        <v>2095</v>
+      </c>
+      <c r="C340" s="13" t="s">
+        <v>2111</v>
+      </c>
+      <c r="D340" s="13" t="s">
+        <v>2127</v>
+      </c>
+      <c r="E340" s="13" t="s">
+        <v>2143</v>
+      </c>
+      <c r="F340" s="16" t="str">
+        <f t="shared" si="36"/>
+        <v>Bag (Bucky Balls (C60))</v>
+      </c>
+      <c r="G340" s="16" t="str">
+        <f t="shared" si="37"/>
+        <v>Sack (Bucky Balls (C60))</v>
+      </c>
+      <c r="H340" s="16" t="str">
+        <f t="shared" si="38"/>
+        <v>Powder Keg (Bucky Balls (C60))</v>
+      </c>
+      <c r="I340" s="16" t="str">
+        <f t="shared" si="39"/>
+        <v>Chemical Silo (Bucky Balls (C60))</v>
+      </c>
+      <c r="J340" s="16" t="str">
+        <f>[1]Compounds!$B349</f>
+        <v>Bucky Balls (C60)</v>
+      </c>
+      <c r="K340" t="str">
+        <f>[1]Compounds!$D349</f>
+        <v>Solid</v>
+      </c>
+      <c r="L340" s="4" t="str">
+        <f>IF(K340=[1]Enums!$A$18, [1]Enums!$A$23, IF(K340=[1]Enums!$B$22, [1]Enums!$A$22, [1]Enums!$A$21))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M340" s="4" t="str">
+        <f>IF(K340=[1]Enums!$A$18, [1]Enums!$A$26, IF(K340=[1]Enums!$B$25, [1]Enums!$A$25, [1]Enums!$A$24))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N340" s="4" t="str">
+        <f>IF(K340=[1]Enums!$A$18, [1]Enums!$A$29, IF(K340=[1]Enums!$B$22, [1]Enums!$A$28, [1]Enums!$A$27))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O340" s="4" t="str">
+        <f>IF(K340=[1]Enums!$A$18, [1]Enums!$A$32, IF(K340=[1]Enums!$B$22, [1]Enums!$A$31, [1]Enums!$A$30))</f>
+        <v>Chemical Silo</v>
+      </c>
+    </row>
+    <row r="341" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A341" s="4"/>
+      <c r="B341" s="13" t="s">
+        <v>2094</v>
+      </c>
+      <c r="C341" s="13" t="s">
+        <v>2110</v>
+      </c>
+      <c r="D341" s="13" t="s">
+        <v>2126</v>
+      </c>
+      <c r="E341" s="13" t="s">
+        <v>2142</v>
+      </c>
+      <c r="F341" s="16" t="str">
+        <f t="shared" ref="F341" si="40">L341&amp;" ("&amp;$J341&amp;")"</f>
+        <v>Bag (Zinc Nitrate)</v>
+      </c>
+      <c r="G341" s="16" t="str">
+        <f t="shared" ref="G341" si="41">M341&amp;" ("&amp;$J341&amp;")"</f>
+        <v>Sack (Zinc Nitrate)</v>
+      </c>
+      <c r="H341" s="16" t="str">
+        <f t="shared" ref="H341" si="42">N341&amp;" ("&amp;$J341&amp;")"</f>
+        <v>Powder Keg (Zinc Nitrate)</v>
+      </c>
+      <c r="I341" s="16" t="str">
+        <f t="shared" ref="I341" si="43">O341&amp;" ("&amp;$J341&amp;")"</f>
+        <v>Chemical Silo (Zinc Nitrate)</v>
+      </c>
+      <c r="J341" s="16" t="str">
+        <f>[1]Compounds!$B350</f>
+        <v>Zinc Nitrate</v>
+      </c>
+      <c r="K341" t="str">
+        <f>[1]Compounds!$D350</f>
+        <v>Solid</v>
+      </c>
+      <c r="L341" s="4" t="str">
+        <f>IF(K341=[1]Enums!$A$18, [1]Enums!$A$23, IF(K341=[1]Enums!$B$22, [1]Enums!$A$22, [1]Enums!$A$21))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M341" s="4" t="str">
+        <f>IF(K341=[1]Enums!$A$18, [1]Enums!$A$26, IF(K341=[1]Enums!$B$25, [1]Enums!$A$25, [1]Enums!$A$24))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N341" s="4" t="str">
+        <f>IF(K341=[1]Enums!$A$18, [1]Enums!$A$29, IF(K341=[1]Enums!$B$22, [1]Enums!$A$28, [1]Enums!$A$27))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O341" s="4" t="str">
+        <f>IF(K341=[1]Enums!$A$18, [1]Enums!$A$32, IF(K341=[1]Enums!$B$22, [1]Enums!$A$31, [1]Enums!$A$30))</f>
+        <v>Chemical Silo</v>
+      </c>
+    </row>
+    <row r="342" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A342" s="4"/>
+      <c r="B342" s="13" t="s">
+        <v>2093</v>
+      </c>
+      <c r="C342" s="13" t="s">
+        <v>2109</v>
+      </c>
+      <c r="D342" s="13" t="s">
+        <v>2125</v>
+      </c>
+      <c r="E342" s="13" t="s">
+        <v>2141</v>
+      </c>
+      <c r="F342" s="16" t="str">
+        <f t="shared" ref="F342:F343" si="44">L342&amp;" ("&amp;$J342&amp;")"</f>
+        <v>Bag (Lead Oxide)</v>
+      </c>
+      <c r="G342" s="16" t="str">
+        <f t="shared" ref="G342:G343" si="45">M342&amp;" ("&amp;$J342&amp;")"</f>
+        <v>Sack (Lead Oxide)</v>
+      </c>
+      <c r="H342" s="16" t="str">
+        <f t="shared" ref="H342:H343" si="46">N342&amp;" ("&amp;$J342&amp;")"</f>
+        <v>Powder Keg (Lead Oxide)</v>
+      </c>
+      <c r="I342" s="16" t="str">
+        <f t="shared" ref="I342:I343" si="47">O342&amp;" ("&amp;$J342&amp;")"</f>
+        <v>Chemical Silo (Lead Oxide)</v>
+      </c>
+      <c r="J342" s="16" t="str">
+        <f>[1]Compounds!$B351</f>
+        <v>Lead Oxide</v>
+      </c>
+      <c r="K342" t="str">
+        <f>[1]Compounds!$D351</f>
+        <v>Solid</v>
+      </c>
+      <c r="L342" s="4" t="str">
+        <f>IF(K342=[1]Enums!$A$18, [1]Enums!$A$23, IF(K342=[1]Enums!$B$22, [1]Enums!$A$22, [1]Enums!$A$21))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M342" s="4" t="str">
+        <f>IF(K342=[1]Enums!$A$18, [1]Enums!$A$26, IF(K342=[1]Enums!$B$25, [1]Enums!$A$25, [1]Enums!$A$24))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N342" s="4" t="str">
+        <f>IF(K342=[1]Enums!$A$18, [1]Enums!$A$29, IF(K342=[1]Enums!$B$22, [1]Enums!$A$28, [1]Enums!$A$27))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O342" s="4" t="str">
+        <f>IF(K342=[1]Enums!$A$18, [1]Enums!$A$32, IF(K342=[1]Enums!$B$22, [1]Enums!$A$31, [1]Enums!$A$30))</f>
+        <v>Chemical Silo</v>
+      </c>
+    </row>
+    <row r="343" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A343" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B343" s="13" t="s">
+        <v>2092</v>
+      </c>
+      <c r="C343" s="13" t="s">
+        <v>2108</v>
+      </c>
+      <c r="D343" s="13" t="s">
+        <v>2124</v>
+      </c>
+      <c r="E343" s="13" t="s">
+        <v>2140</v>
+      </c>
+      <c r="F343" s="16" t="str">
+        <f t="shared" si="44"/>
+        <v>Bag (Lithium Hexafluorophosphate)</v>
+      </c>
+      <c r="G343" s="16" t="str">
+        <f t="shared" si="45"/>
+        <v>Sack (Lithium Hexafluorophosphate)</v>
+      </c>
+      <c r="H343" s="16" t="str">
+        <f t="shared" si="46"/>
+        <v>Powder Keg (Lithium Hexafluorophosphate)</v>
+      </c>
+      <c r="I343" s="16" t="str">
+        <f t="shared" si="47"/>
+        <v>Chemical Silo (Lithium Hexafluorophosphate)</v>
+      </c>
+      <c r="J343" s="16" t="str">
+        <f>[1]Compounds!$B352</f>
+        <v>Lithium Hexafluorophosphate</v>
+      </c>
+      <c r="K343" t="str">
+        <f>[1]Compounds!$D352</f>
+        <v>Solid</v>
+      </c>
+      <c r="L343" s="4" t="str">
+        <f>IF(K343=[1]Enums!$A$18, [1]Enums!$A$23, IF(K343=[1]Enums!$B$22, [1]Enums!$A$22, [1]Enums!$A$21))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M343" s="4" t="str">
+        <f>IF(K343=[1]Enums!$A$18, [1]Enums!$A$26, IF(K343=[1]Enums!$B$25, [1]Enums!$A$25, [1]Enums!$A$24))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N343" s="4" t="str">
+        <f>IF(K343=[1]Enums!$A$18, [1]Enums!$A$29, IF(K343=[1]Enums!$B$22, [1]Enums!$A$28, [1]Enums!$A$27))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O343" s="4" t="str">
+        <f>IF(K343=[1]Enums!$A$18, [1]Enums!$A$32, IF(K343=[1]Enums!$B$22, [1]Enums!$A$31, [1]Enums!$A$30))</f>
+        <v>Chemical Silo</v>
+      </c>
+    </row>
+    <row r="344" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B344" s="13" t="s">
+        <v>2091</v>
+      </c>
+      <c r="C344" s="13" t="s">
+        <v>2107</v>
+      </c>
+      <c r="D344" s="13" t="s">
+        <v>2123</v>
+      </c>
+      <c r="E344" s="13" t="s">
+        <v>2139</v>
+      </c>
+    </row>
+    <row r="345" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B345" s="13" t="s">
+        <v>2090</v>
+      </c>
+      <c r="C345" s="13" t="s">
+        <v>2106</v>
+      </c>
+      <c r="D345" s="13" t="s">
+        <v>2122</v>
+      </c>
+      <c r="E345" s="13" t="s">
+        <v>2138</v>
+      </c>
+    </row>
+    <row r="346" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B346" s="13" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C346" s="13" t="s">
+        <v>2105</v>
+      </c>
+      <c r="D346" s="13" t="s">
+        <v>2121</v>
+      </c>
+      <c r="E346" s="13" t="s">
+        <v>2137</v>
+      </c>
+    </row>
+    <row r="347" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B347" s="13" t="s">
+        <v>2088</v>
+      </c>
+      <c r="C347" s="13" t="s">
+        <v>2104</v>
+      </c>
+      <c r="D347" s="13" t="s">
+        <v>2120</v>
+      </c>
+      <c r="E347" s="13" t="s">
+        <v>2136</v>
+      </c>
+    </row>
+    <row r="348" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B348" s="13" t="s">
+        <v>2087</v>
+      </c>
+      <c r="C348" s="13" t="s">
+        <v>2103</v>
+      </c>
+      <c r="D348" s="13" t="s">
+        <v>2119</v>
+      </c>
+      <c r="E348" s="13" t="s">
+        <v>2135</v>
+      </c>
+    </row>
+    <row r="349" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B349" s="13" t="s">
+        <v>2086</v>
+      </c>
+      <c r="C349" s="13" t="s">
+        <v>2102</v>
+      </c>
+      <c r="D349" s="13" t="s">
+        <v>2118</v>
+      </c>
+      <c r="E349" s="13" t="s">
+        <v>2134</v>
+      </c>
+    </row>
+    <row r="350" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B350" s="13" t="s">
+        <v>2085</v>
+      </c>
+      <c r="C350" s="13" t="s">
+        <v>2101</v>
+      </c>
+      <c r="D350" s="13" t="s">
+        <v>2117</v>
+      </c>
+      <c r="E350" s="13" t="s">
+        <v>2133</v>
+      </c>
+    </row>
+    <row r="351" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B351" s="13" t="s">
+        <v>2084</v>
+      </c>
+      <c r="C351" s="13" t="s">
+        <v>2100</v>
+      </c>
+      <c r="D351" s="13" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E351" s="13" t="s">
+        <v>2132</v>
+      </c>
+    </row>
+    <row r="352" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B352" s="13" t="s">
+        <v>2083</v>
+      </c>
+      <c r="C352" s="13" t="s">
+        <v>2099</v>
+      </c>
+      <c r="D352" s="13" t="s">
+        <v>2115</v>
+      </c>
+      <c r="E352" s="13" t="s">
+        <v>2131</v>
+      </c>
+    </row>
+    <row r="353" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B353" s="13" t="s">
+        <v>2082</v>
+      </c>
+      <c r="C353" s="13" t="s">
+        <v>2098</v>
+      </c>
+      <c r="D353" s="13" t="s">
+        <v>2114</v>
+      </c>
+      <c r="E353" s="13" t="s">
+        <v>2130</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="F2:P336">

</xml_diff>

<commit_message>
Recipe updates to 1.1.0 - added advanced rubbers
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Walter\Documents\GitHub\polycraft-1.7.10\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Walter\Documents\GitHub\polycraftworld\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="57495" yWindow="495" windowWidth="19200" windowHeight="19455" tabRatio="877" activeTab="5"/>
+    <workbookView xWindow="59355" yWindow="495" windowWidth="19200" windowHeight="19455" tabRatio="877"/>
   </bookViews>
   <sheets>
     <sheet name="Custom Objects" sheetId="41" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2187" uniqueCount="2161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2211" uniqueCount="2179">
   <si>
     <t>Ore</t>
   </si>
@@ -6058,9 +6058,6 @@
     <t>3P</t>
   </si>
   <si>
-    <t>Regulator</t>
-  </si>
-  <si>
     <t>3M</t>
   </si>
   <si>
@@ -6097,9 +6094,6 @@
     <t>AirUnitsFull, AirUnitsConsumePerTick</t>
   </si>
   <si>
-    <t>Scuba Tank</t>
-  </si>
-  <si>
     <t>3x</t>
   </si>
   <si>
@@ -6524,6 +6518,66 @@
   </si>
   <si>
     <t>Custom Object</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>Flame Tosser</t>
+  </si>
+  <si>
+    <t>Flame Chucker</t>
+  </si>
+  <si>
+    <t>Flame Hurler</t>
+  </si>
+  <si>
+    <t>Regulator (Low Pressure)</t>
+  </si>
+  <si>
+    <t>Regulator (Medium Pressure)</t>
+  </si>
+  <si>
+    <t>Regulator (High Pressure)</t>
+  </si>
+  <si>
+    <t>Regulator (Extreme Pressure)</t>
+  </si>
+  <si>
+    <t>13a</t>
+  </si>
+  <si>
+    <t>13b</t>
+  </si>
+  <si>
+    <t>13c</t>
+  </si>
+  <si>
+    <t>Scuba Tank (Beginner)</t>
+  </si>
+  <si>
+    <t>Scuba Tank (Intermediate)</t>
+  </si>
+  <si>
+    <t>Scuba Tank (Advanced)</t>
+  </si>
+  <si>
+    <t>Scuba Tank (Pro)</t>
   </si>
 </sst>
 </file>
@@ -12425,10 +12479,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R66"/>
+  <dimension ref="A1:R75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12457,22 +12511,22 @@
         <v>Game ID</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>2160</v>
+        <v>2158</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>2045</v>
+        <v>2043</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>2044</v>
+        <v>2042</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>2043</v>
+        <v>2041</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>2042</v>
+        <v>2040</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>2041</v>
+        <v>2039</v>
       </c>
       <c r="I1" s="35" t="s">
         <v>1959</v>
@@ -12511,10 +12565,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>2040</v>
+        <v>2038</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>2039</v>
+        <v>2037</v>
       </c>
       <c r="D2" s="32" t="str">
         <f>[1]Enums!$A$40</f>
@@ -12533,10 +12587,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>2038</v>
+        <v>2036</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>2037</v>
+        <v>2035</v>
       </c>
       <c r="D3" s="32" t="str">
         <f>[1]Enums!$A$40</f>
@@ -12555,10 +12609,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>2036</v>
+        <v>2034</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>2035</v>
+        <v>2165</v>
       </c>
       <c r="D4" s="32" t="str">
         <f>[1]Enums!$A$36</f>
@@ -12574,7 +12628,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="31" t="s">
-        <v>2034</v>
+        <v>2032</v>
       </c>
       <c r="J4" s="26">
         <v>1000</v>
@@ -12583,7 +12637,7 @@
         <v>1</v>
       </c>
       <c r="L4" s="26">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M4" s="26">
         <v>2</v>
@@ -12592,122 +12646,161 @@
         <v>5</v>
       </c>
       <c r="O4" s="26">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B5" s="33" t="s">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>2159</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>2166</v>
+      </c>
+      <c r="D5" s="32" t="str">
+        <f>[1]Enums!$A$36</f>
+        <v>Weapon</v>
+      </c>
+      <c r="E5" s="32">
+        <v>7</v>
+      </c>
+      <c r="F5" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="26">
+        <v>1</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>2032</v>
+      </c>
+      <c r="J5" s="26">
+        <v>1500</v>
+      </c>
+      <c r="K5" s="26">
+        <v>1</v>
+      </c>
+      <c r="L5" s="26">
+        <v>8</v>
+      </c>
+      <c r="M5" s="26">
+        <v>2</v>
+      </c>
+      <c r="N5" s="26">
+        <v>5</v>
+      </c>
+      <c r="O5" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>2160</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>2167</v>
+      </c>
+      <c r="D6" s="32" t="str">
+        <f>[1]Enums!$A$36</f>
+        <v>Weapon</v>
+      </c>
+      <c r="E6" s="32">
+        <v>7</v>
+      </c>
+      <c r="F6" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="26">
+        <v>1</v>
+      </c>
+      <c r="I6" s="31" t="s">
+        <v>2032</v>
+      </c>
+      <c r="J6" s="26">
+        <v>2000</v>
+      </c>
+      <c r="K6" s="26">
+        <v>1</v>
+      </c>
+      <c r="L6" s="26">
+        <v>10</v>
+      </c>
+      <c r="M6" s="26">
+        <v>2</v>
+      </c>
+      <c r="N6" s="26">
+        <v>5</v>
+      </c>
+      <c r="O6" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>2161</v>
+      </c>
+      <c r="C7" s="34" t="s">
         <v>2033</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="D7" s="32" t="str">
+        <f>[1]Enums!$A$36</f>
+        <v>Weapon</v>
+      </c>
+      <c r="E7" s="32">
+        <v>7</v>
+      </c>
+      <c r="F7" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="26">
+        <v>1</v>
+      </c>
+      <c r="I7" s="31" t="s">
         <v>2032</v>
       </c>
-      <c r="D5" s="32" t="str">
+      <c r="J7" s="26">
+        <v>2500</v>
+      </c>
+      <c r="K7" s="26">
+        <v>1</v>
+      </c>
+      <c r="L7" s="26">
+        <v>12</v>
+      </c>
+      <c r="M7" s="26">
+        <v>2</v>
+      </c>
+      <c r="N7" s="26">
+        <v>5</v>
+      </c>
+      <c r="O7" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="29" t="str">
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>2031</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>2030</v>
+      </c>
+      <c r="D8" s="32" t="str">
         <f>[1]Enums!$A$37</f>
         <v>Utility</v>
-      </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="26">
-        <v>1</v>
-      </c>
-      <c r="I5" s="26" t="s">
-        <v>2031</v>
-      </c>
-      <c r="J5" s="26">
-        <v>15</v>
-      </c>
-      <c r="K5" s="26">
-        <v>0.5</v>
-      </c>
-      <c r="L5" s="26">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>2030</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>2029</v>
-      </c>
-      <c r="D6" s="32" t="str">
-        <f>[1]Enums!$A$35</f>
-        <v>Armor</v>
-      </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="26">
-        <v>1</v>
-      </c>
-      <c r="I6" s="31" t="s">
-        <v>2028</v>
-      </c>
-      <c r="J6" s="26">
-        <v>5000</v>
-      </c>
-      <c r="K6" s="26">
-        <v>1</v>
-      </c>
-      <c r="L6" s="26">
-        <v>0.4</v>
-      </c>
-      <c r="M6" s="26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>2027</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>2026</v>
-      </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="26">
-        <v>1</v>
-      </c>
-      <c r="I7" s="31" t="s">
-        <v>2025</v>
-      </c>
-      <c r="J7" s="26">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>2024</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>2023</v>
-      </c>
-      <c r="D8" s="32" t="str">
-        <f>[1]Enums!$A$38</f>
-        <v>Tool</v>
       </c>
       <c r="E8" s="32"/>
       <c r="F8" s="26" t="b">
@@ -12716,6 +12809,18 @@
       <c r="H8" s="26">
         <v>1</v>
       </c>
+      <c r="I8" s="26" t="s">
+        <v>2029</v>
+      </c>
+      <c r="J8" s="26">
+        <v>15</v>
+      </c>
+      <c r="K8" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="L8" s="26">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="str">
@@ -12723,36 +12828,36 @@
         <v>1.0.0</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>2022</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>2021</v>
+        <v>2028</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>2027</v>
       </c>
       <c r="D9" s="32" t="str">
-        <f>[1]Enums!$A$38</f>
-        <v>Tool</v>
-      </c>
-      <c r="E9" s="32">
-        <v>7</v>
-      </c>
+        <f>[1]Enums!$A$35</f>
+        <v>Armor</v>
+      </c>
+      <c r="E9" s="32"/>
       <c r="F9" s="26" t="b">
         <v>1</v>
       </c>
       <c r="H9" s="26">
         <v>1</v>
       </c>
-      <c r="I9" s="26" t="s">
-        <v>2020</v>
+      <c r="I9" s="31" t="s">
+        <v>2026</v>
       </c>
       <c r="J9" s="26">
-        <v>3</v>
+        <v>5000</v>
       </c>
       <c r="K9" s="26">
-        <v>0.6</v>
-      </c>
-      <c r="L9" s="26" t="str">
-        <f>'[1]Blocks (MC)'!$A$22</f>
-        <v>1.0.0</v>
+        <v>1</v>
+      </c>
+      <c r="L9" s="26">
+        <v>0.4</v>
+      </c>
+      <c r="M9" s="26">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -12760,16 +12865,13 @@
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
       </c>
-      <c r="B10" s="33" t="s">
-        <v>2019</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>2018</v>
-      </c>
-      <c r="D10" s="32" t="str">
-        <f>[1]Enums!$A$35</f>
-        <v>Armor</v>
-      </c>
+      <c r="B10" s="13" t="s">
+        <v>2025</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>2024</v>
+      </c>
+      <c r="D10" s="32"/>
       <c r="E10" s="32"/>
       <c r="F10" s="26" t="b">
         <v>1</v>
@@ -12777,14 +12879,11 @@
       <c r="H10" s="26">
         <v>1</v>
       </c>
-      <c r="I10" s="26" t="s">
-        <v>2017</v>
+      <c r="I10" s="31" t="s">
+        <v>2023</v>
       </c>
       <c r="J10" s="26">
-        <v>5000</v>
-      </c>
-      <c r="K10" s="26">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -12793,14 +12892,14 @@
         <v>1.0.0</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>2016</v>
+        <v>2022</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="D11" s="32" t="str">
-        <f>[1]Enums!$A$35</f>
-        <v>Armor</v>
+        <f>[1]Enums!$A$38</f>
+        <v>Tool</v>
       </c>
       <c r="E11" s="32"/>
       <c r="F11" s="26" t="b">
@@ -12816,435 +12915,470 @@
         <v>1.0.0</v>
       </c>
       <c r="B12" s="33" t="s">
+        <v>2020</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>2019</v>
+      </c>
+      <c r="D12" s="32" t="str">
+        <f>[1]Enums!$A$38</f>
+        <v>Tool</v>
+      </c>
+      <c r="E12" s="32">
+        <v>7</v>
+      </c>
+      <c r="F12" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="26">
+        <v>1</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>2018</v>
+      </c>
+      <c r="J12" s="26">
+        <v>3</v>
+      </c>
+      <c r="K12" s="26">
+        <v>0.6</v>
+      </c>
+      <c r="L12" s="26" t="str">
+        <f>'[1]Blocks (MC)'!$A$22</f>
+        <v>1.0.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="29" t="str">
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>2017</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>2175</v>
+      </c>
+      <c r="D13" s="32" t="str">
+        <f>[1]Enums!$A$35</f>
+        <v>Armor</v>
+      </c>
+      <c r="E13" s="32"/>
+      <c r="F13" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="26">
+        <v>1</v>
+      </c>
+      <c r="I13" s="26" t="s">
+        <v>2016</v>
+      </c>
+      <c r="J13" s="26">
+        <v>5000</v>
+      </c>
+      <c r="K13" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>2172</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>2176</v>
+      </c>
+      <c r="D14" s="32" t="str">
+        <f>[1]Enums!$A$35</f>
+        <v>Armor</v>
+      </c>
+      <c r="E14" s="32"/>
+      <c r="F14" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="26">
+        <v>1</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>2016</v>
+      </c>
+      <c r="J14" s="26">
+        <v>10000</v>
+      </c>
+      <c r="K14" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="29" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>2173</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>2177</v>
+      </c>
+      <c r="D15" s="32" t="str">
+        <f>[1]Enums!$A$35</f>
+        <v>Armor</v>
+      </c>
+      <c r="E15" s="32"/>
+      <c r="F15" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="26">
+        <v>1</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>2016</v>
+      </c>
+      <c r="J15" s="26">
+        <v>25000</v>
+      </c>
+      <c r="K15" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>2174</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>2178</v>
+      </c>
+      <c r="D16" s="32" t="str">
+        <f>[1]Enums!$A$35</f>
+        <v>Armor</v>
+      </c>
+      <c r="E16" s="32"/>
+      <c r="F16" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="26">
+        <v>1</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>2016</v>
+      </c>
+      <c r="J16" s="26">
+        <v>50000</v>
+      </c>
+      <c r="K16" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="29" t="str">
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>2015</v>
+      </c>
+      <c r="C17" s="32" t="s">
         <v>2014</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="D17" s="32" t="str">
+        <f>[1]Enums!$A$35</f>
+        <v>Armor</v>
+      </c>
+      <c r="E17" s="32"/>
+      <c r="F17" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="29" t="str">
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B18" s="33" t="s">
         <v>2013</v>
       </c>
-      <c r="D12" s="34" t="str">
+      <c r="C18" s="32" t="s">
+        <v>2012</v>
+      </c>
+      <c r="D18" s="34" t="str">
         <f>[1]Enums!$A$41</f>
         <v>PC Block</v>
       </c>
-      <c r="F12" s="26" t="b">
+      <c r="F18" s="26" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>2012</v>
-      </c>
-      <c r="C13" s="34" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="29" t="str">
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B19" s="33" t="s">
         <v>2011</v>
       </c>
-      <c r="D13" s="34" t="str">
+      <c r="C19" s="34" t="s">
+        <v>2010</v>
+      </c>
+      <c r="D19" s="34" t="str">
         <f>[1]Enums!$A$42</f>
         <v>Food</v>
       </c>
-      <c r="F13" s="26" t="b">
+      <c r="F19" s="26" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>2010</v>
-      </c>
-      <c r="C14" s="34" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="29" t="str">
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B20" s="33" t="s">
         <v>2009</v>
       </c>
-      <c r="D14" s="34" t="str">
+      <c r="C20" s="34" t="s">
+        <v>2008</v>
+      </c>
+      <c r="D20" s="34" t="str">
         <f>[1]Enums!$A$42</f>
         <v>Food</v>
       </c>
-      <c r="F14" s="26" t="b">
+      <c r="F20" s="26" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>2008</v>
-      </c>
-      <c r="C15" s="28" t="s">
+    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="29" t="str">
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B21" s="33" t="s">
         <v>2007</v>
       </c>
-      <c r="D15" s="34" t="str">
+      <c r="C21" s="28" t="s">
+        <v>2006</v>
+      </c>
+      <c r="D21" s="34" t="str">
         <f>[1]Enums!$A$41</f>
         <v>PC Block</v>
       </c>
-      <c r="F15" s="26" t="b">
+      <c r="F21" s="26" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>2006</v>
-      </c>
-      <c r="C16" s="28" t="s">
+    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="29" t="str">
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B22" s="33" t="s">
         <v>2005</v>
       </c>
-      <c r="D16" s="26" t="str">
+      <c r="C22" s="28" t="s">
+        <v>2168</v>
+      </c>
+      <c r="D22" s="26" t="str">
         <f>[1]Enums!$A$40</f>
         <v>PC Item</v>
       </c>
-      <c r="F16" s="26" t="b">
+      <c r="F22" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-    </row>
-    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B17" s="33" t="s">
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+    </row>
+    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A23" s="29" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>2162</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>2169</v>
+      </c>
+      <c r="D23" s="26" t="str">
+        <f>[1]Enums!$A$40</f>
+        <v>PC Item</v>
+      </c>
+      <c r="F23" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+    </row>
+    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A24" s="29" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>2163</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>2170</v>
+      </c>
+      <c r="D24" s="26" t="str">
+        <f>[1]Enums!$A$40</f>
+        <v>PC Item</v>
+      </c>
+      <c r="F24" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+    </row>
+    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="29" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>2164</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>2171</v>
+      </c>
+      <c r="D25" s="26" t="str">
+        <f>[1]Enums!$A$40</f>
+        <v>PC Item</v>
+      </c>
+      <c r="F25" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+    </row>
+    <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="29" t="str">
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B26" s="33" t="s">
         <v>2004</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C26" s="28" t="s">
         <v>2003</v>
       </c>
-      <c r="D17" s="28" t="str">
+      <c r="D26" s="28" t="str">
         <f>[1]Enums!$A$37</f>
         <v>Utility</v>
       </c>
-      <c r="E17" s="26">
-        <v>4</v>
-      </c>
-      <c r="F17" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B18" s="33" t="s">
-        <v>2002</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>2001</v>
-      </c>
-      <c r="D18" s="28" t="str">
-        <f>[1]Enums!$A$40</f>
-        <v>PC Item</v>
-      </c>
-      <c r="F18" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B19" s="33" t="s">
-        <v>2000</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>1999</v>
-      </c>
-      <c r="D19" s="28" t="str">
-        <f>[1]Enums!$A$40</f>
-        <v>PC Item</v>
-      </c>
-      <c r="F19" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B20" s="33" t="s">
-        <v>1998</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>1997</v>
-      </c>
-      <c r="D20" s="28" t="str">
-        <f>[1]Enums!$A$40</f>
-        <v>PC Item</v>
-      </c>
-      <c r="F20" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B21" s="33" t="s">
-        <v>1996</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>1995</v>
-      </c>
-      <c r="D21" s="28" t="str">
-        <f>[1]Enums!$A$41</f>
-        <v>PC Block</v>
-      </c>
-      <c r="F21" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" s="26" t="s">
-        <v>1994</v>
-      </c>
-      <c r="J21" s="26">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B22" s="33" t="s">
-        <v>1993</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>1992</v>
-      </c>
-      <c r="D22" s="28" t="str">
-        <f>[1]Enums!$A$40</f>
-        <v>PC Item</v>
-      </c>
-      <c r="E22" s="26">
-        <v>4</v>
-      </c>
-      <c r="F22" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>1991</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>1990</v>
-      </c>
-      <c r="F23" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="H23" s="27">
-        <v>1</v>
-      </c>
-      <c r="I23" s="27" t="s">
-        <v>1989</v>
-      </c>
-      <c r="J23" s="27">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>1988</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>1987</v>
-      </c>
-      <c r="D24" s="28" t="str">
-        <f>[1]Enums!$A$40</f>
-        <v>PC Item</v>
-      </c>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>1986</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>1985</v>
-      </c>
-      <c r="D25" s="28" t="str">
-        <f>[1]Enums!$A$40</f>
-        <v>PC Item</v>
-      </c>
-      <c r="F25" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>1984</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>1983</v>
-      </c>
-      <c r="D26" s="32" t="str">
-        <f>[1]Enums!$A$37</f>
-        <v>Utility</v>
-      </c>
       <c r="E26" s="26">
         <v>4</v>
       </c>
       <c r="F26" s="26" t="b">
         <v>1</v>
       </c>
+      <c r="H26" s="26">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>1982</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>1981</v>
+      <c r="B27" s="33" t="s">
+        <v>2002</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>2001</v>
       </c>
       <c r="D27" s="28" t="str">
         <f>[1]Enums!$A$40</f>
         <v>PC Item</v>
       </c>
-      <c r="E27" s="26">
-        <v>8</v>
-      </c>
       <c r="F27" s="26" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="29" t="str">
-        <f>[1]Enums!$A$5</f>
-        <v>1.0.3</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>1980</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>1979</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>1965</v>
-      </c>
-      <c r="E28" s="26">
-        <v>4</v>
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>2000</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>1999</v>
+      </c>
+      <c r="D28" s="28" t="str">
+        <f>[1]Enums!$A$40</f>
+        <v>PC Item</v>
       </c>
       <c r="F28" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28">
-        <v>1</v>
-      </c>
-      <c r="I28" s="31" t="s">
-        <v>1968</v>
-      </c>
-      <c r="J28" s="26">
-        <v>10</v>
-      </c>
     </row>
     <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="29" t="str">
-        <f>[1]Enums!$A$5</f>
-        <v>1.0.3</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>1978</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>1977</v>
-      </c>
-      <c r="D29" s="28" t="s">
-        <v>1965</v>
-      </c>
-      <c r="E29" s="26">
-        <v>4</v>
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>1998</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>1997</v>
+      </c>
+      <c r="D29" s="28" t="str">
+        <f>[1]Enums!$A$40</f>
+        <v>PC Item</v>
       </c>
       <c r="F29" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="31" t="s">
-        <v>1968</v>
-      </c>
-      <c r="J29" s="26">
-        <v>15</v>
-      </c>
     </row>
     <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="29" t="str">
-        <f>[1]Enums!$A$5</f>
-        <v>1.0.3</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>1976</v>
-      </c>
-      <c r="C30" s="31" t="s">
-        <v>1975</v>
-      </c>
-      <c r="D30" s="28" t="s">
-        <v>1965</v>
-      </c>
-      <c r="E30" s="26">
-        <v>4</v>
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>1996</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>1995</v>
+      </c>
+      <c r="D30" s="28" t="str">
+        <f>[1]Enums!$A$41</f>
+        <v>PC Block</v>
       </c>
       <c r="F30" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="31" t="s">
-        <v>1968</v>
+      <c r="I30" s="26" t="s">
+        <v>1994</v>
       </c>
       <c r="J30" s="26">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="29" t="str">
-        <f>[1]Enums!$A$5</f>
-        <v>1.0.3</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>1974</v>
-      </c>
-      <c r="C31" s="31" t="s">
-        <v>1973</v>
-      </c>
-      <c r="D31" s="28" t="s">
-        <v>1965</v>
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>1993</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>1992</v>
+      </c>
+      <c r="D31" s="28" t="str">
+        <f>[1]Enums!$A$40</f>
+        <v>PC Item</v>
       </c>
       <c r="E31" s="26">
         <v>4</v>
@@ -13252,137 +13386,102 @@
       <c r="F31" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="31" t="s">
-        <v>1968</v>
-      </c>
-      <c r="J31" s="26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="29" t="str">
-        <f>[1]Enums!$A$5</f>
-        <v>1.0.3</v>
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>1972</v>
-      </c>
-      <c r="C32" s="31" t="s">
-        <v>1971</v>
-      </c>
-      <c r="D32" s="28" t="s">
-        <v>1965</v>
-      </c>
-      <c r="E32" s="26">
-        <v>4</v>
+        <v>1991</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>1990</v>
       </c>
       <c r="F32" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="31" t="s">
-        <v>1968</v>
-      </c>
-      <c r="J32" s="26">
-        <v>10</v>
+      <c r="H32" s="27">
+        <v>1</v>
+      </c>
+      <c r="I32" s="27" t="s">
+        <v>1989</v>
+      </c>
+      <c r="J32" s="27">
+        <v>1.5</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="29" t="str">
-        <f>[1]Enums!$A$5</f>
-        <v>1.0.3</v>
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>1970</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>1969</v>
-      </c>
-      <c r="D33" s="28" t="s">
-        <v>1965</v>
-      </c>
-      <c r="E33" s="26">
-        <v>4</v>
-      </c>
-      <c r="F33" s="26" t="b">
+        <v>1988</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>1987</v>
+      </c>
+      <c r="D33" s="28" t="str">
+        <f>[1]Enums!$A$40</f>
+        <v>PC Item</v>
+      </c>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28" t="b">
         <v>1</v>
-      </c>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="31" t="s">
-        <v>1968</v>
-      </c>
-      <c r="J33" s="26">
-        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="29" t="str">
-        <f>[1]Enums!$A$5</f>
-        <v>1.0.3</v>
-      </c>
-      <c r="B34" s="31" t="s">
-        <v>1967</v>
-      </c>
-      <c r="C34" s="31" t="s">
-        <v>1966</v>
-      </c>
-      <c r="D34" s="31" t="s">
-        <v>1965</v>
-      </c>
-      <c r="E34" s="26">
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>1986</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>1985</v>
+      </c>
+      <c r="D34" s="28" t="str">
+        <f>[1]Enums!$A$40</f>
+        <v>PC Item</v>
+      </c>
+      <c r="F34" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="29" t="str">
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>1983</v>
+      </c>
+      <c r="D35" s="32" t="str">
+        <f>[1]Enums!$A$37</f>
+        <v>Utility</v>
+      </c>
+      <c r="E35" s="26">
         <v>4</v>
-      </c>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-    </row>
-    <row r="35" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="29" t="str">
-        <f>[1]Enums!$A$12</f>
-        <v>1.1.0</v>
-      </c>
-      <c r="B35" s="26" t="s">
-        <v>1964</v>
-      </c>
-      <c r="C35" s="31" t="s">
-        <v>1963</v>
-      </c>
-      <c r="D35" s="26" t="s">
-        <v>1962</v>
-      </c>
-      <c r="E35" s="26">
-        <v>8</v>
       </c>
       <c r="F35" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28">
-        <v>1</v>
-      </c>
-      <c r="I35" s="30" t="s">
-        <v>1961</v>
-      </c>
-      <c r="J35" s="26">
-        <v>0.4</v>
-      </c>
-      <c r="K35" s="26">
-        <v>60</v>
-      </c>
     </row>
     <row r="36" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="29" t="str">
-        <f>[1]Enums!$A$12</f>
-        <v>1.1.0</v>
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>2157</v>
-      </c>
-      <c r="C36" s="28" t="s">
-        <v>2147</v>
+        <v>1982</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>1981</v>
       </c>
       <c r="D36" s="28" t="str">
         <f>[1]Enums!$A$40</f>
@@ -13391,233 +13490,506 @@
       <c r="E36" s="26">
         <v>8</v>
       </c>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28">
+      <c r="F36" s="26" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="29" t="str">
-        <f>[1]Enums!$A$12</f>
-        <v>1.1.0</v>
+        <f>[1]Enums!$A$5</f>
+        <v>1.0.3</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>2156</v>
-      </c>
-      <c r="C37" s="28" t="s">
-        <v>2148</v>
-      </c>
-      <c r="D37" s="28" t="str">
-        <f>[1]Enums!$A$40</f>
-        <v>PC Item</v>
+        <v>1980</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>1979</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>1965</v>
       </c>
       <c r="E37" s="26">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="F37" s="26" t="b">
+        <v>1</v>
       </c>
       <c r="G37" s="28"/>
       <c r="H37" s="28">
         <v>1</v>
       </c>
+      <c r="I37" s="31" t="s">
+        <v>1968</v>
+      </c>
+      <c r="J37" s="26">
+        <v>10</v>
+      </c>
     </row>
     <row r="38" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="29" t="str">
+        <f>[1]Enums!$A$5</f>
+        <v>1.0.3</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>1978</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>1977</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>1965</v>
+      </c>
+      <c r="E38" s="26">
+        <v>4</v>
+      </c>
+      <c r="F38" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="31" t="s">
+        <v>1968</v>
+      </c>
+      <c r="J38" s="26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A39" s="29" t="str">
+        <f>[1]Enums!$A$5</f>
+        <v>1.0.3</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>1976</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>1975</v>
+      </c>
+      <c r="D39" s="28" t="s">
+        <v>1965</v>
+      </c>
+      <c r="E39" s="26">
+        <v>4</v>
+      </c>
+      <c r="F39" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="31" t="s">
+        <v>1968</v>
+      </c>
+      <c r="J39" s="26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A40" s="29" t="str">
+        <f>[1]Enums!$A$5</f>
+        <v>1.0.3</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>1974</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>1973</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>1965</v>
+      </c>
+      <c r="E40" s="26">
+        <v>4</v>
+      </c>
+      <c r="F40" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" s="28"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="31" t="s">
+        <v>1968</v>
+      </c>
+      <c r="J40" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="29" t="str">
+        <f>[1]Enums!$A$5</f>
+        <v>1.0.3</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>1972</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>1971</v>
+      </c>
+      <c r="D41" s="28" t="s">
+        <v>1965</v>
+      </c>
+      <c r="E41" s="26">
+        <v>4</v>
+      </c>
+      <c r="F41" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" s="28"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="31" t="s">
+        <v>1968</v>
+      </c>
+      <c r="J41" s="26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A42" s="29" t="str">
+        <f>[1]Enums!$A$5</f>
+        <v>1.0.3</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>1970</v>
+      </c>
+      <c r="C42" s="31" t="s">
+        <v>1969</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>1965</v>
+      </c>
+      <c r="E42" s="26">
+        <v>4</v>
+      </c>
+      <c r="F42" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="31" t="s">
+        <v>1968</v>
+      </c>
+      <c r="J42" s="26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A43" s="29" t="str">
+        <f>[1]Enums!$A$5</f>
+        <v>1.0.3</v>
+      </c>
+      <c r="B43" s="31" t="s">
+        <v>1967</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>1966</v>
+      </c>
+      <c r="D43" s="31" t="s">
+        <v>1965</v>
+      </c>
+      <c r="E43" s="26">
+        <v>4</v>
+      </c>
+      <c r="F43" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G43" s="28"/>
+      <c r="H43" s="28"/>
+    </row>
+    <row r="44" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A44" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B44" s="26" t="s">
+        <v>1964</v>
+      </c>
+      <c r="C44" s="31" t="s">
+        <v>1963</v>
+      </c>
+      <c r="D44" s="26" t="s">
+        <v>1962</v>
+      </c>
+      <c r="E44" s="26">
+        <v>8</v>
+      </c>
+      <c r="F44" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G44" s="28"/>
+      <c r="H44" s="28">
+        <v>1</v>
+      </c>
+      <c r="I44" s="30" t="s">
+        <v>1961</v>
+      </c>
+      <c r="J44" s="26">
+        <v>0.4</v>
+      </c>
+      <c r="K44" s="26">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A45" s="29" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B45" s="13" t="s">
         <v>2155</v>
       </c>
-      <c r="C38" s="28" t="s">
-        <v>2149</v>
-      </c>
-      <c r="D38" s="28" t="str">
+      <c r="C45" s="28" t="s">
+        <v>2145</v>
+      </c>
+      <c r="D45" s="28" t="str">
         <f>[1]Enums!$A$40</f>
         <v>PC Item</v>
       </c>
-      <c r="E38" s="26">
+      <c r="E45" s="26">
         <v>8</v>
       </c>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28">
+      <c r="F45" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="29" t="str">
+    <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A46" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B46" s="13" t="s">
         <v>2154</v>
       </c>
-      <c r="C39" s="28" t="s">
-        <v>2150</v>
-      </c>
-      <c r="D39" s="28" t="str">
+      <c r="C46" s="28" t="s">
+        <v>2146</v>
+      </c>
+      <c r="D46" s="28" t="str">
         <f>[1]Enums!$A$40</f>
         <v>PC Item</v>
       </c>
-      <c r="E39" s="26">
+      <c r="E46" s="26">
         <v>8</v>
       </c>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28">
+      <c r="F46" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46" s="28"/>
+      <c r="H46" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="29" t="str">
+    <row r="47" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A47" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B47" s="13" t="s">
         <v>2153</v>
       </c>
-      <c r="C40" s="26" t="s">
-        <v>2151</v>
-      </c>
-      <c r="D40" s="28" t="str">
+      <c r="C47" s="28" t="s">
+        <v>2147</v>
+      </c>
+      <c r="D47" s="28" t="str">
         <f>[1]Enums!$A$40</f>
         <v>PC Item</v>
       </c>
-      <c r="E40" s="26">
+      <c r="E47" s="26">
         <v>8</v>
       </c>
-      <c r="G40" s="28"/>
-      <c r="H40" s="28">
+      <c r="F47" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" s="28"/>
+      <c r="H47" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="29" t="str">
+    <row r="48" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A48" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B48" s="13" t="s">
         <v>2152</v>
       </c>
-      <c r="C41" s="26" t="s">
-        <v>2159</v>
-      </c>
-      <c r="D41" s="28" t="str">
+      <c r="C48" s="28" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D48" s="28" t="str">
         <f>[1]Enums!$A$40</f>
         <v>PC Item</v>
       </c>
-      <c r="E41" s="26">
+      <c r="E48" s="26">
         <v>8</v>
       </c>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28">
+      <c r="F48" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" s="28"/>
+      <c r="H48" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-    </row>
-    <row r="43" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="G43" s="28"/>
-      <c r="H43" s="28"/>
-    </row>
-    <row r="44" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
-    </row>
-    <row r="45" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="G45" s="28"/>
-      <c r="H45" s="28"/>
-    </row>
-    <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="G46" s="28"/>
-      <c r="H46" s="28"/>
-    </row>
-    <row r="47" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="G47" s="28"/>
-      <c r="H47" s="28"/>
-    </row>
-    <row r="48" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="G48" s="28"/>
-      <c r="H48" s="28"/>
-    </row>
-    <row r="49" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A49" s="29" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>2151</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>2149</v>
+      </c>
+      <c r="D49" s="28" t="str">
+        <f>[1]Enums!$A$40</f>
+        <v>PC Item</v>
+      </c>
+      <c r="E49" s="26">
+        <v>8</v>
+      </c>
+      <c r="F49" s="26" t="b">
+        <v>0</v>
+      </c>
       <c r="G49" s="28"/>
-      <c r="H49" s="28"/>
-    </row>
-    <row r="50" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="H49" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A50" s="29" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>2150</v>
+      </c>
+      <c r="C50" s="26" t="s">
+        <v>2157</v>
+      </c>
+      <c r="D50" s="28" t="str">
+        <f>[1]Enums!$A$40</f>
+        <v>PC Item</v>
+      </c>
+      <c r="E50" s="26">
+        <v>8</v>
+      </c>
+      <c r="F50" s="26" t="b">
+        <v>0</v>
+      </c>
       <c r="G50" s="28"/>
-      <c r="H50" s="28"/>
-    </row>
-    <row r="51" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="H50" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="G51" s="28"/>
       <c r="H51" s="28"/>
     </row>
-    <row r="52" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="G52" s="28"/>
       <c r="H52" s="28"/>
     </row>
-    <row r="53" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="G53" s="28"/>
       <c r="H53" s="28"/>
     </row>
-    <row r="54" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="G54" s="28"/>
       <c r="H54" s="28"/>
     </row>
-    <row r="55" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="G55" s="28"/>
       <c r="H55" s="28"/>
     </row>
-    <row r="56" spans="3:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="C56" s="28"/>
-      <c r="D56" s="28"/>
-      <c r="E56" s="28"/>
-      <c r="F56" s="28"/>
+    <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="G56" s="28"/>
       <c r="H56" s="28"/>
     </row>
-    <row r="57" spans="3:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="28"/>
+    <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="G57" s="28"/>
       <c r="H57" s="28"/>
     </row>
-    <row r="58" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="G58" s="28"/>
       <c r="H58" s="28"/>
     </row>
-    <row r="59" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="G59" s="28"/>
       <c r="H59" s="28"/>
     </row>
-    <row r="60" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="G60" s="28"/>
       <c r="H60" s="28"/>
     </row>
-    <row r="61" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="G61" s="28"/>
       <c r="H61" s="28"/>
     </row>
-    <row r="62" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="G62" s="28"/>
       <c r="H62" s="28"/>
     </row>
-    <row r="63" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="G63" s="28"/>
       <c r="H63" s="28"/>
     </row>
-    <row r="64" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="G64" s="28"/>
       <c r="H64" s="28"/>
     </row>
-    <row r="65" spans="7:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="C65" s="28"/>
+      <c r="D65" s="28"/>
+      <c r="E65" s="28"/>
+      <c r="F65" s="28"/>
       <c r="G65" s="28"/>
       <c r="H65" s="28"/>
     </row>
-    <row r="66" spans="7:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="C66" s="28"/>
+      <c r="D66" s="28"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="28"/>
       <c r="G66" s="28"/>
       <c r="H66" s="28"/>
+    </row>
+    <row r="67" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="G67" s="28"/>
+      <c r="H67" s="28"/>
+    </row>
+    <row r="68" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="G68" s="28"/>
+      <c r="H68" s="28"/>
+    </row>
+    <row r="69" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="G69" s="28"/>
+      <c r="H69" s="28"/>
+    </row>
+    <row r="70" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="G70" s="28"/>
+      <c r="H70" s="28"/>
+    </row>
+    <row r="71" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="G71" s="28"/>
+      <c r="H71" s="28"/>
+    </row>
+    <row r="72" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="G72" s="28"/>
+      <c r="H72" s="28"/>
+    </row>
+    <row r="73" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="G73" s="28"/>
+      <c r="H73" s="28"/>
+    </row>
+    <row r="74" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="G74" s="28"/>
+      <c r="H74" s="28"/>
+    </row>
+    <row r="75" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="G75" s="28"/>
+      <c r="H75" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13656,10 +14028,10 @@
         <v>Game ID</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>2064</v>
+        <v>2062</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>2063</v>
+        <v>2061</v>
       </c>
       <c r="E1" s="39" t="str">
         <f>"Tile Entity "&amp;'[1]Game IDs'!$A$1</f>
@@ -13669,7 +14041,7 @@
         <v>1960</v>
       </c>
       <c r="G1" s="38" t="s">
-        <v>2062</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -13678,10 +14050,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>2061</v>
+        <v>2059</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>2060</v>
+        <v>2058</v>
       </c>
       <c r="D2" s="27" t="str">
         <f xml:space="preserve"> C2</f>
@@ -13691,7 +14063,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>2059</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -13700,10 +14072,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>2058</v>
+        <v>2056</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>2057</v>
+        <v>2055</v>
       </c>
       <c r="D3" s="27" t="str">
         <f xml:space="preserve"> C3</f>
@@ -13713,27 +14085,27 @@
         <v>0</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>2056</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
-        <v>2055</v>
+        <v>2053</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>2054</v>
+        <v>2052</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>2053</v>
+        <v>2051</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>2052</v>
+        <v>2050</v>
       </c>
       <c r="F4" s="27">
         <v>0</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>2051</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -13741,22 +14113,22 @@
         <v>1949</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>2048</v>
+        <v>2046</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
       <c r="F5" s="27">
         <v>3000</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>2046</v>
+        <v>2044</v>
       </c>
     </row>
   </sheetData>
@@ -16829,7 +17201,7 @@
   </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9:E9"/>
     </sheetView>
   </sheetViews>
@@ -17033,7 +17405,7 @@
         <v>74</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" ref="C10:C32" si="1">E10&amp;" "&amp;$C$1</f>
+        <f t="shared" ref="C10:C31" si="1">E10&amp;" "&amp;$C$1</f>
         <v>Antimony Trioxide Catalyst</v>
       </c>
       <c r="D10" t="str">
@@ -17435,7 +17807,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>2146</v>
+        <v>2144</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="1"/>
@@ -17456,7 +17828,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>2145</v>
+        <v>2143</v>
       </c>
       <c r="C32" t="str">
         <f>E32&amp;" "&amp;$C$1</f>
@@ -17477,7 +17849,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>2158</v>
+        <v>2156</v>
       </c>
       <c r="C33" t="str">
         <f>E33&amp;" "&amp;$C$1</f>
@@ -43765,16 +44137,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B334" s="13" t="s">
-        <v>2068</v>
+        <v>2066</v>
       </c>
       <c r="C334" s="13" t="s">
-        <v>2072</v>
+        <v>2070</v>
       </c>
       <c r="D334" s="13" t="s">
-        <v>2076</v>
+        <v>2074</v>
       </c>
       <c r="E334" s="13" t="s">
-        <v>2080</v>
+        <v>2078</v>
       </c>
       <c r="F334" s="16" t="str">
         <f t="shared" ref="F334" si="28">L334&amp;" ("&amp;$J334&amp;")"</f>
@@ -43823,16 +44195,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B335" s="13" t="s">
-        <v>2067</v>
+        <v>2065</v>
       </c>
       <c r="C335" s="13" t="s">
-        <v>2071</v>
+        <v>2069</v>
       </c>
       <c r="D335" s="13" t="s">
-        <v>2075</v>
+        <v>2073</v>
       </c>
       <c r="E335" s="13" t="s">
-        <v>2079</v>
+        <v>2077</v>
       </c>
       <c r="F335" s="16" t="str">
         <f t="shared" ref="F335:F337" si="32">L335&amp;" ("&amp;$J335&amp;")"</f>
@@ -43881,16 +44253,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B336" s="13" t="s">
-        <v>2066</v>
+        <v>2064</v>
       </c>
       <c r="C336" s="13" t="s">
-        <v>2070</v>
+        <v>2068</v>
       </c>
       <c r="D336" s="13" t="s">
-        <v>2074</v>
+        <v>2072</v>
       </c>
       <c r="E336" s="13" t="s">
-        <v>2078</v>
+        <v>2076</v>
       </c>
       <c r="F336" s="16" t="str">
         <f t="shared" si="32"/>
@@ -43939,16 +44311,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B337" s="13" t="s">
-        <v>2065</v>
+        <v>2063</v>
       </c>
       <c r="C337" s="13" t="s">
-        <v>2069</v>
+        <v>2067</v>
       </c>
       <c r="D337" s="13" t="s">
-        <v>2073</v>
+        <v>2071</v>
       </c>
       <c r="E337" s="13" t="s">
-        <v>2077</v>
+        <v>2075</v>
       </c>
       <c r="F337" s="16" t="str">
         <f t="shared" si="32"/>
@@ -43997,16 +44369,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B338" s="13" t="s">
-        <v>2096</v>
+        <v>2094</v>
       </c>
       <c r="C338" s="13" t="s">
-        <v>2112</v>
+        <v>2110</v>
       </c>
       <c r="D338" s="13" t="s">
-        <v>2128</v>
+        <v>2126</v>
       </c>
       <c r="E338" s="13" t="s">
-        <v>2144</v>
+        <v>2142</v>
       </c>
       <c r="F338" s="16" t="str">
         <f t="shared" ref="F338:F340" si="36">L338&amp;" ("&amp;$J338&amp;")"</f>
@@ -44055,16 +44427,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B339" s="13" t="s">
-        <v>2095</v>
+        <v>2093</v>
       </c>
       <c r="C339" s="13" t="s">
-        <v>2111</v>
+        <v>2109</v>
       </c>
       <c r="D339" s="13" t="s">
-        <v>2127</v>
+        <v>2125</v>
       </c>
       <c r="E339" s="13" t="s">
-        <v>2143</v>
+        <v>2141</v>
       </c>
       <c r="F339" s="16" t="str">
         <f t="shared" si="36"/>
@@ -44113,16 +44485,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B340" s="13" t="s">
-        <v>2094</v>
+        <v>2092</v>
       </c>
       <c r="C340" s="13" t="s">
-        <v>2110</v>
+        <v>2108</v>
       </c>
       <c r="D340" s="13" t="s">
-        <v>2126</v>
+        <v>2124</v>
       </c>
       <c r="E340" s="13" t="s">
-        <v>2142</v>
+        <v>2140</v>
       </c>
       <c r="F340" s="16" t="str">
         <f t="shared" si="36"/>
@@ -44168,16 +44540,16 @@
     <row r="341" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A341" s="4"/>
       <c r="B341" s="13" t="s">
-        <v>2093</v>
+        <v>2091</v>
       </c>
       <c r="C341" s="13" t="s">
-        <v>2109</v>
+        <v>2107</v>
       </c>
       <c r="D341" s="13" t="s">
-        <v>2125</v>
+        <v>2123</v>
       </c>
       <c r="E341" s="13" t="s">
-        <v>2141</v>
+        <v>2139</v>
       </c>
       <c r="F341" s="16" t="str">
         <f t="shared" ref="F341" si="40">L341&amp;" ("&amp;$J341&amp;")"</f>
@@ -44223,16 +44595,16 @@
     <row r="342" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A342" s="4"/>
       <c r="B342" s="13" t="s">
-        <v>2092</v>
+        <v>2090</v>
       </c>
       <c r="C342" s="13" t="s">
-        <v>2108</v>
+        <v>2106</v>
       </c>
       <c r="D342" s="13" t="s">
-        <v>2124</v>
+        <v>2122</v>
       </c>
       <c r="E342" s="13" t="s">
-        <v>2140</v>
+        <v>2138</v>
       </c>
       <c r="F342" s="16" t="str">
         <f t="shared" ref="F342:F343" si="44">L342&amp;" ("&amp;$J342&amp;")"</f>
@@ -44281,16 +44653,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B343" s="13" t="s">
-        <v>2091</v>
+        <v>2089</v>
       </c>
       <c r="C343" s="13" t="s">
-        <v>2107</v>
+        <v>2105</v>
       </c>
       <c r="D343" s="13" t="s">
-        <v>2123</v>
+        <v>2121</v>
       </c>
       <c r="E343" s="13" t="s">
-        <v>2139</v>
+        <v>2137</v>
       </c>
       <c r="F343" s="16" t="str">
         <f t="shared" si="44"/>
@@ -44335,142 +44707,142 @@
     </row>
     <row r="344" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B344" s="13" t="s">
-        <v>2090</v>
+        <v>2088</v>
       </c>
       <c r="C344" s="13" t="s">
-        <v>2106</v>
+        <v>2104</v>
       </c>
       <c r="D344" s="13" t="s">
-        <v>2122</v>
+        <v>2120</v>
       </c>
       <c r="E344" s="13" t="s">
-        <v>2138</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="345" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B345" s="13" t="s">
-        <v>2089</v>
+        <v>2087</v>
       </c>
       <c r="C345" s="13" t="s">
-        <v>2105</v>
+        <v>2103</v>
       </c>
       <c r="D345" s="13" t="s">
-        <v>2121</v>
+        <v>2119</v>
       </c>
       <c r="E345" s="13" t="s">
-        <v>2137</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="346" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B346" s="13" t="s">
-        <v>2088</v>
+        <v>2086</v>
       </c>
       <c r="C346" s="13" t="s">
-        <v>2104</v>
+        <v>2102</v>
       </c>
       <c r="D346" s="13" t="s">
-        <v>2120</v>
+        <v>2118</v>
       </c>
       <c r="E346" s="13" t="s">
-        <v>2136</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="347" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B347" s="13" t="s">
-        <v>2087</v>
+        <v>2085</v>
       </c>
       <c r="C347" s="13" t="s">
-        <v>2103</v>
+        <v>2101</v>
       </c>
       <c r="D347" s="13" t="s">
-        <v>2119</v>
+        <v>2117</v>
       </c>
       <c r="E347" s="13" t="s">
-        <v>2135</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="348" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B348" s="13" t="s">
-        <v>2086</v>
+        <v>2084</v>
       </c>
       <c r="C348" s="13" t="s">
-        <v>2102</v>
+        <v>2100</v>
       </c>
       <c r="D348" s="13" t="s">
-        <v>2118</v>
+        <v>2116</v>
       </c>
       <c r="E348" s="13" t="s">
-        <v>2134</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="349" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B349" s="13" t="s">
-        <v>2085</v>
+        <v>2083</v>
       </c>
       <c r="C349" s="13" t="s">
-        <v>2101</v>
+        <v>2099</v>
       </c>
       <c r="D349" s="13" t="s">
-        <v>2117</v>
+        <v>2115</v>
       </c>
       <c r="E349" s="13" t="s">
-        <v>2133</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="350" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B350" s="13" t="s">
-        <v>2084</v>
+        <v>2082</v>
       </c>
       <c r="C350" s="13" t="s">
-        <v>2100</v>
+        <v>2098</v>
       </c>
       <c r="D350" s="13" t="s">
-        <v>2116</v>
+        <v>2114</v>
       </c>
       <c r="E350" s="13" t="s">
-        <v>2132</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="351" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B351" s="13" t="s">
-        <v>2083</v>
+        <v>2081</v>
       </c>
       <c r="C351" s="13" t="s">
-        <v>2099</v>
+        <v>2097</v>
       </c>
       <c r="D351" s="13" t="s">
-        <v>2115</v>
+        <v>2113</v>
       </c>
       <c r="E351" s="13" t="s">
-        <v>2131</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="352" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B352" s="13" t="s">
-        <v>2082</v>
+        <v>2080</v>
       </c>
       <c r="C352" s="13" t="s">
-        <v>2098</v>
+        <v>2096</v>
       </c>
       <c r="D352" s="13" t="s">
-        <v>2114</v>
+        <v>2112</v>
       </c>
       <c r="E352" s="13" t="s">
-        <v>2130</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="353" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B353" s="13" t="s">
-        <v>2081</v>
+        <v>2079</v>
       </c>
       <c r="C353" s="13" t="s">
-        <v>2097</v>
+        <v>2095</v>
       </c>
       <c r="D353" s="13" t="s">
-        <v>2113</v>
+        <v>2111</v>
       </c>
       <c r="E353" s="13" t="s">
-        <v>2129</v>
+        <v>2127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added light to items - doesnt compile
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Walter\Documents\GitHub\polycraftworld\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PolycraftWorld\polycraft\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="59355" yWindow="495" windowWidth="19200" windowHeight="19455" tabRatio="877"/>
+    <workbookView xWindow="60285" yWindow="495" windowWidth="19200" windowHeight="19455" tabRatio="877"/>
   </bookViews>
   <sheets>
     <sheet name="Custom Objects" sheetId="41" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2211" uniqueCount="2179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2213" uniqueCount="2181">
   <si>
     <t>Ore</t>
   </si>
@@ -6130,9 +6130,6 @@
     <t>3p</t>
   </si>
   <si>
-    <t>MaxLightLevel, LightLevelDecreaseByDistance, ViewingConeAngle</t>
-  </si>
-  <si>
     <t>Flashlight</t>
   </si>
   <si>
@@ -6578,6 +6575,15 @@
   </si>
   <si>
     <t>Scuba Tank (Pro)</t>
+  </si>
+  <si>
+    <t>12Z</t>
+  </si>
+  <si>
+    <t>13d</t>
+  </si>
+  <si>
+    <t>Flashlight Range</t>
   </si>
 </sst>
 </file>
@@ -12181,6 +12187,50 @@
             <v>Solid</v>
           </cell>
         </row>
+        <row r="353">
+          <cell r="B353" t="str">
+            <v>Potassium Persulfate</v>
+          </cell>
+          <cell r="C353" t="str">
+            <v>K2S2O8</v>
+          </cell>
+          <cell r="D353" t="str">
+            <v>Solid</v>
+          </cell>
+        </row>
+        <row r="354">
+          <cell r="B354" t="str">
+            <v>Potassium Bisulfate</v>
+          </cell>
+          <cell r="C354" t="str">
+            <v>KHSO4</v>
+          </cell>
+          <cell r="D354" t="str">
+            <v>Solid</v>
+          </cell>
+        </row>
+        <row r="355">
+          <cell r="B355" t="str">
+            <v>Salt Water</v>
+          </cell>
+          <cell r="C355" t="str">
+            <v>H20</v>
+          </cell>
+          <cell r="D355" t="str">
+            <v>Liquid</v>
+          </cell>
+        </row>
+        <row r="356">
+          <cell r="B356" t="str">
+            <v>Isoprene</v>
+          </cell>
+          <cell r="C356" t="str">
+            <v>CH2=C(CH3)CH=CH2</v>
+          </cell>
+          <cell r="D356" t="str">
+            <v>Liquid</v>
+          </cell>
+        </row>
       </sheetData>
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
@@ -12479,10 +12529,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:R75"/>
+  <dimension ref="A1:S75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12495,13 +12545,14 @@
     <col min="6" max="6" width="17.42578125" style="26" customWidth="1"/>
     <col min="7" max="7" width="6" style="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="102.85546875" style="26" customWidth="1"/>
-    <col min="10" max="11" width="8.85546875" style="26"/>
-    <col min="12" max="12" width="11.85546875" style="26" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="26"/>
+    <col min="9" max="9" width="15.140625" style="26" customWidth="1"/>
+    <col min="10" max="10" width="102.85546875" style="26" customWidth="1"/>
+    <col min="11" max="12" width="8.85546875" style="26"/>
+    <col min="13" max="13" width="11.85546875" style="26" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="str">
         <f>[1]Enums!$A$1</f>
         <v>Version</v>
@@ -12511,64 +12562,67 @@
         <v>Game ID</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>2158</v>
+        <v>2157</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="I1" s="35" t="s">
+        <v>2180</v>
+      </c>
+      <c r="J1" s="35" t="s">
         <v>1959</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="K1" s="35" t="s">
         <v>1958</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="L1" s="35" t="s">
         <v>1957</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="M1" s="35" t="s">
         <v>1956</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="N1" s="35" t="s">
         <v>1955</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="O1" s="35" t="s">
         <v>1954</v>
       </c>
-      <c r="O1" s="35" t="s">
+      <c r="P1" s="35" t="s">
         <v>1953</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="Q1" s="35" t="s">
         <v>1952</v>
       </c>
-      <c r="Q1" s="35" t="s">
+      <c r="R1" s="35" t="s">
         <v>1951</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="S1" s="35" t="s">
         <v>1950</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="D2" s="32" t="str">
         <f>[1]Enums!$A$40</f>
@@ -12581,16 +12635,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="D3" s="32" t="str">
         <f>[1]Enums!$A$40</f>
@@ -12603,16 +12657,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>2165</v>
+        <v>2164</v>
       </c>
       <c r="D4" s="32" t="str">
         <f>[1]Enums!$A$36</f>
@@ -12627,38 +12681,38 @@
       <c r="H4" s="26">
         <v>1</v>
       </c>
-      <c r="I4" s="31" t="s">
-        <v>2032</v>
-      </c>
-      <c r="J4" s="26">
+      <c r="J4" s="31" t="s">
+        <v>2031</v>
+      </c>
+      <c r="K4" s="26">
         <v>1000</v>
       </c>
-      <c r="K4" s="26">
+      <c r="L4" s="26">
         <v>1</v>
       </c>
-      <c r="L4" s="26">
+      <c r="M4" s="26">
         <v>6</v>
       </c>
-      <c r="M4" s="26">
+      <c r="N4" s="26">
         <v>2</v>
       </c>
-      <c r="N4" s="26">
+      <c r="O4" s="26">
         <v>5</v>
       </c>
-      <c r="O4" s="26">
+      <c r="P4" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>2159</v>
+        <v>2158</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>2166</v>
+        <v>2165</v>
       </c>
       <c r="D5" s="32" t="str">
         <f>[1]Enums!$A$36</f>
@@ -12673,38 +12727,41 @@
       <c r="H5" s="26">
         <v>1</v>
       </c>
-      <c r="I5" s="31" t="s">
-        <v>2032</v>
-      </c>
-      <c r="J5" s="26">
+      <c r="I5" s="26">
+        <v>10</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>2031</v>
+      </c>
+      <c r="K5" s="26">
         <v>1500</v>
       </c>
-      <c r="K5" s="26">
+      <c r="L5" s="26">
         <v>1</v>
       </c>
-      <c r="L5" s="26">
+      <c r="M5" s="26">
         <v>8</v>
       </c>
-      <c r="M5" s="26">
+      <c r="N5" s="26">
         <v>2</v>
       </c>
-      <c r="N5" s="26">
+      <c r="O5" s="26">
         <v>5</v>
       </c>
-      <c r="O5" s="26">
+      <c r="P5" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>2160</v>
+        <v>2159</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="D6" s="32" t="str">
         <f>[1]Enums!$A$36</f>
@@ -12719,38 +12776,41 @@
       <c r="H6" s="26">
         <v>1</v>
       </c>
-      <c r="I6" s="31" t="s">
-        <v>2032</v>
-      </c>
-      <c r="J6" s="26">
+      <c r="I6" s="26">
+        <v>30</v>
+      </c>
+      <c r="J6" s="31" t="s">
+        <v>2031</v>
+      </c>
+      <c r="K6" s="26">
         <v>2000</v>
       </c>
-      <c r="K6" s="26">
+      <c r="L6" s="26">
         <v>1</v>
       </c>
-      <c r="L6" s="26">
+      <c r="M6" s="26">
         <v>10</v>
       </c>
-      <c r="M6" s="26">
+      <c r="N6" s="26">
         <v>2</v>
       </c>
-      <c r="N6" s="26">
+      <c r="O6" s="26">
         <v>5</v>
       </c>
-      <c r="O6" s="26">
+      <c r="P6" s="26">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>2161</v>
+        <v>2160</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="D7" s="32" t="str">
         <f>[1]Enums!$A$36</f>
@@ -12765,38 +12825,41 @@
       <c r="H7" s="26">
         <v>1</v>
       </c>
-      <c r="I7" s="31" t="s">
-        <v>2032</v>
-      </c>
-      <c r="J7" s="26">
+      <c r="I7" s="26">
+        <v>50</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>2031</v>
+      </c>
+      <c r="K7" s="26">
         <v>2500</v>
       </c>
-      <c r="K7" s="26">
+      <c r="L7" s="26">
         <v>1</v>
       </c>
-      <c r="L7" s="26">
+      <c r="M7" s="26">
         <v>12</v>
       </c>
-      <c r="M7" s="26">
+      <c r="N7" s="26">
         <v>2</v>
       </c>
-      <c r="N7" s="26">
+      <c r="O7" s="26">
         <v>5</v>
       </c>
-      <c r="O7" s="26">
+      <c r="P7" s="26">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="D8" s="32" t="str">
         <f>[1]Enums!$A$37</f>
@@ -12809,20 +12872,11 @@
       <c r="H8" s="26">
         <v>1</v>
       </c>
-      <c r="I8" s="26" t="s">
-        <v>2029</v>
-      </c>
-      <c r="J8" s="26">
-        <v>15</v>
-      </c>
-      <c r="K8" s="26">
-        <v>0.5</v>
-      </c>
-      <c r="L8" s="26">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I8" s="26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -12844,23 +12898,23 @@
       <c r="H9" s="26">
         <v>1</v>
       </c>
-      <c r="I9" s="31" t="s">
+      <c r="J9" s="31" t="s">
         <v>2026</v>
       </c>
-      <c r="J9" s="26">
+      <c r="K9" s="26">
         <v>5000</v>
       </c>
-      <c r="K9" s="26">
+      <c r="L9" s="26">
         <v>1</v>
       </c>
-      <c r="L9" s="26">
+      <c r="M9" s="26">
         <v>0.4</v>
       </c>
-      <c r="M9" s="26">
+      <c r="N9" s="26">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -12879,14 +12933,14 @@
       <c r="H10" s="26">
         <v>1</v>
       </c>
-      <c r="I10" s="31" t="s">
+      <c r="J10" s="31" t="s">
         <v>2023</v>
       </c>
-      <c r="J10" s="26">
+      <c r="K10" s="26">
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -12909,7 +12963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -12933,21 +12987,21 @@
       <c r="H12" s="26">
         <v>1</v>
       </c>
-      <c r="I12" s="26" t="s">
+      <c r="J12" s="26" t="s">
         <v>2018</v>
       </c>
-      <c r="J12" s="26">
+      <c r="K12" s="26">
         <v>3</v>
       </c>
-      <c r="K12" s="26">
+      <c r="L12" s="26">
         <v>0.6</v>
       </c>
-      <c r="L12" s="26" t="str">
+      <c r="M12" s="26" t="str">
         <f>'[1]Blocks (MC)'!$A$22</f>
         <v>1.0.0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -12956,7 +13010,7 @@
         <v>2017</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>2175</v>
+        <v>2174</v>
       </c>
       <c r="D13" s="32" t="str">
         <f>[1]Enums!$A$35</f>
@@ -12969,26 +13023,26 @@
       <c r="H13" s="26">
         <v>1</v>
       </c>
-      <c r="I13" s="26" t="s">
+      <c r="J13" s="26" t="s">
         <v>2016</v>
       </c>
-      <c r="J13" s="26">
+      <c r="K13" s="26">
         <v>5000</v>
       </c>
-      <c r="K13" s="26">
+      <c r="L13" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>2176</v>
+        <v>2175</v>
       </c>
       <c r="D14" s="32" t="str">
         <f>[1]Enums!$A$35</f>
@@ -13001,26 +13055,26 @@
       <c r="H14" s="26">
         <v>1</v>
       </c>
-      <c r="I14" s="26" t="s">
+      <c r="J14" s="26" t="s">
         <v>2016</v>
       </c>
-      <c r="J14" s="26">
+      <c r="K14" s="26">
         <v>10000</v>
       </c>
-      <c r="K14" s="26">
+      <c r="L14" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>2177</v>
+        <v>2176</v>
       </c>
       <c r="D15" s="32" t="str">
         <f>[1]Enums!$A$35</f>
@@ -13033,26 +13087,26 @@
       <c r="H15" s="26">
         <v>1</v>
       </c>
-      <c r="I15" s="26" t="s">
+      <c r="J15" s="26" t="s">
         <v>2016</v>
       </c>
-      <c r="J15" s="26">
+      <c r="K15" s="26">
         <v>25000</v>
       </c>
-      <c r="K15" s="26">
+      <c r="L15" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>2174</v>
+        <v>2173</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
       <c r="D16" s="32" t="str">
         <f>[1]Enums!$A$35</f>
@@ -13065,17 +13119,17 @@
       <c r="H16" s="26">
         <v>1</v>
       </c>
-      <c r="I16" s="26" t="s">
+      <c r="J16" s="26" t="s">
         <v>2016</v>
       </c>
-      <c r="J16" s="26">
+      <c r="K16" s="26">
         <v>50000</v>
       </c>
-      <c r="K16" s="26">
+      <c r="L16" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -13098,7 +13152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -13117,7 +13171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -13136,7 +13190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -13155,7 +13209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -13174,7 +13228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -13183,7 +13237,7 @@
         <v>2005</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
       <c r="D22" s="26" t="str">
         <f>[1]Enums!$A$40</f>
@@ -13194,17 +13248,18 @@
       </c>
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
-    </row>
-    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="I22" s="28"/>
+    </row>
+    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>2162</v>
+        <v>2161</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>2169</v>
+        <v>2168</v>
       </c>
       <c r="D23" s="26" t="str">
         <f>[1]Enums!$A$40</f>
@@ -13215,17 +13270,18 @@
       </c>
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
-    </row>
-    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="I23" s="28"/>
+    </row>
+    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>2163</v>
+        <v>2162</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="D24" s="26" t="str">
         <f>[1]Enums!$A$40</f>
@@ -13236,17 +13292,18 @@
       </c>
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
-    </row>
-    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="I24" s="28"/>
+    </row>
+    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>2164</v>
+        <v>2163</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
       <c r="D25" s="26" t="str">
         <f>[1]Enums!$A$40</f>
@@ -13257,8 +13314,9 @@
       </c>
       <c r="G25" s="28"/>
       <c r="H25" s="28"/>
-    </row>
-    <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="I25" s="28"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -13283,7 +13341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -13302,7 +13360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -13321,7 +13379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -13340,7 +13398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -13358,14 +13416,14 @@
       <c r="F30" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="I30" s="26" t="s">
+      <c r="J30" s="26" t="s">
         <v>1994</v>
       </c>
-      <c r="J30" s="26">
+      <c r="K30" s="26">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -13387,7 +13445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -13404,14 +13462,14 @@
       <c r="H32" s="27">
         <v>1</v>
       </c>
-      <c r="I32" s="27" t="s">
+      <c r="J32" s="27" t="s">
         <v>1989</v>
       </c>
-      <c r="J32" s="27">
+      <c r="K32" s="27">
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -13431,7 +13489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -13450,7 +13508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -13472,7 +13530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
@@ -13494,7 +13552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="29" t="str">
         <f>[1]Enums!$A$5</f>
         <v>1.0.3</v>
@@ -13518,14 +13576,15 @@
       <c r="H37" s="28">
         <v>1</v>
       </c>
-      <c r="I37" s="31" t="s">
+      <c r="I37" s="28"/>
+      <c r="J37" s="31" t="s">
         <v>1968</v>
       </c>
-      <c r="J37" s="26">
+      <c r="K37" s="26">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="29" t="str">
         <f>[1]Enums!$A$5</f>
         <v>1.0.3</v>
@@ -13547,14 +13606,15 @@
       </c>
       <c r="G38" s="28"/>
       <c r="H38" s="28"/>
-      <c r="I38" s="31" t="s">
+      <c r="I38" s="28"/>
+      <c r="J38" s="31" t="s">
         <v>1968</v>
       </c>
-      <c r="J38" s="26">
+      <c r="K38" s="26">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="29" t="str">
         <f>[1]Enums!$A$5</f>
         <v>1.0.3</v>
@@ -13576,14 +13636,15 @@
       </c>
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
-      <c r="I39" s="31" t="s">
+      <c r="I39" s="28"/>
+      <c r="J39" s="31" t="s">
         <v>1968</v>
       </c>
-      <c r="J39" s="26">
+      <c r="K39" s="26">
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="29" t="str">
         <f>[1]Enums!$A$5</f>
         <v>1.0.3</v>
@@ -13605,14 +13666,15 @@
       </c>
       <c r="G40" s="28"/>
       <c r="H40" s="28"/>
-      <c r="I40" s="31" t="s">
+      <c r="I40" s="28"/>
+      <c r="J40" s="31" t="s">
         <v>1968</v>
       </c>
-      <c r="J40" s="26">
+      <c r="K40" s="26">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="29" t="str">
         <f>[1]Enums!$A$5</f>
         <v>1.0.3</v>
@@ -13634,14 +13696,15 @@
       </c>
       <c r="G41" s="28"/>
       <c r="H41" s="28"/>
-      <c r="I41" s="31" t="s">
+      <c r="I41" s="28"/>
+      <c r="J41" s="31" t="s">
         <v>1968</v>
       </c>
-      <c r="J41" s="26">
+      <c r="K41" s="26">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="29" t="str">
         <f>[1]Enums!$A$5</f>
         <v>1.0.3</v>
@@ -13663,14 +13726,15 @@
       </c>
       <c r="G42" s="28"/>
       <c r="H42" s="28"/>
-      <c r="I42" s="31" t="s">
+      <c r="I42" s="28"/>
+      <c r="J42" s="31" t="s">
         <v>1968</v>
       </c>
-      <c r="J42" s="26">
+      <c r="K42" s="26">
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="29" t="str">
         <f>[1]Enums!$A$5</f>
         <v>1.0.3</v>
@@ -13692,8 +13756,9 @@
       </c>
       <c r="G43" s="28"/>
       <c r="H43" s="28"/>
-    </row>
-    <row r="44" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="I43" s="28"/>
+    </row>
+    <row r="44" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
@@ -13717,26 +13782,27 @@
       <c r="H44" s="28">
         <v>1</v>
       </c>
-      <c r="I44" s="30" t="s">
+      <c r="I44" s="28"/>
+      <c r="J44" s="30" t="s">
         <v>1961</v>
       </c>
-      <c r="J44" s="26">
+      <c r="K44" s="26">
         <v>0.4</v>
       </c>
-      <c r="K44" s="26">
+      <c r="L44" s="26">
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>2155</v>
+        <v>2154</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>2145</v>
+        <v>2144</v>
       </c>
       <c r="D45" s="28" t="str">
         <f>[1]Enums!$A$40</f>
@@ -13752,17 +13818,18 @@
       <c r="H45" s="28">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="I45" s="28"/>
+    </row>
+    <row r="46" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>2154</v>
+        <v>2153</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="D46" s="28" t="str">
         <f>[1]Enums!$A$40</f>
@@ -13778,17 +13845,18 @@
       <c r="H46" s="28">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="I46" s="28"/>
+    </row>
+    <row r="47" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>2153</v>
+        <v>2152</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="D47" s="28" t="str">
         <f>[1]Enums!$A$40</f>
@@ -13804,17 +13872,18 @@
       <c r="H47" s="28">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="I47" s="28"/>
+    </row>
+    <row r="48" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>2152</v>
+        <v>2151</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>2148</v>
+        <v>2147</v>
       </c>
       <c r="D48" s="28" t="str">
         <f>[1]Enums!$A$40</f>
@@ -13830,17 +13899,18 @@
       <c r="H48" s="28">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I48" s="28"/>
+    </row>
+    <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>2151</v>
+        <v>2150</v>
       </c>
       <c r="C49" s="26" t="s">
-        <v>2149</v>
+        <v>2148</v>
       </c>
       <c r="D49" s="28" t="str">
         <f>[1]Enums!$A$40</f>
@@ -13856,17 +13926,18 @@
       <c r="H49" s="28">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I49" s="28"/>
+    </row>
+    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>2150</v>
+        <v>2149</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>2157</v>
+        <v>2156</v>
       </c>
       <c r="D50" s="28" t="str">
         <f>[1]Enums!$A$40</f>
@@ -13882,114 +13953,140 @@
       <c r="H50" s="28">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I50" s="28"/>
+    </row>
+    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G51" s="28"/>
       <c r="H51" s="28"/>
-    </row>
-    <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I51" s="28"/>
+    </row>
+    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G52" s="28"/>
       <c r="H52" s="28"/>
-    </row>
-    <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I52" s="28"/>
+    </row>
+    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G53" s="28"/>
       <c r="H53" s="28"/>
-    </row>
-    <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I53" s="28"/>
+    </row>
+    <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G54" s="28"/>
       <c r="H54" s="28"/>
-    </row>
-    <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I54" s="28"/>
+    </row>
+    <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G55" s="28"/>
       <c r="H55" s="28"/>
-    </row>
-    <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I55" s="28"/>
+    </row>
+    <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G56" s="28"/>
       <c r="H56" s="28"/>
-    </row>
-    <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I56" s="28"/>
+    </row>
+    <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G57" s="28"/>
       <c r="H57" s="28"/>
-    </row>
-    <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I57" s="28"/>
+    </row>
+    <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G58" s="28"/>
       <c r="H58" s="28"/>
-    </row>
-    <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I58" s="28"/>
+    </row>
+    <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G59" s="28"/>
       <c r="H59" s="28"/>
-    </row>
-    <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I59" s="28"/>
+    </row>
+    <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G60" s="28"/>
       <c r="H60" s="28"/>
-    </row>
-    <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I60" s="28"/>
+    </row>
+    <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G61" s="28"/>
       <c r="H61" s="28"/>
-    </row>
-    <row r="62" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I61" s="28"/>
+    </row>
+    <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G62" s="28"/>
       <c r="H62" s="28"/>
-    </row>
-    <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I62" s="28"/>
+    </row>
+    <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G63" s="28"/>
       <c r="H63" s="28"/>
-    </row>
-    <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I63" s="28"/>
+    </row>
+    <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G64" s="28"/>
       <c r="H64" s="28"/>
-    </row>
-    <row r="65" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I64" s="28"/>
+    </row>
+    <row r="65" spans="3:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C65" s="28"/>
       <c r="D65" s="28"/>
       <c r="E65" s="28"/>
       <c r="F65" s="28"/>
       <c r="G65" s="28"/>
       <c r="H65" s="28"/>
-    </row>
-    <row r="66" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I65" s="28"/>
+    </row>
+    <row r="66" spans="3:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C66" s="28"/>
       <c r="D66" s="28"/>
       <c r="E66" s="28"/>
       <c r="F66" s="28"/>
       <c r="G66" s="28"/>
       <c r="H66" s="28"/>
-    </row>
-    <row r="67" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I66" s="28"/>
+    </row>
+    <row r="67" spans="3:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G67" s="28"/>
       <c r="H67" s="28"/>
-    </row>
-    <row r="68" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I67" s="28"/>
+    </row>
+    <row r="68" spans="3:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G68" s="28"/>
       <c r="H68" s="28"/>
-    </row>
-    <row r="69" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I68" s="28"/>
+    </row>
+    <row r="69" spans="3:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G69" s="28"/>
       <c r="H69" s="28"/>
-    </row>
-    <row r="70" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I69" s="28"/>
+    </row>
+    <row r="70" spans="3:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G70" s="28"/>
       <c r="H70" s="28"/>
-    </row>
-    <row r="71" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I70" s="28"/>
+    </row>
+    <row r="71" spans="3:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G71" s="28"/>
       <c r="H71" s="28"/>
-    </row>
-    <row r="72" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I71" s="28"/>
+    </row>
+    <row r="72" spans="3:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G72" s="28"/>
       <c r="H72" s="28"/>
-    </row>
-    <row r="73" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I72" s="28"/>
+    </row>
+    <row r="73" spans="3:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G73" s="28"/>
       <c r="H73" s="28"/>
-    </row>
-    <row r="74" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I73" s="28"/>
+    </row>
+    <row r="74" spans="3:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G74" s="28"/>
       <c r="H74" s="28"/>
-    </row>
-    <row r="75" spans="3:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="I74" s="28"/>
+    </row>
+    <row r="75" spans="3:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G75" s="28"/>
       <c r="H75" s="28"/>
+      <c r="I75" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14028,10 +14125,10 @@
         <v>Game ID</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="E1" s="39" t="str">
         <f>"Tile Entity "&amp;'[1]Game IDs'!$A$1</f>
@@ -14041,7 +14138,7 @@
         <v>1960</v>
       </c>
       <c r="G1" s="38" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -14050,10 +14147,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="D2" s="27" t="str">
         <f xml:space="preserve"> C2</f>
@@ -14063,7 +14160,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -14072,10 +14169,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="D3" s="27" t="str">
         <f xml:space="preserve"> C3</f>
@@ -14085,27 +14182,27 @@
         <v>0</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="F4" s="27">
         <v>0</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -14113,22 +14210,22 @@
         <v>1949</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="F5" s="27">
         <v>3000</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
     </row>
   </sheetData>
@@ -14145,7 +14242,7 @@
   <dimension ref="A1:R120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+      <selection activeCell="J19" sqref="J19:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15392,7 +15489,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K23" s="8">
         <v>6</v>
@@ -17199,10 +17296,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:E9"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17807,7 +17904,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>2144</v>
+        <v>2143</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="1"/>
@@ -17828,7 +17925,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
       <c r="C32" t="str">
         <f>E32&amp;" "&amp;$C$1</f>
@@ -17849,7 +17946,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>2156</v>
+        <v>2155</v>
       </c>
       <c r="C33" t="str">
         <f>E33&amp;" "&amp;$C$1</f>
@@ -17862,6 +17959,48 @@
       <c r="E33" t="str">
         <f>[1]Compounds!$B$351</f>
         <v>Lead Oxide</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>2178</v>
+      </c>
+      <c r="C34" t="str">
+        <f>E34&amp;" "&amp;$C$1</f>
+        <v>Ruthenium Catalyst</v>
+      </c>
+      <c r="D34" t="str">
+        <f>[1]Elements!$B$1</f>
+        <v>Element</v>
+      </c>
+      <c r="E34" t="str">
+        <f>[1]Elements!$B$45</f>
+        <v>Ruthenium</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>2179</v>
+      </c>
+      <c r="C35" t="str">
+        <f>E35&amp;" "&amp;$C$1</f>
+        <v>Osmium Catalyst</v>
+      </c>
+      <c r="D35" t="str">
+        <f>[1]Elements!$B$1</f>
+        <v>Element</v>
+      </c>
+      <c r="E35" t="str">
+        <f>[1]Elements!$B$77</f>
+        <v>Osmium</v>
       </c>
     </row>
   </sheetData>
@@ -25283,8 +25422,8 @@
   </sheetPr>
   <dimension ref="A1:O353"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="R121" sqref="R121"/>
+    <sheetView topLeftCell="A331" workbookViewId="0">
+      <selection activeCell="N361" sqref="N361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -38937,7 +39076,10 @@
       </c>
     </row>
     <row r="242" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A242" s="4"/>
+      <c r="A242" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
       <c r="B242" s="13" t="s">
         <v>698</v>
       </c>
@@ -44137,16 +44279,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B334" s="13" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="C334" s="13" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="D334" s="13" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="E334" s="13" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="F334" s="16" t="str">
         <f t="shared" ref="F334" si="28">L334&amp;" ("&amp;$J334&amp;")"</f>
@@ -44195,16 +44337,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B335" s="13" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="C335" s="13" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="D335" s="13" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="E335" s="13" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="F335" s="16" t="str">
         <f t="shared" ref="F335:F337" si="32">L335&amp;" ("&amp;$J335&amp;")"</f>
@@ -44253,16 +44395,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B336" s="13" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="C336" s="13" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="D336" s="13" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="E336" s="13" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="F336" s="16" t="str">
         <f t="shared" si="32"/>
@@ -44311,16 +44453,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B337" s="13" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="C337" s="13" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="D337" s="13" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="E337" s="13" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="F337" s="16" t="str">
         <f t="shared" si="32"/>
@@ -44369,16 +44511,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B338" s="13" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="C338" s="13" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
       <c r="D338" s="13" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
       <c r="E338" s="13" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="F338" s="16" t="str">
         <f t="shared" ref="F338:F340" si="36">L338&amp;" ("&amp;$J338&amp;")"</f>
@@ -44427,16 +44569,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B339" s="13" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="C339" s="13" t="s">
-        <v>2109</v>
+        <v>2108</v>
       </c>
       <c r="D339" s="13" t="s">
-        <v>2125</v>
+        <v>2124</v>
       </c>
       <c r="E339" s="13" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
       <c r="F339" s="16" t="str">
         <f t="shared" si="36"/>
@@ -44485,16 +44627,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B340" s="13" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="C340" s="13" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
       <c r="D340" s="13" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
       <c r="E340" s="13" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="F340" s="16" t="str">
         <f t="shared" si="36"/>
@@ -44540,16 +44682,16 @@
     <row r="341" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A341" s="4"/>
       <c r="B341" s="13" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="C341" s="13" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
       <c r="D341" s="13" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
       <c r="E341" s="13" t="s">
-        <v>2139</v>
+        <v>2138</v>
       </c>
       <c r="F341" s="16" t="str">
         <f t="shared" ref="F341" si="40">L341&amp;" ("&amp;$J341&amp;")"</f>
@@ -44595,16 +44737,16 @@
     <row r="342" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A342" s="4"/>
       <c r="B342" s="13" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
       <c r="C342" s="13" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="D342" s="13" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
       <c r="E342" s="13" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
       <c r="F342" s="16" t="str">
         <f t="shared" ref="F342:F343" si="44">L342&amp;" ("&amp;$J342&amp;")"</f>
@@ -44653,16 +44795,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B343" s="13" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
       <c r="C343" s="13" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
       <c r="D343" s="13" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
       <c r="E343" s="13" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
       <c r="F343" s="16" t="str">
         <f t="shared" si="44"/>
@@ -44706,143 +44848,319 @@
       </c>
     </row>
     <row r="344" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A344" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
       <c r="B344" s="13" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
       <c r="C344" s="13" t="s">
-        <v>2104</v>
+        <v>2103</v>
       </c>
       <c r="D344" s="13" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="E344" s="13" t="s">
-        <v>2136</v>
+        <v>2135</v>
+      </c>
+      <c r="F344" s="16" t="str">
+        <f t="shared" ref="F344" si="48">L344&amp;" ("&amp;$J344&amp;")"</f>
+        <v>Bag (Potassium Persulfate)</v>
+      </c>
+      <c r="G344" s="16" t="str">
+        <f t="shared" ref="G344" si="49">M344&amp;" ("&amp;$J344&amp;")"</f>
+        <v>Sack (Potassium Persulfate)</v>
+      </c>
+      <c r="H344" s="16" t="str">
+        <f t="shared" ref="H344" si="50">N344&amp;" ("&amp;$J344&amp;")"</f>
+        <v>Powder Keg (Potassium Persulfate)</v>
+      </c>
+      <c r="I344" s="16" t="str">
+        <f t="shared" ref="I344" si="51">O344&amp;" ("&amp;$J344&amp;")"</f>
+        <v>Chemical Silo (Potassium Persulfate)</v>
+      </c>
+      <c r="J344" s="16" t="str">
+        <f>[1]Compounds!$B353</f>
+        <v>Potassium Persulfate</v>
+      </c>
+      <c r="K344" t="str">
+        <f>[1]Compounds!$D353</f>
+        <v>Solid</v>
+      </c>
+      <c r="L344" s="4" t="str">
+        <f>IF(K344=[1]Enums!$A$18, [1]Enums!$A$23, IF(K344=[1]Enums!$B$22, [1]Enums!$A$22, [1]Enums!$A$21))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M344" s="4" t="str">
+        <f>IF(K344=[1]Enums!$A$18, [1]Enums!$A$26, IF(K344=[1]Enums!$B$25, [1]Enums!$A$25, [1]Enums!$A$24))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N344" s="4" t="str">
+        <f>IF(K344=[1]Enums!$A$18, [1]Enums!$A$29, IF(K344=[1]Enums!$B$22, [1]Enums!$A$28, [1]Enums!$A$27))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O344" s="4" t="str">
+        <f>IF(K344=[1]Enums!$A$18, [1]Enums!$A$32, IF(K344=[1]Enums!$B$22, [1]Enums!$A$31, [1]Enums!$A$30))</f>
+        <v>Chemical Silo</v>
       </c>
     </row>
     <row r="345" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A345" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
       <c r="B345" s="13" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="C345" s="13" t="s">
-        <v>2103</v>
+        <v>2102</v>
       </c>
       <c r="D345" s="13" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="E345" s="13" t="s">
-        <v>2135</v>
+        <v>2134</v>
+      </c>
+      <c r="F345" s="16" t="str">
+        <f t="shared" ref="F345" si="52">L345&amp;" ("&amp;$J345&amp;")"</f>
+        <v>Bag (Potassium Bisulfate)</v>
+      </c>
+      <c r="G345" s="16" t="str">
+        <f t="shared" ref="G345" si="53">M345&amp;" ("&amp;$J345&amp;")"</f>
+        <v>Sack (Potassium Bisulfate)</v>
+      </c>
+      <c r="H345" s="16" t="str">
+        <f t="shared" ref="H345" si="54">N345&amp;" ("&amp;$J345&amp;")"</f>
+        <v>Powder Keg (Potassium Bisulfate)</v>
+      </c>
+      <c r="I345" s="16" t="str">
+        <f t="shared" ref="I345" si="55">O345&amp;" ("&amp;$J345&amp;")"</f>
+        <v>Chemical Silo (Potassium Bisulfate)</v>
+      </c>
+      <c r="J345" s="16" t="str">
+        <f>[1]Compounds!$B354</f>
+        <v>Potassium Bisulfate</v>
+      </c>
+      <c r="K345" t="str">
+        <f>[1]Compounds!$D354</f>
+        <v>Solid</v>
+      </c>
+      <c r="L345" s="4" t="str">
+        <f>IF(K345=[1]Enums!$A$18, [1]Enums!$A$23, IF(K345=[1]Enums!$B$22, [1]Enums!$A$22, [1]Enums!$A$21))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M345" s="4" t="str">
+        <f>IF(K345=[1]Enums!$A$18, [1]Enums!$A$26, IF(K345=[1]Enums!$B$25, [1]Enums!$A$25, [1]Enums!$A$24))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N345" s="4" t="str">
+        <f>IF(K345=[1]Enums!$A$18, [1]Enums!$A$29, IF(K345=[1]Enums!$B$22, [1]Enums!$A$28, [1]Enums!$A$27))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O345" s="4" t="str">
+        <f>IF(K345=[1]Enums!$A$18, [1]Enums!$A$32, IF(K345=[1]Enums!$B$22, [1]Enums!$A$31, [1]Enums!$A$30))</f>
+        <v>Chemical Silo</v>
       </c>
     </row>
     <row r="346" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A346" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
       <c r="B346" s="13" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="C346" s="13" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="D346" s="13" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="E346" s="13" t="s">
-        <v>2134</v>
+        <v>2133</v>
+      </c>
+      <c r="F346" s="16" t="str">
+        <f t="shared" ref="F346" si="56">L346&amp;" ("&amp;$J346&amp;")"</f>
+        <v>Vial (Salt Water)</v>
+      </c>
+      <c r="G346" s="16" t="str">
+        <f t="shared" ref="G346" si="57">M346&amp;" ("&amp;$J346&amp;")"</f>
+        <v>Beaker (Salt Water)</v>
+      </c>
+      <c r="H346" s="16" t="str">
+        <f t="shared" ref="H346" si="58">N346&amp;" ("&amp;$J346&amp;")"</f>
+        <v>Drum (Salt Water)</v>
+      </c>
+      <c r="I346" s="16" t="str">
+        <f t="shared" ref="I346" si="59">O346&amp;" ("&amp;$J346&amp;")"</f>
+        <v>Chemical Vat (Salt Water)</v>
+      </c>
+      <c r="J346" s="16" t="str">
+        <f>[1]Compounds!$B355</f>
+        <v>Salt Water</v>
+      </c>
+      <c r="K346" t="str">
+        <f>[1]Compounds!$D355</f>
+        <v>Liquid</v>
+      </c>
+      <c r="L346" s="4" t="str">
+        <f>IF(K346=[1]Enums!$A$18, [1]Enums!$A$23, IF(K346=[1]Enums!$B$22, [1]Enums!$A$22, [1]Enums!$A$21))</f>
+        <v>Vial</v>
+      </c>
+      <c r="M346" s="4" t="str">
+        <f>IF(K346=[1]Enums!$A$18, [1]Enums!$A$26, IF(K346=[1]Enums!$B$25, [1]Enums!$A$25, [1]Enums!$A$24))</f>
+        <v>Beaker</v>
+      </c>
+      <c r="N346" s="4" t="str">
+        <f>IF(K346=[1]Enums!$A$18, [1]Enums!$A$29, IF(K346=[1]Enums!$B$22, [1]Enums!$A$28, [1]Enums!$A$27))</f>
+        <v>Drum</v>
+      </c>
+      <c r="O346" s="4" t="str">
+        <f>IF(K346=[1]Enums!$A$18, [1]Enums!$A$32, IF(K346=[1]Enums!$B$22, [1]Enums!$A$31, [1]Enums!$A$30))</f>
+        <v>Chemical Vat</v>
       </c>
     </row>
     <row r="347" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A347" s="4" t="str">
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
       <c r="B347" s="13" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="C347" s="13" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
       <c r="D347" s="13" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="E347" s="13" t="s">
-        <v>2133</v>
+        <v>2132</v>
+      </c>
+      <c r="F347" s="16" t="str">
+        <f t="shared" ref="F347" si="60">L347&amp;" ("&amp;$J347&amp;")"</f>
+        <v>Vial (Isoprene)</v>
+      </c>
+      <c r="G347" s="16" t="str">
+        <f t="shared" ref="G347" si="61">M347&amp;" ("&amp;$J347&amp;")"</f>
+        <v>Beaker (Isoprene)</v>
+      </c>
+      <c r="H347" s="16" t="str">
+        <f t="shared" ref="H347" si="62">N347&amp;" ("&amp;$J347&amp;")"</f>
+        <v>Drum (Isoprene)</v>
+      </c>
+      <c r="I347" s="16" t="str">
+        <f t="shared" ref="I347" si="63">O347&amp;" ("&amp;$J347&amp;")"</f>
+        <v>Chemical Vat (Isoprene)</v>
+      </c>
+      <c r="J347" s="16" t="str">
+        <f>[1]Compounds!$B356</f>
+        <v>Isoprene</v>
+      </c>
+      <c r="K347" t="str">
+        <f>[1]Compounds!$D356</f>
+        <v>Liquid</v>
+      </c>
+      <c r="L347" s="4" t="str">
+        <f>IF(K347=[1]Enums!$A$18, [1]Enums!$A$23, IF(K347=[1]Enums!$B$22, [1]Enums!$A$22, [1]Enums!$A$21))</f>
+        <v>Vial</v>
+      </c>
+      <c r="M347" s="4" t="str">
+        <f>IF(K347=[1]Enums!$A$18, [1]Enums!$A$26, IF(K347=[1]Enums!$B$25, [1]Enums!$A$25, [1]Enums!$A$24))</f>
+        <v>Beaker</v>
+      </c>
+      <c r="N347" s="4" t="str">
+        <f>IF(K347=[1]Enums!$A$18, [1]Enums!$A$29, IF(K347=[1]Enums!$B$22, [1]Enums!$A$28, [1]Enums!$A$27))</f>
+        <v>Drum</v>
+      </c>
+      <c r="O347" s="4" t="str">
+        <f>IF(K347=[1]Enums!$A$18, [1]Enums!$A$32, IF(K347=[1]Enums!$B$22, [1]Enums!$A$31, [1]Enums!$A$30))</f>
+        <v>Chemical Vat</v>
       </c>
     </row>
     <row r="348" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B348" s="13" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="C348" s="13" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
       <c r="D348" s="13" t="s">
-        <v>2116</v>
+        <v>2115</v>
       </c>
       <c r="E348" s="13" t="s">
-        <v>2132</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="349" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B349" s="13" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="C349" s="13" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="D349" s="13" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="E349" s="13" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="350" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B350" s="13" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
       <c r="C350" s="13" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="D350" s="13" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="E350" s="13" t="s">
-        <v>2130</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="351" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B351" s="13" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
       <c r="C351" s="13" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="D351" s="13" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="E351" s="13" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="352" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B352" s="13" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
       <c r="C352" s="13" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="D352" s="13" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="E352" s="13" t="s">
-        <v>2128</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="353" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B353" s="13" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="C353" s="13" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="D353" s="13" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
       <c r="E353" s="13" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged 1.1.2 with Jim
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="65865" yWindow="495" windowWidth="19200" windowHeight="19455" tabRatio="877" activeTab="7"/>
+    <workbookView xWindow="65865" yWindow="495" windowWidth="19200" windowHeight="19455" tabRatio="877"/>
   </bookViews>
   <sheets>
     <sheet name="Custom Objects" sheetId="41" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2364" uniqueCount="2332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2362" uniqueCount="2330">
   <si>
     <t>Ore</t>
   </si>
@@ -6069,12 +6069,6 @@
   </si>
   <si>
     <t>3C</t>
-  </si>
-  <si>
-    <t>Wetsuit</t>
-  </si>
-  <si>
-    <t>3A</t>
   </si>
   <si>
     <t>AirUnitsFull, AirUnitsConsumePerTick</t>
@@ -7601,7 +7595,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3">
         <row r="22">
           <cell r="A22" t="str">
@@ -12943,8 +12937,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -13240,10 +13234,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:S74"/>
+  <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13273,25 +13267,25 @@
         <v>Game ID</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>2154</v>
+        <v>2152</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>2039</v>
+        <v>2037</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>2038</v>
+        <v>2036</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>2037</v>
+        <v>2035</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>2036</v>
+        <v>2034</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>2035</v>
+        <v>2033</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>2177</v>
+        <v>2175</v>
       </c>
       <c r="J1" s="35" t="s">
         <v>1959</v>
@@ -13330,10 +13324,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>2034</v>
+        <v>2032</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>2033</v>
+        <v>2031</v>
       </c>
       <c r="D2" s="32" t="str">
         <f>[1]Enums!$A$42</f>
@@ -13352,10 +13346,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>2031</v>
+        <v>2029</v>
       </c>
       <c r="D3" s="32" t="str">
         <f>[1]Enums!$A$42</f>
@@ -13374,10 +13368,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>2030</v>
+        <v>2028</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>2161</v>
+        <v>2159</v>
       </c>
       <c r="D4" s="32" t="str">
         <f>[1]Enums!$A$38</f>
@@ -13393,7 +13387,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="31" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="K4" s="26">
         <v>1000</v>
@@ -13420,10 +13414,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>2155</v>
+        <v>2153</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>2162</v>
+        <v>2160</v>
       </c>
       <c r="D5" s="32" t="str">
         <f>[1]Enums!$A$38</f>
@@ -13442,7 +13436,7 @@
         <v>10</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="K5" s="26">
         <v>1500</v>
@@ -13469,10 +13463,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>2156</v>
+        <v>2154</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>2163</v>
+        <v>2161</v>
       </c>
       <c r="D6" s="32" t="str">
         <f>[1]Enums!$A$38</f>
@@ -13491,7 +13485,7 @@
         <v>30</v>
       </c>
       <c r="J6" s="31" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="K6" s="26">
         <v>2000</v>
@@ -13518,10 +13512,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>2157</v>
+        <v>2155</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>2029</v>
+        <v>2027</v>
       </c>
       <c r="D7" s="32" t="str">
         <f>[1]Enums!$A$38</f>
@@ -13540,7 +13534,7 @@
         <v>80</v>
       </c>
       <c r="J7" s="31" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="K7" s="26">
         <v>2500</v>
@@ -13549,7 +13543,7 @@
         <v>1</v>
       </c>
       <c r="M7" s="26">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="N7" s="26">
         <v>2</v>
@@ -13558,7 +13552,7 @@
         <v>5</v>
       </c>
       <c r="P7" s="26">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -13567,10 +13561,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>2027</v>
+        <v>2025</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>2026</v>
+        <v>2024</v>
       </c>
       <c r="D8" s="32" t="str">
         <f>[1]Enums!$A$39</f>
@@ -13593,10 +13587,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="D9" s="32" t="str">
         <f>[1]Enums!$A$37</f>
@@ -13610,7 +13604,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="31" t="s">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="K9" s="26">
         <v>5000</v>
@@ -13631,10 +13625,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="32"/>
@@ -13645,7 +13639,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="31" t="s">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="K10" s="26">
         <v>0.3</v>
@@ -13657,10 +13651,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="D11" s="32" t="str">
         <f>[1]Enums!$A$40</f>
@@ -13680,10 +13674,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="D12" s="32" t="str">
         <f>[1]Enums!$A$40</f>
@@ -13699,7 +13693,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="K12" s="26">
         <v>3</v>
@@ -13718,10 +13712,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>2171</v>
+        <v>2169</v>
       </c>
       <c r="D13" s="32" t="str">
         <f>[1]Enums!$A$37</f>
@@ -13735,7 +13729,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="26" t="s">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="K13" s="26">
         <v>5000</v>
@@ -13750,10 +13744,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>2168</v>
+        <v>2166</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>2172</v>
+        <v>2170</v>
       </c>
       <c r="D14" s="32" t="str">
         <f>[1]Enums!$A$37</f>
@@ -13767,7 +13761,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="26" t="s">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="K14" s="26">
         <v>10000</v>
@@ -13782,10 +13776,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>2169</v>
+        <v>2167</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>2173</v>
+        <v>2171</v>
       </c>
       <c r="D15" s="32" t="str">
         <f>[1]Enums!$A$37</f>
@@ -13799,7 +13793,7 @@
         <v>1</v>
       </c>
       <c r="J15" s="26" t="s">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="K15" s="26">
         <v>25000</v>
@@ -13814,10 +13808,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>2170</v>
+        <v>2168</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>2174</v>
+        <v>2172</v>
       </c>
       <c r="D16" s="32" t="str">
         <f>[1]Enums!$A$37</f>
@@ -13831,7 +13825,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="26" t="s">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="K16" s="26">
         <v>50000</v>
@@ -13846,22 +13840,18 @@
         <v>1.0.0</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>2011</v>
-      </c>
-      <c r="D17" s="32" t="str">
-        <f>[1]Enums!$A$37</f>
-        <v>Armor</v>
-      </c>
-      <c r="E17" s="32"/>
+        <v>2009</v>
+      </c>
+      <c r="D17" s="34" t="str">
+        <f>[1]Enums!$A$43</f>
+        <v>PC Block</v>
+      </c>
       <c r="F17" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="H17" s="26">
-        <v>1</v>
-      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="29" t="str">
@@ -13869,14 +13859,14 @@
         <v>1.0.0</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>2010</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>2009</v>
+        <v>2008</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>2007</v>
       </c>
       <c r="D18" s="34" t="str">
-        <f>[1]Enums!$A$43</f>
-        <v>PC Block</v>
+        <f>[1]Enums!$A$44</f>
+        <v>Food</v>
       </c>
       <c r="F18" s="26" t="b">
         <v>1</v>
@@ -13888,10 +13878,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="D19" s="34" t="str">
         <f>[1]Enums!$A$44</f>
@@ -13901,20 +13891,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>2006</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>2005</v>
+        <v>2004</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>2003</v>
       </c>
       <c r="D20" s="34" t="str">
-        <f>[1]Enums!$A$44</f>
-        <v>Food</v>
+        <f>[1]Enums!$A$43</f>
+        <v>PC Block</v>
       </c>
       <c r="F20" s="26" t="b">
         <v>1</v>
@@ -13926,36 +13916,39 @@
         <v>1.0.0</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>2003</v>
-      </c>
-      <c r="D21" s="34" t="str">
-        <f>[1]Enums!$A$43</f>
-        <v>PC Block</v>
+        <v>2162</v>
+      </c>
+      <c r="D21" s="26" t="str">
+        <f>[1]Enums!$A$42</f>
+        <v>PC Item</v>
       </c>
       <c r="F21" s="26" t="b">
         <v>1</v>
       </c>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
     </row>
     <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B22" s="33" t="s">
-        <v>2002</v>
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>2156</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>2164</v>
+        <v>2163</v>
       </c>
       <c r="D22" s="26" t="str">
         <f>[1]Enums!$A$42</f>
         <v>PC Item</v>
       </c>
       <c r="F22" s="26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
@@ -13967,10 +13960,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>2158</v>
+        <v>2157</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>2165</v>
+        <v>2164</v>
       </c>
       <c r="D23" s="26" t="str">
         <f>[1]Enums!$A$42</f>
@@ -13989,10 +13982,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>2159</v>
+        <v>2158</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>2166</v>
+        <v>2165</v>
       </c>
       <c r="D24" s="26" t="str">
         <f>[1]Enums!$A$42</f>
@@ -14007,50 +14000,47 @@
     </row>
     <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="29" t="str">
-        <f>[1]Enums!$A$12</f>
-        <v>1.1.0</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>2160</v>
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>2001</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>2167</v>
-      </c>
-      <c r="D25" s="26" t="str">
+        <v>2000</v>
+      </c>
+      <c r="D25" s="28" t="str">
+        <f>[1]Enums!$A$39</f>
+        <v>Utility</v>
+      </c>
+      <c r="E25" s="26">
+        <v>4</v>
+      </c>
+      <c r="F25" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="29" t="str">
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>1999</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>1998</v>
+      </c>
+      <c r="D26" s="28" t="str">
         <f>[1]Enums!$A$42</f>
         <v>PC Item</v>
       </c>
-      <c r="F25" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-    </row>
-    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B26" s="33" t="s">
-        <v>2001</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>2000</v>
-      </c>
-      <c r="D26" s="28" t="str">
-        <f>[1]Enums!$A$39</f>
-        <v>Utility</v>
-      </c>
-      <c r="E26" s="26">
-        <v>4</v>
-      </c>
       <c r="F26" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="H26" s="26">
-        <v>1</v>
-      </c>
     </row>
     <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="29" t="str">
@@ -14058,10 +14048,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="D27" s="28" t="str">
         <f>[1]Enums!$A$42</f>
@@ -14077,10 +14067,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="D28" s="28" t="str">
         <f>[1]Enums!$A$42</f>
@@ -14096,63 +14086,64 @@
         <v>1.0.0</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="D29" s="28" t="str">
+        <f>[1]Enums!$A$43</f>
+        <v>PC Block</v>
+      </c>
+      <c r="F29" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" s="26" t="s">
+        <v>1991</v>
+      </c>
+      <c r="K29" s="26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="29" t="str">
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>1990</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>1989</v>
+      </c>
+      <c r="D30" s="28" t="str">
         <f>[1]Enums!$A$42</f>
         <v>PC Item</v>
       </c>
-      <c r="F29" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B30" s="33" t="s">
-        <v>1993</v>
-      </c>
-      <c r="C30" s="28" t="s">
-        <v>1992</v>
-      </c>
-      <c r="D30" s="28" t="str">
-        <f>[1]Enums!$A$43</f>
-        <v>PC Block</v>
+      <c r="E30" s="26">
+        <v>4</v>
       </c>
       <c r="F30" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="J30" s="26" t="s">
-        <v>1991</v>
-      </c>
-      <c r="K30" s="26">
-        <v>24</v>
-      </c>
     </row>
     <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
       </c>
-      <c r="B31" s="33" t="s">
-        <v>1990</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>1989</v>
+      <c r="B31" s="13" t="s">
+        <v>1988</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>1987</v>
       </c>
       <c r="D31" s="28" t="str">
         <f>[1]Enums!$A$42</f>
         <v>PC Item</v>
       </c>
-      <c r="E31" s="26">
-        <v>4</v>
-      </c>
-      <c r="F31" s="26" t="b">
+      <c r="E31" s="28"/>
+      <c r="F31" s="28" t="b">
         <v>1</v>
       </c>
     </row>
@@ -14162,56 +14153,58 @@
         <v>1.0.0</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>1988</v>
+        <v>1986</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>1987</v>
+        <v>1985</v>
       </c>
       <c r="D32" s="28" t="str">
         <f>[1]Enums!$A$42</f>
         <v>PC Item</v>
       </c>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28" t="b">
+      <c r="F32" s="26" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="29" t="str">
         <f>[1]Enums!$A$2</f>
         <v>1.0.0</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>1986</v>
+        <v>1984</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>1985</v>
-      </c>
-      <c r="D33" s="28" t="str">
+        <v>1983</v>
+      </c>
+      <c r="D33" s="32" t="str">
+        <f>[1]Enums!$A$39</f>
+        <v>Utility</v>
+      </c>
+      <c r="E33" s="26">
+        <v>4</v>
+      </c>
+      <c r="F33" s="26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A34" s="29" t="str">
+        <f>[1]Enums!$A$2</f>
+        <v>1.0.0</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>1982</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>1981</v>
+      </c>
+      <c r="D34" s="28" t="str">
         <f>[1]Enums!$A$42</f>
         <v>PC Item</v>
       </c>
-      <c r="F33" s="26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>1984</v>
-      </c>
-      <c r="C34" s="26" t="s">
-        <v>1983</v>
-      </c>
-      <c r="D34" s="32" t="str">
-        <f>[1]Enums!$A$39</f>
-        <v>Utility</v>
-      </c>
       <c r="E34" s="26">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F34" s="26" t="b">
         <v>1</v>
@@ -14219,24 +14212,34 @@
     </row>
     <row r="35" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="29" t="str">
-        <f>[1]Enums!$A$2</f>
-        <v>1.0.0</v>
+        <f>[1]Enums!$A$5</f>
+        <v>1.0.3</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>1982</v>
-      </c>
-      <c r="C35" s="26" t="s">
-        <v>1981</v>
-      </c>
-      <c r="D35" s="28" t="str">
-        <f>[1]Enums!$A$42</f>
-        <v>PC Item</v>
+        <v>1980</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>1979</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>1965</v>
       </c>
       <c r="E35" s="26">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F35" s="26" t="b">
         <v>1</v>
+      </c>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28">
+        <v>1</v>
+      </c>
+      <c r="I35" s="28"/>
+      <c r="J35" s="31" t="s">
+        <v>1968</v>
+      </c>
+      <c r="K35" s="26">
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="15" x14ac:dyDescent="0.2">
@@ -14245,10 +14248,10 @@
         <v>1.0.3</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>1980</v>
+        <v>1978</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>1979</v>
+        <v>1977</v>
       </c>
       <c r="D36" s="28" t="s">
         <v>1965</v>
@@ -14260,15 +14263,13 @@
         <v>1</v>
       </c>
       <c r="G36" s="28"/>
-      <c r="H36" s="28">
-        <v>1</v>
-      </c>
+      <c r="H36" s="28"/>
       <c r="I36" s="28"/>
       <c r="J36" s="31" t="s">
         <v>1968</v>
       </c>
       <c r="K36" s="26">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="15" x14ac:dyDescent="0.2">
@@ -14277,10 +14278,10 @@
         <v>1.0.3</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>1978</v>
+        <v>1976</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>1977</v>
+        <v>1975</v>
       </c>
       <c r="D37" s="28" t="s">
         <v>1965</v>
@@ -14298,7 +14299,7 @@
         <v>1968</v>
       </c>
       <c r="K37" s="26">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="15" x14ac:dyDescent="0.2">
@@ -14307,10 +14308,10 @@
         <v>1.0.3</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>1976</v>
+        <v>1974</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>1975</v>
+        <v>1973</v>
       </c>
       <c r="D38" s="28" t="s">
         <v>1965</v>
@@ -14328,7 +14329,7 @@
         <v>1968</v>
       </c>
       <c r="K38" s="26">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="15" x14ac:dyDescent="0.2">
@@ -14337,10 +14338,10 @@
         <v>1.0.3</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>1974</v>
+        <v>1972</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>1973</v>
+        <v>1971</v>
       </c>
       <c r="D39" s="28" t="s">
         <v>1965</v>
@@ -14358,7 +14359,7 @@
         <v>1968</v>
       </c>
       <c r="K39" s="26">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="15" x14ac:dyDescent="0.2">
@@ -14367,10 +14368,10 @@
         <v>1.0.3</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>1972</v>
+        <v>1970</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>1971</v>
+        <v>1969</v>
       </c>
       <c r="D40" s="28" t="s">
         <v>1965</v>
@@ -14388,7 +14389,7 @@
         <v>1968</v>
       </c>
       <c r="K40" s="26">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="15" x14ac:dyDescent="0.2">
@@ -14396,89 +14397,86 @@
         <f>[1]Enums!$A$5</f>
         <v>1.0.3</v>
       </c>
-      <c r="B41" s="13" t="s">
-        <v>1970</v>
+      <c r="B41" s="31" t="s">
+        <v>1967</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>1969</v>
-      </c>
-      <c r="D41" s="28" t="s">
+        <v>1966</v>
+      </c>
+      <c r="D41" s="31" t="s">
         <v>1965</v>
       </c>
       <c r="E41" s="26">
         <v>4</v>
       </c>
       <c r="F41" s="26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" s="28"/>
       <c r="H41" s="28"/>
       <c r="I41" s="28"/>
-      <c r="J41" s="31" t="s">
-        <v>1968</v>
-      </c>
-      <c r="K41" s="26">
-        <v>15</v>
-      </c>
     </row>
     <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="29" t="str">
-        <f>[1]Enums!$A$5</f>
-        <v>1.0.3</v>
-      </c>
-      <c r="B42" s="31" t="s">
-        <v>1967</v>
+        <f>[1]Enums!$A$12</f>
+        <v>1.1.0</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>1964</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>1966</v>
-      </c>
-      <c r="D42" s="31" t="s">
-        <v>1965</v>
+        <v>1963</v>
+      </c>
+      <c r="D42" s="26" t="s">
+        <v>1962</v>
       </c>
       <c r="E42" s="26">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F42" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
+      <c r="H42" s="28">
+        <v>1</v>
+      </c>
       <c r="I42" s="28"/>
+      <c r="J42" s="30" t="s">
+        <v>1961</v>
+      </c>
+      <c r="K42" s="26">
+        <v>0.4</v>
+      </c>
+      <c r="L42" s="26">
+        <v>60</v>
+      </c>
     </row>
     <row r="43" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="29" t="str">
         <f>[1]Enums!$A$12</f>
         <v>1.1.0</v>
       </c>
-      <c r="B43" s="26" t="s">
-        <v>1964</v>
-      </c>
-      <c r="C43" s="31" t="s">
-        <v>1963</v>
-      </c>
-      <c r="D43" s="26" t="s">
-        <v>1962</v>
+      <c r="B43" s="13" t="s">
+        <v>2149</v>
+      </c>
+      <c r="C43" s="28" t="s">
+        <v>2139</v>
+      </c>
+      <c r="D43" s="28" t="str">
+        <f>[1]Enums!$A$42</f>
+        <v>PC Item</v>
       </c>
       <c r="E43" s="26">
         <v>8</v>
       </c>
       <c r="F43" s="26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43" s="28"/>
       <c r="H43" s="28">
         <v>1</v>
       </c>
       <c r="I43" s="28"/>
-      <c r="J43" s="30" t="s">
-        <v>1961</v>
-      </c>
-      <c r="K43" s="26">
-        <v>0.4</v>
-      </c>
-      <c r="L43" s="26">
-        <v>60</v>
-      </c>
     </row>
     <row r="44" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="29" t="str">
@@ -14486,10 +14484,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>2151</v>
+        <v>2148</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
       <c r="D44" s="28" t="str">
         <f>[1]Enums!$A$42</f>
@@ -14513,10 +14511,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>2150</v>
+        <v>2147</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="D45" s="28" t="str">
         <f>[1]Enums!$A$42</f>
@@ -14540,10 +14538,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>2149</v>
+        <v>2146</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
       <c r="D46" s="28" t="str">
         <f>[1]Enums!$A$42</f>
@@ -14567,10 +14565,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>2148</v>
-      </c>
-      <c r="C47" s="28" t="s">
-        <v>2144</v>
+        <v>2145</v>
+      </c>
+      <c r="C47" s="26" t="s">
+        <v>2143</v>
       </c>
       <c r="D47" s="28" t="str">
         <f>[1]Enums!$A$42</f>
@@ -14594,10 +14592,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>2147</v>
+        <v>2144</v>
       </c>
       <c r="C48" s="26" t="s">
-        <v>2145</v>
+        <v>2151</v>
       </c>
       <c r="D48" s="28" t="str">
         <f>[1]Enums!$A$42</f>
@@ -14621,10 +14619,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>2146</v>
+        <v>2179</v>
       </c>
       <c r="C49" s="26" t="s">
-        <v>2153</v>
+        <v>2180</v>
       </c>
       <c r="D49" s="28" t="str">
         <f>[1]Enums!$A$42</f>
@@ -14640,7 +14638,11 @@
       <c r="H49" s="28">
         <v>1</v>
       </c>
-      <c r="I49" s="28"/>
+      <c r="I49" s="28">
+        <v>5</v>
+      </c>
+      <c r="J49" s="30"/>
+      <c r="K49" s="30"/>
     </row>
     <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="29" t="str">
@@ -14648,10 +14650,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B50" s="13" t="s">
+        <v>2178</v>
+      </c>
+      <c r="C50" s="26" t="s">
         <v>2181</v>
-      </c>
-      <c r="C50" s="26" t="s">
-        <v>2182</v>
       </c>
       <c r="D50" s="28" t="str">
         <f>[1]Enums!$A$42</f>
@@ -14668,7 +14670,7 @@
         <v>1</v>
       </c>
       <c r="I50" s="28">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J50" s="30"/>
       <c r="K50" s="30"/>
@@ -14679,10 +14681,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>2180</v>
+        <v>2177</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>2183</v>
+        <v>2182</v>
       </c>
       <c r="D51" s="28" t="str">
         <f>[1]Enums!$A$42</f>
@@ -14699,7 +14701,7 @@
         <v>1</v>
       </c>
       <c r="I51" s="28">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J51" s="30"/>
       <c r="K51" s="30"/>
@@ -14710,10 +14712,10 @@
         <v>1.1.0</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>2179</v>
+        <v>2176</v>
       </c>
       <c r="C52" s="26" t="s">
-        <v>2184</v>
+        <v>2183</v>
       </c>
       <c r="D52" s="28" t="str">
         <f>[1]Enums!$A$42</f>
@@ -14730,41 +14732,16 @@
         <v>1</v>
       </c>
       <c r="I52" s="28">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J52" s="30"/>
       <c r="K52" s="30"/>
     </row>
     <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A53" s="29" t="str">
-        <f>[1]Enums!$A$12</f>
-        <v>1.1.0</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>2178</v>
-      </c>
-      <c r="C53" s="26" t="s">
-        <v>2185</v>
-      </c>
-      <c r="D53" s="28" t="str">
-        <f>[1]Enums!$A$42</f>
-        <v>PC Item</v>
-      </c>
-      <c r="E53" s="26">
-        <v>8</v>
-      </c>
-      <c r="F53" s="26" t="b">
-        <v>0</v>
-      </c>
+      <c r="A53" s="29"/>
       <c r="G53" s="28"/>
-      <c r="H53" s="28">
-        <v>1</v>
-      </c>
-      <c r="I53" s="28">
-        <v>25</v>
-      </c>
-      <c r="J53" s="30"/>
-      <c r="K53" s="30"/>
+      <c r="H53" s="28"/>
+      <c r="I53" s="28"/>
     </row>
     <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="G54" s="28"/>
@@ -14812,6 +14789,10 @@
       <c r="I62" s="28"/>
     </row>
     <row r="63" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="28"/>
       <c r="G63" s="28"/>
       <c r="H63" s="28"/>
       <c r="I63" s="28"/>
@@ -14825,59 +14806,50 @@
       <c r="H64" s="28"/>
       <c r="I64" s="28"/>
     </row>
-    <row r="65" spans="3:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C65" s="28"/>
-      <c r="D65" s="28"/>
-      <c r="E65" s="28"/>
-      <c r="F65" s="28"/>
+    <row r="65" spans="7:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G65" s="28"/>
       <c r="H65" s="28"/>
       <c r="I65" s="28"/>
     </row>
-    <row r="66" spans="3:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="7:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G66" s="28"/>
       <c r="H66" s="28"/>
       <c r="I66" s="28"/>
     </row>
-    <row r="67" spans="3:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="67" spans="7:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G67" s="28"/>
       <c r="H67" s="28"/>
       <c r="I67" s="28"/>
     </row>
-    <row r="68" spans="3:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="68" spans="7:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G68" s="28"/>
       <c r="H68" s="28"/>
       <c r="I68" s="28"/>
     </row>
-    <row r="69" spans="3:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="69" spans="7:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G69" s="28"/>
       <c r="H69" s="28"/>
       <c r="I69" s="28"/>
     </row>
-    <row r="70" spans="3:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="70" spans="7:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G70" s="28"/>
       <c r="H70" s="28"/>
       <c r="I70" s="28"/>
     </row>
-    <row r="71" spans="3:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="71" spans="7:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G71" s="28"/>
       <c r="H71" s="28"/>
       <c r="I71" s="28"/>
     </row>
-    <row r="72" spans="3:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="72" spans="7:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G72" s="28"/>
       <c r="H72" s="28"/>
       <c r="I72" s="28"/>
     </row>
-    <row r="73" spans="3:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="73" spans="7:9" ht="15" x14ac:dyDescent="0.2">
       <c r="G73" s="28"/>
       <c r="H73" s="28"/>
       <c r="I73" s="28"/>
-    </row>
-    <row r="74" spans="3:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="G74" s="28"/>
-      <c r="H74" s="28"/>
-      <c r="I74" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14916,10 +14888,10 @@
         <v>Game ID</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>2058</v>
+        <v>2056</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>2057</v>
+        <v>2055</v>
       </c>
       <c r="E1" s="39" t="str">
         <f>"Tile Entity "&amp;'[1]Game IDs'!$A$1</f>
@@ -14929,7 +14901,7 @@
         <v>1960</v>
       </c>
       <c r="G1" s="38" t="s">
-        <v>2056</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -14938,10 +14910,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>2055</v>
+        <v>2053</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>2054</v>
+        <v>2052</v>
       </c>
       <c r="D2" s="27" t="str">
         <f xml:space="preserve"> C2</f>
@@ -14951,7 +14923,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>2053</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -14960,10 +14932,10 @@
         <v>1.0.0</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>2052</v>
+        <v>2050</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>2051</v>
+        <v>2049</v>
       </c>
       <c r="D3" s="27" t="str">
         <f xml:space="preserve"> C3</f>
@@ -14973,27 +14945,27 @@
         <v>0</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>2048</v>
+        <v>2046</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>2046</v>
+        <v>2044</v>
       </c>
       <c r="F4" s="27">
         <v>0</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>2045</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -15001,22 +14973,22 @@
         <v>1949</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>2044</v>
+        <v>2042</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>2043</v>
+        <v>2041</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>2042</v>
+        <v>2040</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>2041</v>
+        <v>2039</v>
       </c>
       <c r="F5" s="27">
         <v>3000</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>2040</v>
+        <v>2038</v>
       </c>
     </row>
   </sheetData>
@@ -18683,7 +18655,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>2140</v>
+        <v>2138</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="1"/>
@@ -18704,7 +18676,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>2139</v>
+        <v>2137</v>
       </c>
       <c r="C32" t="str">
         <f>E32&amp;" "&amp;$C$1</f>
@@ -18725,7 +18697,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>2152</v>
+        <v>2150</v>
       </c>
       <c r="C33" t="str">
         <f>E33&amp;" "&amp;$C$1</f>
@@ -18746,7 +18718,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>2175</v>
+        <v>2173</v>
       </c>
       <c r="C34" t="str">
         <f>E34&amp;" "&amp;$C$1</f>
@@ -18767,7 +18739,7 @@
         <v>1.1.0</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>2176</v>
+        <v>2174</v>
       </c>
       <c r="C35" t="str">
         <f>E35&amp;" "&amp;$C$1</f>
@@ -18788,7 +18760,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>2270</v>
+        <v>2268</v>
       </c>
       <c r="C36" t="str">
         <f>E36&amp;" "&amp;$C$1</f>
@@ -18809,7 +18781,7 @@
         <v>1.1.2</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>2331</v>
+        <v>2329</v>
       </c>
       <c r="C37" t="str">
         <f>E37&amp;" Pentoxide "&amp;$C$1</f>
@@ -26233,8 +26205,8 @@
   </sheetPr>
   <dimension ref="A1:O390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A355" workbookViewId="0">
-      <selection activeCell="N397" sqref="N397"/>
+    <sheetView topLeftCell="A355" workbookViewId="0">
+      <selection activeCell="J380" sqref="J380"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -45102,16 +45074,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B334" s="13" t="s">
-        <v>2062</v>
+        <v>2060</v>
       </c>
       <c r="C334" s="13" t="s">
-        <v>2066</v>
+        <v>2064</v>
       </c>
       <c r="D334" s="13" t="s">
-        <v>2070</v>
+        <v>2068</v>
       </c>
       <c r="E334" s="13" t="s">
-        <v>2074</v>
+        <v>2072</v>
       </c>
       <c r="F334" s="16" t="str">
         <f t="shared" ref="F334:F347" si="28">L334&amp;" ("&amp;$J334&amp;")"</f>
@@ -45160,16 +45132,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B335" s="13" t="s">
-        <v>2061</v>
+        <v>2059</v>
       </c>
       <c r="C335" s="13" t="s">
-        <v>2065</v>
+        <v>2063</v>
       </c>
       <c r="D335" s="13" t="s">
-        <v>2069</v>
+        <v>2067</v>
       </c>
       <c r="E335" s="13" t="s">
-        <v>2073</v>
+        <v>2071</v>
       </c>
       <c r="F335" s="16" t="str">
         <f t="shared" si="28"/>
@@ -45218,16 +45190,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B336" s="13" t="s">
-        <v>2060</v>
+        <v>2058</v>
       </c>
       <c r="C336" s="13" t="s">
-        <v>2064</v>
+        <v>2062</v>
       </c>
       <c r="D336" s="13" t="s">
-        <v>2068</v>
+        <v>2066</v>
       </c>
       <c r="E336" s="13" t="s">
-        <v>2072</v>
+        <v>2070</v>
       </c>
       <c r="F336" s="16" t="str">
         <f t="shared" si="28"/>
@@ -45276,16 +45248,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B337" s="13" t="s">
-        <v>2059</v>
+        <v>2057</v>
       </c>
       <c r="C337" s="13" t="s">
-        <v>2063</v>
+        <v>2061</v>
       </c>
       <c r="D337" s="13" t="s">
-        <v>2067</v>
+        <v>2065</v>
       </c>
       <c r="E337" s="13" t="s">
-        <v>2071</v>
+        <v>2069</v>
       </c>
       <c r="F337" s="16" t="str">
         <f t="shared" si="28"/>
@@ -45334,16 +45306,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B338" s="13" t="s">
-        <v>2090</v>
+        <v>2088</v>
       </c>
       <c r="C338" s="13" t="s">
-        <v>2106</v>
+        <v>2104</v>
       </c>
       <c r="D338" s="13" t="s">
-        <v>2122</v>
+        <v>2120</v>
       </c>
       <c r="E338" s="13" t="s">
-        <v>2138</v>
+        <v>2136</v>
       </c>
       <c r="F338" s="16" t="str">
         <f t="shared" si="28"/>
@@ -45392,16 +45364,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B339" s="13" t="s">
-        <v>2089</v>
+        <v>2087</v>
       </c>
       <c r="C339" s="13" t="s">
-        <v>2105</v>
+        <v>2103</v>
       </c>
       <c r="D339" s="13" t="s">
-        <v>2121</v>
+        <v>2119</v>
       </c>
       <c r="E339" s="13" t="s">
-        <v>2137</v>
+        <v>2135</v>
       </c>
       <c r="F339" s="16" t="str">
         <f t="shared" si="28"/>
@@ -45450,16 +45422,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B340" s="13" t="s">
-        <v>2088</v>
+        <v>2086</v>
       </c>
       <c r="C340" s="13" t="s">
-        <v>2104</v>
+        <v>2102</v>
       </c>
       <c r="D340" s="13" t="s">
-        <v>2120</v>
+        <v>2118</v>
       </c>
       <c r="E340" s="13" t="s">
-        <v>2136</v>
+        <v>2134</v>
       </c>
       <c r="F340" s="16" t="str">
         <f t="shared" si="28"/>
@@ -45505,16 +45477,16 @@
     <row r="341" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A341" s="4"/>
       <c r="B341" s="13" t="s">
-        <v>2087</v>
+        <v>2085</v>
       </c>
       <c r="C341" s="13" t="s">
-        <v>2103</v>
+        <v>2101</v>
       </c>
       <c r="D341" s="13" t="s">
-        <v>2119</v>
+        <v>2117</v>
       </c>
       <c r="E341" s="13" t="s">
-        <v>2135</v>
+        <v>2133</v>
       </c>
       <c r="F341" s="16" t="str">
         <f t="shared" si="28"/>
@@ -45560,16 +45532,16 @@
     <row r="342" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A342" s="4"/>
       <c r="B342" s="13" t="s">
-        <v>2086</v>
+        <v>2084</v>
       </c>
       <c r="C342" s="13" t="s">
-        <v>2102</v>
+        <v>2100</v>
       </c>
       <c r="D342" s="13" t="s">
-        <v>2118</v>
+        <v>2116</v>
       </c>
       <c r="E342" s="13" t="s">
-        <v>2134</v>
+        <v>2132</v>
       </c>
       <c r="F342" s="16" t="str">
         <f t="shared" si="28"/>
@@ -45618,16 +45590,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B343" s="13" t="s">
-        <v>2085</v>
+        <v>2083</v>
       </c>
       <c r="C343" s="13" t="s">
-        <v>2101</v>
+        <v>2099</v>
       </c>
       <c r="D343" s="13" t="s">
-        <v>2117</v>
+        <v>2115</v>
       </c>
       <c r="E343" s="13" t="s">
-        <v>2133</v>
+        <v>2131</v>
       </c>
       <c r="F343" s="16" t="str">
         <f t="shared" si="28"/>
@@ -45676,16 +45648,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B344" s="13" t="s">
-        <v>2084</v>
+        <v>2082</v>
       </c>
       <c r="C344" s="13" t="s">
-        <v>2100</v>
+        <v>2098</v>
       </c>
       <c r="D344" s="13" t="s">
-        <v>2116</v>
+        <v>2114</v>
       </c>
       <c r="E344" s="13" t="s">
-        <v>2132</v>
+        <v>2130</v>
       </c>
       <c r="F344" s="16" t="str">
         <f t="shared" si="28"/>
@@ -45734,16 +45706,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B345" s="13" t="s">
-        <v>2083</v>
+        <v>2081</v>
       </c>
       <c r="C345" s="13" t="s">
-        <v>2099</v>
+        <v>2097</v>
       </c>
       <c r="D345" s="13" t="s">
-        <v>2115</v>
+        <v>2113</v>
       </c>
       <c r="E345" s="13" t="s">
-        <v>2131</v>
+        <v>2129</v>
       </c>
       <c r="F345" s="16" t="str">
         <f t="shared" si="28"/>
@@ -45792,16 +45764,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B346" s="13" t="s">
-        <v>2082</v>
+        <v>2080</v>
       </c>
       <c r="C346" s="13" t="s">
-        <v>2098</v>
+        <v>2096</v>
       </c>
       <c r="D346" s="13" t="s">
-        <v>2114</v>
+        <v>2112</v>
       </c>
       <c r="E346" s="13" t="s">
-        <v>2130</v>
+        <v>2128</v>
       </c>
       <c r="F346" s="16" t="str">
         <f t="shared" si="28"/>
@@ -45850,16 +45822,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B347" s="13" t="s">
-        <v>2081</v>
+        <v>2079</v>
       </c>
       <c r="C347" s="13" t="s">
-        <v>2097</v>
+        <v>2095</v>
       </c>
       <c r="D347" s="13" t="s">
-        <v>2113</v>
+        <v>2111</v>
       </c>
       <c r="E347" s="13" t="s">
-        <v>2129</v>
+        <v>2127</v>
       </c>
       <c r="F347" s="16" t="str">
         <f t="shared" si="28"/>
@@ -45908,16 +45880,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B348" s="13" t="s">
-        <v>2080</v>
+        <v>2078</v>
       </c>
       <c r="C348" s="13" t="s">
-        <v>2096</v>
+        <v>2094</v>
       </c>
       <c r="D348" s="13" t="s">
-        <v>2112</v>
+        <v>2110</v>
       </c>
       <c r="E348" s="13" t="s">
-        <v>2128</v>
+        <v>2126</v>
       </c>
       <c r="F348" s="16" t="str">
         <f t="shared" ref="F348:I354" si="32">L348&amp;" ("&amp;$J348&amp;")"</f>
@@ -45966,16 +45938,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B349" s="13" t="s">
-        <v>2079</v>
+        <v>2077</v>
       </c>
       <c r="C349" s="13" t="s">
-        <v>2095</v>
+        <v>2093</v>
       </c>
       <c r="D349" s="13" t="s">
-        <v>2111</v>
+        <v>2109</v>
       </c>
       <c r="E349" s="13" t="s">
-        <v>2127</v>
+        <v>2125</v>
       </c>
       <c r="F349" s="16" t="str">
         <f t="shared" si="32"/>
@@ -46024,16 +45996,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B350" s="13" t="s">
-        <v>2078</v>
+        <v>2076</v>
       </c>
       <c r="C350" s="13" t="s">
-        <v>2094</v>
+        <v>2092</v>
       </c>
       <c r="D350" s="13" t="s">
-        <v>2110</v>
+        <v>2108</v>
       </c>
       <c r="E350" s="13" t="s">
-        <v>2126</v>
+        <v>2124</v>
       </c>
       <c r="F350" s="16" t="str">
         <f t="shared" si="32"/>
@@ -46082,16 +46054,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B351" s="13" t="s">
-        <v>2077</v>
+        <v>2075</v>
       </c>
       <c r="C351" s="13" t="s">
-        <v>2093</v>
+        <v>2091</v>
       </c>
       <c r="D351" s="13" t="s">
-        <v>2109</v>
+        <v>2107</v>
       </c>
       <c r="E351" s="13" t="s">
-        <v>2125</v>
+        <v>2123</v>
       </c>
       <c r="F351" s="16" t="str">
         <f t="shared" si="32"/>
@@ -46140,16 +46112,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B352" s="13" t="s">
-        <v>2076</v>
+        <v>2074</v>
       </c>
       <c r="C352" s="13" t="s">
-        <v>2092</v>
+        <v>2090</v>
       </c>
       <c r="D352" s="13" t="s">
-        <v>2108</v>
+        <v>2106</v>
       </c>
       <c r="E352" s="13" t="s">
-        <v>2124</v>
+        <v>2122</v>
       </c>
       <c r="F352" s="16" t="str">
         <f t="shared" si="32"/>
@@ -46198,16 +46170,16 @@
         <v>1.1.0</v>
       </c>
       <c r="B353" s="13" t="s">
-        <v>2075</v>
+        <v>2073</v>
       </c>
       <c r="C353" s="13" t="s">
-        <v>2091</v>
+        <v>2089</v>
       </c>
       <c r="D353" s="13" t="s">
-        <v>2107</v>
+        <v>2105</v>
       </c>
       <c r="E353" s="13" t="s">
-        <v>2123</v>
+        <v>2121</v>
       </c>
       <c r="F353" s="16" t="str">
         <f t="shared" si="32"/>
@@ -46256,16 +46228,16 @@
         <v>1.1.1</v>
       </c>
       <c r="B354" s="12" t="s">
-        <v>2189</v>
+        <v>2187</v>
       </c>
       <c r="C354" s="13" t="s">
-        <v>2188</v>
+        <v>2186</v>
       </c>
       <c r="D354" s="13" t="s">
-        <v>2187</v>
+        <v>2185</v>
       </c>
       <c r="E354" s="13" t="s">
-        <v>2186</v>
+        <v>2184</v>
       </c>
       <c r="F354" s="16" t="str">
         <f t="shared" si="32"/>
@@ -46314,16 +46286,16 @@
         <v>1.1.1</v>
       </c>
       <c r="B355" s="12" t="s">
-        <v>2237</v>
+        <v>2235</v>
       </c>
       <c r="C355" s="13" t="s">
-        <v>2236</v>
+        <v>2234</v>
       </c>
       <c r="D355" s="13" t="s">
-        <v>2235</v>
+        <v>2233</v>
       </c>
       <c r="E355" s="13" t="s">
-        <v>2234</v>
+        <v>2232</v>
       </c>
       <c r="F355" s="16" t="str">
         <f t="shared" ref="F355:F366" si="33">L355&amp;" ("&amp;$J355&amp;")"</f>
@@ -46372,16 +46344,16 @@
         <v>1.1.1</v>
       </c>
       <c r="B356" s="12" t="s">
-        <v>2233</v>
+        <v>2231</v>
       </c>
       <c r="C356" s="13" t="s">
-        <v>2232</v>
+        <v>2230</v>
       </c>
       <c r="D356" s="13" t="s">
-        <v>2231</v>
+        <v>2229</v>
       </c>
       <c r="E356" s="13" t="s">
-        <v>2230</v>
+        <v>2228</v>
       </c>
       <c r="F356" s="16" t="str">
         <f t="shared" si="33"/>
@@ -46430,16 +46402,16 @@
         <v>1.1.1</v>
       </c>
       <c r="B357" s="12" t="s">
-        <v>2229</v>
+        <v>2227</v>
       </c>
       <c r="C357" s="13" t="s">
-        <v>2228</v>
+        <v>2226</v>
       </c>
       <c r="D357" s="13" t="s">
-        <v>2227</v>
+        <v>2225</v>
       </c>
       <c r="E357" s="13" t="s">
-        <v>2226</v>
+        <v>2224</v>
       </c>
       <c r="F357" s="16" t="str">
         <f t="shared" si="33"/>
@@ -46488,16 +46460,16 @@
         <v>1.1.1</v>
       </c>
       <c r="B358" s="12" t="s">
-        <v>2225</v>
+        <v>2223</v>
       </c>
       <c r="C358" s="13" t="s">
-        <v>2224</v>
+        <v>2222</v>
       </c>
       <c r="D358" s="13" t="s">
-        <v>2223</v>
+        <v>2221</v>
       </c>
       <c r="E358" s="13" t="s">
-        <v>2222</v>
+        <v>2220</v>
       </c>
       <c r="F358" s="16" t="str">
         <f t="shared" si="33"/>
@@ -46546,16 +46518,16 @@
         <v>1.1.1</v>
       </c>
       <c r="B359" s="12" t="s">
-        <v>2221</v>
+        <v>2219</v>
       </c>
       <c r="C359" s="13" t="s">
-        <v>2220</v>
+        <v>2218</v>
       </c>
       <c r="D359" s="13" t="s">
-        <v>2219</v>
+        <v>2217</v>
       </c>
       <c r="E359" s="13" t="s">
-        <v>2218</v>
+        <v>2216</v>
       </c>
       <c r="F359" s="16" t="str">
         <f t="shared" si="33"/>
@@ -46604,16 +46576,16 @@
         <v>1.1.1</v>
       </c>
       <c r="B360" s="12" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
       <c r="C360" s="13" t="s">
-        <v>2216</v>
+        <v>2214</v>
       </c>
       <c r="D360" s="13" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
       <c r="E360" s="13" t="s">
-        <v>2214</v>
+        <v>2212</v>
       </c>
       <c r="F360" s="16" t="str">
         <f t="shared" si="33"/>
@@ -46662,16 +46634,16 @@
         <v>1.1.1</v>
       </c>
       <c r="B361" s="12" t="s">
-        <v>2213</v>
+        <v>2211</v>
       </c>
       <c r="C361" s="13" t="s">
-        <v>2212</v>
+        <v>2210</v>
       </c>
       <c r="D361" s="13" t="s">
-        <v>2211</v>
+        <v>2209</v>
       </c>
       <c r="E361" s="13" t="s">
-        <v>2210</v>
+        <v>2208</v>
       </c>
       <c r="F361" s="16" t="str">
         <f t="shared" si="33"/>
@@ -46720,16 +46692,16 @@
         <v>1.1.1</v>
       </c>
       <c r="B362" s="12" t="s">
-        <v>2209</v>
+        <v>2207</v>
       </c>
       <c r="C362" s="13" t="s">
-        <v>2208</v>
+        <v>2206</v>
       </c>
       <c r="D362" s="13" t="s">
-        <v>2207</v>
+        <v>2205</v>
       </c>
       <c r="E362" s="13" t="s">
-        <v>2206</v>
+        <v>2204</v>
       </c>
       <c r="F362" s="16" t="str">
         <f t="shared" si="33"/>
@@ -46778,16 +46750,16 @@
         <v>1.1.1</v>
       </c>
       <c r="B363" s="12" t="s">
-        <v>2205</v>
+        <v>2203</v>
       </c>
       <c r="C363" s="13" t="s">
-        <v>2204</v>
+        <v>2202</v>
       </c>
       <c r="D363" s="13" t="s">
-        <v>2203</v>
+        <v>2201</v>
       </c>
       <c r="E363" s="13" t="s">
-        <v>2202</v>
+        <v>2200</v>
       </c>
       <c r="F363" s="16" t="str">
         <f t="shared" si="33"/>
@@ -46836,16 +46808,16 @@
         <v>1.1.1</v>
       </c>
       <c r="B364" s="12" t="s">
-        <v>2201</v>
+        <v>2199</v>
       </c>
       <c r="C364" s="13" t="s">
-        <v>2200</v>
+        <v>2198</v>
       </c>
       <c r="D364" s="13" t="s">
-        <v>2199</v>
+        <v>2197</v>
       </c>
       <c r="E364" s="13" t="s">
-        <v>2198</v>
+        <v>2196</v>
       </c>
       <c r="F364" s="16" t="str">
         <f t="shared" si="33"/>
@@ -46894,16 +46866,16 @@
         <v>1.1.2</v>
       </c>
       <c r="B365" s="12" t="s">
-        <v>2197</v>
+        <v>2195</v>
       </c>
       <c r="C365" s="13" t="s">
-        <v>2196</v>
+        <v>2194</v>
       </c>
       <c r="D365" s="13" t="s">
-        <v>2195</v>
+        <v>2193</v>
       </c>
       <c r="E365" s="13" t="s">
-        <v>2194</v>
+        <v>2192</v>
       </c>
       <c r="F365" s="16" t="str">
         <f t="shared" si="33"/>
@@ -46952,16 +46924,16 @@
         <v>1.1.2</v>
       </c>
       <c r="B366" s="12" t="s">
-        <v>2193</v>
+        <v>2191</v>
       </c>
       <c r="C366" s="13" t="s">
-        <v>2192</v>
+        <v>2190</v>
       </c>
       <c r="D366" s="13" t="s">
-        <v>2191</v>
+        <v>2189</v>
       </c>
       <c r="E366" s="13" t="s">
-        <v>2190</v>
+        <v>2188</v>
       </c>
       <c r="F366" s="16" t="str">
         <f t="shared" si="33"/>
@@ -47010,16 +46982,16 @@
         <v>1.1.2</v>
       </c>
       <c r="B367" s="12" t="s">
-        <v>2269</v>
+        <v>2267</v>
       </c>
       <c r="C367" s="13" t="s">
-        <v>2268</v>
+        <v>2266</v>
       </c>
       <c r="D367" s="13" t="s">
-        <v>2267</v>
+        <v>2265</v>
       </c>
       <c r="E367" s="13" t="s">
-        <v>2266</v>
+        <v>2264</v>
       </c>
       <c r="F367" s="16" t="str">
         <f t="shared" ref="F367" si="37">L367&amp;" ("&amp;$J367&amp;")"</f>
@@ -47068,16 +47040,16 @@
         <v>1.1.2</v>
       </c>
       <c r="B368" s="12" t="s">
-        <v>2265</v>
+        <v>2263</v>
       </c>
       <c r="C368" s="13" t="s">
-        <v>2264</v>
+        <v>2262</v>
       </c>
       <c r="D368" s="13" t="s">
-        <v>2263</v>
+        <v>2261</v>
       </c>
       <c r="E368" s="13" t="s">
-        <v>2262</v>
+        <v>2260</v>
       </c>
       <c r="F368" s="16" t="str">
         <f t="shared" ref="F368:F374" si="41">L368&amp;" ("&amp;$J368&amp;")"</f>
@@ -47126,16 +47098,16 @@
         <v>1.1.2</v>
       </c>
       <c r="B369" s="12" t="s">
-        <v>2261</v>
+        <v>2259</v>
       </c>
       <c r="C369" s="13" t="s">
-        <v>2260</v>
+        <v>2258</v>
       </c>
       <c r="D369" s="13" t="s">
-        <v>2259</v>
+        <v>2257</v>
       </c>
       <c r="E369" s="13" t="s">
-        <v>2258</v>
+        <v>2256</v>
       </c>
       <c r="F369" s="16" t="str">
         <f t="shared" si="41"/>
@@ -47184,16 +47156,16 @@
         <v>1.1.2</v>
       </c>
       <c r="B370" s="12" t="s">
-        <v>2257</v>
+        <v>2255</v>
       </c>
       <c r="C370" s="13" t="s">
-        <v>2256</v>
+        <v>2254</v>
       </c>
       <c r="D370" s="13" t="s">
-        <v>2255</v>
+        <v>2253</v>
       </c>
       <c r="E370" s="13" t="s">
-        <v>2254</v>
+        <v>2252</v>
       </c>
       <c r="F370" s="16" t="str">
         <f t="shared" si="41"/>
@@ -47242,16 +47214,16 @@
         <v>1.1.2</v>
       </c>
       <c r="B371" s="12" t="s">
-        <v>2253</v>
+        <v>2251</v>
       </c>
       <c r="C371" s="13" t="s">
-        <v>2252</v>
+        <v>2250</v>
       </c>
       <c r="D371" s="13" t="s">
-        <v>2251</v>
+        <v>2249</v>
       </c>
       <c r="E371" s="13" t="s">
-        <v>2250</v>
+        <v>2248</v>
       </c>
       <c r="F371" s="16" t="str">
         <f t="shared" si="41"/>
@@ -47300,16 +47272,16 @@
         <v>1.1.2</v>
       </c>
       <c r="B372" s="12" t="s">
-        <v>2249</v>
+        <v>2247</v>
       </c>
       <c r="C372" s="13" t="s">
-        <v>2248</v>
+        <v>2246</v>
       </c>
       <c r="D372" s="13" t="s">
-        <v>2247</v>
+        <v>2245</v>
       </c>
       <c r="E372" s="13" t="s">
-        <v>2246</v>
+        <v>2244</v>
       </c>
       <c r="F372" s="16" t="str">
         <f t="shared" si="41"/>
@@ -47358,16 +47330,16 @@
         <v>1.1.2</v>
       </c>
       <c r="B373" s="12" t="s">
-        <v>2245</v>
+        <v>2243</v>
       </c>
       <c r="C373" s="13" t="s">
-        <v>2244</v>
+        <v>2242</v>
       </c>
       <c r="D373" s="13" t="s">
-        <v>2243</v>
+        <v>2241</v>
       </c>
       <c r="E373" s="13" t="s">
-        <v>2242</v>
+        <v>2240</v>
       </c>
       <c r="F373" s="16" t="str">
         <f t="shared" si="41"/>
@@ -47416,16 +47388,16 @@
         <v>1.1.2</v>
       </c>
       <c r="B374" s="12" t="s">
-        <v>2241</v>
+        <v>2239</v>
       </c>
       <c r="C374" s="13" t="s">
-        <v>2240</v>
+        <v>2238</v>
       </c>
       <c r="D374" s="13" t="s">
-        <v>2239</v>
+        <v>2237</v>
       </c>
       <c r="E374" s="13" t="s">
-        <v>2238</v>
+        <v>2236</v>
       </c>
       <c r="F374" s="16" t="str">
         <f t="shared" si="41"/>
@@ -47474,16 +47446,16 @@
         <v>1.1.2</v>
       </c>
       <c r="B375" s="13" t="s">
-        <v>2330</v>
+        <v>2328</v>
       </c>
       <c r="C375" s="13" t="s">
-        <v>2329</v>
+        <v>2327</v>
       </c>
       <c r="D375" s="13" t="s">
-        <v>2328</v>
+        <v>2326</v>
       </c>
       <c r="E375" s="13" t="s">
-        <v>2327</v>
+        <v>2325</v>
       </c>
       <c r="F375" s="16" t="str">
         <f t="shared" ref="F375:F390" si="45">L375&amp;" ("&amp;$J375&amp;")"</f>
@@ -47532,16 +47504,16 @@
         <v>1.1.2</v>
       </c>
       <c r="B376" s="13" t="s">
-        <v>2326</v>
+        <v>2324</v>
       </c>
       <c r="C376" s="13" t="s">
-        <v>2325</v>
+        <v>2323</v>
       </c>
       <c r="D376" s="13" t="s">
-        <v>2324</v>
+        <v>2322</v>
       </c>
       <c r="E376" s="13" t="s">
-        <v>2323</v>
+        <v>2321</v>
       </c>
       <c r="F376" s="16" t="str">
         <f t="shared" si="45"/>
@@ -47590,16 +47562,16 @@
         <v>1.1.2</v>
       </c>
       <c r="B377" s="13" t="s">
-        <v>2322</v>
+        <v>2320</v>
       </c>
       <c r="C377" s="13" t="s">
-        <v>2321</v>
+        <v>2319</v>
       </c>
       <c r="D377" s="13" t="s">
-        <v>2320</v>
+        <v>2318</v>
       </c>
       <c r="E377" s="13" t="s">
-        <v>2319</v>
+        <v>2317</v>
       </c>
       <c r="F377" s="16" t="str">
         <f t="shared" si="45"/>
@@ -47648,16 +47620,16 @@
         <v>1.1.2</v>
       </c>
       <c r="B378" s="13" t="s">
-        <v>2318</v>
+        <v>2316</v>
       </c>
       <c r="C378" s="13" t="s">
-        <v>2317</v>
+        <v>2315</v>
       </c>
       <c r="D378" s="13" t="s">
-        <v>2316</v>
+        <v>2314</v>
       </c>
       <c r="E378" s="13" t="s">
-        <v>2315</v>
+        <v>2313</v>
       </c>
       <c r="F378" s="16" t="str">
         <f t="shared" si="45"/>
@@ -47706,16 +47678,16 @@
         <v>1.1.2</v>
       </c>
       <c r="B379" s="13" t="s">
-        <v>2314</v>
+        <v>2312</v>
       </c>
       <c r="C379" s="13" t="s">
-        <v>2313</v>
+        <v>2311</v>
       </c>
       <c r="D379" s="13" t="s">
-        <v>2312</v>
+        <v>2310</v>
       </c>
       <c r="E379" s="13" t="s">
-        <v>2311</v>
+        <v>2309</v>
       </c>
       <c r="F379" s="16" t="str">
         <f t="shared" si="45"/>
@@ -47764,16 +47736,16 @@
         <v>1.1.2</v>
       </c>
       <c r="B380" s="13" t="s">
-        <v>2310</v>
+        <v>2308</v>
       </c>
       <c r="C380" s="13" t="s">
-        <v>2309</v>
+        <v>2307</v>
       </c>
       <c r="D380" s="13" t="s">
-        <v>2308</v>
+        <v>2306</v>
       </c>
       <c r="E380" s="13" t="s">
-        <v>2307</v>
+        <v>2305</v>
       </c>
       <c r="F380" s="16" t="str">
         <f t="shared" si="45"/>
@@ -47818,16 +47790,16 @@
     </row>
     <row r="381" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B381" s="13" t="s">
-        <v>2306</v>
+        <v>2304</v>
       </c>
       <c r="C381" s="13" t="s">
-        <v>2305</v>
+        <v>2303</v>
       </c>
       <c r="D381" s="13" t="s">
-        <v>2304</v>
+        <v>2302</v>
       </c>
       <c r="E381" s="13" t="s">
-        <v>2303</v>
+        <v>2301</v>
       </c>
       <c r="F381" s="16" t="str">
         <f t="shared" si="45"/>
@@ -47872,16 +47844,16 @@
     </row>
     <row r="382" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B382" s="13" t="s">
-        <v>2302</v>
+        <v>2300</v>
       </c>
       <c r="C382" s="13" t="s">
-        <v>2301</v>
+        <v>2299</v>
       </c>
       <c r="D382" s="13" t="s">
-        <v>2300</v>
+        <v>2298</v>
       </c>
       <c r="E382" s="13" t="s">
-        <v>2299</v>
+        <v>2297</v>
       </c>
       <c r="F382" s="16" t="str">
         <f t="shared" si="45"/>
@@ -47926,16 +47898,16 @@
     </row>
     <row r="383" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B383" s="13" t="s">
-        <v>2298</v>
+        <v>2296</v>
       </c>
       <c r="C383" s="13" t="s">
-        <v>2297</v>
+        <v>2295</v>
       </c>
       <c r="D383" s="13" t="s">
-        <v>2296</v>
+        <v>2294</v>
       </c>
       <c r="E383" s="13" t="s">
-        <v>2295</v>
+        <v>2293</v>
       </c>
       <c r="F383" s="16" t="str">
         <f t="shared" si="45"/>
@@ -47980,16 +47952,16 @@
     </row>
     <row r="384" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B384" s="13" t="s">
-        <v>2294</v>
+        <v>2292</v>
       </c>
       <c r="C384" s="13" t="s">
-        <v>2293</v>
+        <v>2291</v>
       </c>
       <c r="D384" s="13" t="s">
-        <v>2292</v>
+        <v>2290</v>
       </c>
       <c r="E384" s="13" t="s">
-        <v>2291</v>
+        <v>2289</v>
       </c>
       <c r="F384" s="16" t="str">
         <f t="shared" si="45"/>
@@ -48034,16 +48006,16 @@
     </row>
     <row r="385" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B385" s="13" t="s">
-        <v>2290</v>
+        <v>2288</v>
       </c>
       <c r="C385" s="13" t="s">
-        <v>2289</v>
+        <v>2287</v>
       </c>
       <c r="D385" s="13" t="s">
-        <v>2288</v>
+        <v>2286</v>
       </c>
       <c r="E385" s="13" t="s">
-        <v>2287</v>
+        <v>2285</v>
       </c>
       <c r="F385" s="16" t="str">
         <f t="shared" si="45"/>
@@ -48088,16 +48060,16 @@
     </row>
     <row r="386" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B386" s="13" t="s">
-        <v>2286</v>
+        <v>2284</v>
       </c>
       <c r="C386" s="13" t="s">
-        <v>2285</v>
+        <v>2283</v>
       </c>
       <c r="D386" s="13" t="s">
-        <v>2284</v>
+        <v>2282</v>
       </c>
       <c r="E386" s="13" t="s">
-        <v>2283</v>
+        <v>2281</v>
       </c>
       <c r="F386" s="16" t="str">
         <f t="shared" si="45"/>
@@ -48142,16 +48114,16 @@
     </row>
     <row r="387" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B387" s="13" t="s">
-        <v>2282</v>
+        <v>2280</v>
       </c>
       <c r="C387" s="13" t="s">
-        <v>2281</v>
+        <v>2279</v>
       </c>
       <c r="D387" s="13" t="s">
-        <v>2280</v>
+        <v>2278</v>
       </c>
       <c r="E387" s="13" t="s">
-        <v>2279</v>
+        <v>2277</v>
       </c>
       <c r="F387" s="16" t="str">
         <f t="shared" si="45"/>
@@ -48196,16 +48168,16 @@
     </row>
     <row r="388" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B388" s="13" t="s">
-        <v>2278</v>
+        <v>2276</v>
       </c>
       <c r="C388" s="13" t="s">
-        <v>2277</v>
+        <v>2275</v>
       </c>
       <c r="D388" s="13" t="s">
-        <v>2276</v>
+        <v>2274</v>
       </c>
       <c r="E388" s="13" t="s">
-        <v>2275</v>
+        <v>2273</v>
       </c>
       <c r="F388" s="16" t="str">
         <f t="shared" si="45"/>
@@ -48250,16 +48222,16 @@
     </row>
     <row r="389" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B389" s="13" t="s">
-        <v>2274</v>
+        <v>2272</v>
       </c>
       <c r="C389" s="13" t="s">
-        <v>2273</v>
+        <v>2271</v>
       </c>
       <c r="D389" s="13" t="s">
-        <v>2272</v>
+        <v>2270</v>
       </c>
       <c r="E389" s="13" t="s">
-        <v>2271</v>
+        <v>2269</v>
       </c>
       <c r="F389" s="16" t="str">
         <f t="shared" si="45"/>

</xml_diff>

<commit_message>
Update to 1.1.13 with new JAR. Updated ores and added flipped versions. Added test vessels.
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="67725" yWindow="495" windowWidth="19200" windowHeight="19455" tabRatio="877"/>
+    <workbookView xWindow="67725" yWindow="495" windowWidth="19200" windowHeight="19455" tabRatio="877" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Custom Objects" sheetId="41" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2371" uniqueCount="2336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2373" uniqueCount="2338">
   <si>
     <t>Ore</t>
   </si>
@@ -7045,6 +7045,12 @@
   </si>
   <si>
     <t>19P</t>
+  </si>
+  <si>
+    <t>19S</t>
+  </si>
+  <si>
+    <t>19T</t>
   </si>
 </sst>
 </file>
@@ -7550,6 +7556,9 @@
           <cell r="A30" t="str">
             <v>Drum</v>
           </cell>
+          <cell r="B30" t="str">
+            <v>Liquid</v>
+          </cell>
         </row>
         <row r="31">
           <cell r="A31" t="str">
@@ -8973,6 +8982,11 @@
             <v>Potash</v>
           </cell>
         </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>Fluorite</v>
+          </cell>
+        </row>
       </sheetData>
       <sheetData sheetId="6">
         <row r="1">
@@ -11739,7 +11753,7 @@
             <v>NaOH</v>
           </cell>
           <cell r="D260" t="str">
-            <v>Liquid</v>
+            <v>Solid</v>
           </cell>
         </row>
         <row r="261">
@@ -12952,6 +12966,33 @@
             <v>Cyclopentadiene</v>
           </cell>
           <cell r="D388" t="str">
+            <v>Liquid</v>
+          </cell>
+        </row>
+        <row r="389">
+          <cell r="B389" t="str">
+            <v>Nitrogen Dioxide</v>
+          </cell>
+          <cell r="D389" t="str">
+            <v>Gas</v>
+          </cell>
+        </row>
+        <row r="390">
+          <cell r="B390" t="str">
+            <v>Sodium Nitrite</v>
+          </cell>
+          <cell r="C390" t="str">
+            <v>NaNO2</v>
+          </cell>
+          <cell r="D390" t="str">
+            <v>Solid</v>
+          </cell>
+        </row>
+        <row r="391">
+          <cell r="B391" t="str">
+            <v>Dicyclopentadiene</v>
+          </cell>
+          <cell r="D391" t="str">
             <v>Liquid</v>
           </cell>
         </row>
@@ -13255,8 +13296,8 @@
   </sheetPr>
   <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14774,7 +14815,9 @@
         <f>[1]Enums!$A$37</f>
         <v>Armor</v>
       </c>
-      <c r="E53" s="32"/>
+      <c r="E53" s="32">
+        <v>8</v>
+      </c>
       <c r="F53" s="26" t="b">
         <v>1</v>
       </c>
@@ -14815,7 +14858,9 @@
         <f>[1]Enums!$A$37</f>
         <v>Armor</v>
       </c>
-      <c r="E54" s="32"/>
+      <c r="E54" s="32">
+        <v>8</v>
+      </c>
       <c r="F54" s="26" t="b">
         <v>1</v>
       </c>
@@ -14856,7 +14901,9 @@
         <f>[1]Enums!$A$37</f>
         <v>Armor</v>
       </c>
-      <c r="E55" s="32"/>
+      <c r="E55" s="32">
+        <v>8</v>
+      </c>
       <c r="F55" s="26" t="b">
         <v>1</v>
       </c>
@@ -15133,8 +15180,8 @@
   </sheetPr>
   <dimension ref="A1:R120"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16439,15 +16486,49 @@
       </c>
     </row>
     <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
+      <c r="A25" s="4" t="str">
+        <f>[1]Enums!$A$14</f>
+        <v>1.1.2</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>2336</v>
+      </c>
+      <c r="C25" t="str">
+        <f xml:space="preserve"> E25&amp;" "&amp;$C$1</f>
+        <v>Fluorite Ore</v>
+      </c>
+      <c r="D25" s="8" t="str">
+        <f>[1]Minerals!B$1</f>
+        <v>Mineral</v>
+      </c>
+      <c r="E25" s="3" t="str">
+        <f>[1]Minerals!B10</f>
+        <v>Fluorite</v>
+      </c>
+      <c r="F25" s="3">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1">
+        <v>5</v>
+      </c>
+      <c r="H25" s="1">
+        <v>2</v>
+      </c>
+      <c r="I25" s="1">
+        <v>5</v>
+      </c>
+      <c r="J25" s="1">
+        <v>2</v>
+      </c>
+      <c r="K25" s="8">
+        <v>6</v>
+      </c>
+      <c r="L25" s="1">
+        <v>40</v>
+      </c>
+      <c r="M25" s="1">
+        <v>60</v>
+      </c>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D26" s="3"/>
@@ -16940,7 +17021,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17565,10 +17646,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18163,6 +18244,27 @@
         <v>Antimony-Lead Ingot</v>
       </c>
     </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="str">
+        <f>[1]Enums!$A$14</f>
+        <v>1.1.2</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>2337</v>
+      </c>
+      <c r="C28" t="str">
+        <f>"Block of "&amp;Ores!E25</f>
+        <v>Block of Fluorite</v>
+      </c>
+      <c r="D28" t="str">
+        <f>Ores!$C$1</f>
+        <v>Ore</v>
+      </c>
+      <c r="E28" t="str">
+        <f>Ores!$C$25</f>
+        <v>Fluorite Ore</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18176,7 +18278,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18872,15 +18974,15 @@
       </c>
       <c r="C35" t="str">
         <f>E35&amp;" "&amp;$C$1</f>
-        <v>Osmium Catalyst</v>
+        <v>Iridium Catalyst</v>
       </c>
       <c r="D35" t="str">
         <f>[1]Elements!$B$1</f>
         <v>Element</v>
       </c>
       <c r="E35" t="str">
-        <f>[1]Elements!$B$77</f>
-        <v>Osmium</v>
+        <f>[1]Elements!$B$78</f>
+        <v>Iridium</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -18937,8 +19039,8 @@
   </sheetPr>
   <dimension ref="A1:P119"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19059,7 +19161,7 @@
         <v>Cartridge</v>
       </c>
       <c r="O2" s="20" t="str">
-        <f>IF(L2=[1]Enums!$A$20, [1]Enums!$A$31, IF(N2=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L2=[1]Enums!$A$20, [1]Enums!$A$31, IF(L2=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Canister</v>
       </c>
       <c r="P2" s="20" t="str">
@@ -19120,8 +19222,8 @@
         <f>IF(L3=[1]Enums!$A$20, [1]Enums!$A$28, IF(L3=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Cartridge</v>
       </c>
-      <c r="O3" s="24" t="str">
-        <f>IF(L3=[1]Enums!$A$20, [1]Enums!$A$31, IF(N3=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O3" s="20" t="str">
+        <f>IF(L3=[1]Enums!$A$20, [1]Enums!$A$31, IF(L3=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Canister</v>
       </c>
       <c r="P3" s="24" t="str">
@@ -19183,7 +19285,7 @@
         <v>Sack</v>
       </c>
       <c r="O4" s="20" t="str">
-        <f>IF(L4=[1]Enums!$A$20, [1]Enums!$A$31, IF(N4=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L4=[1]Enums!$A$20, [1]Enums!$A$31, IF(L4=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P4" s="20" t="str">
@@ -19245,7 +19347,7 @@
         <v>Sack</v>
       </c>
       <c r="O5" s="20" t="str">
-        <f>IF(L5=[1]Enums!$A$20, [1]Enums!$A$31, IF(N5=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L5=[1]Enums!$A$20, [1]Enums!$A$31, IF(L5=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P5" s="20" t="str">
@@ -19307,7 +19409,7 @@
         <v>Sack</v>
       </c>
       <c r="O6" s="20" t="str">
-        <f>IF(L6=[1]Enums!$A$20, [1]Enums!$A$31, IF(N6=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L6=[1]Enums!$A$20, [1]Enums!$A$31, IF(L6=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P6" s="20" t="str">
@@ -19369,7 +19471,7 @@
         <v>Sack</v>
       </c>
       <c r="O7" s="20" t="str">
-        <f>IF(L7=[1]Enums!$A$20, [1]Enums!$A$31, IF(N7=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L7=[1]Enums!$A$20, [1]Enums!$A$31, IF(L7=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P7" s="20" t="str">
@@ -19431,7 +19533,7 @@
         <v>Cartridge</v>
       </c>
       <c r="O8" s="20" t="str">
-        <f>IF(L8=[1]Enums!$A$20, [1]Enums!$A$31, IF(N8=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L8=[1]Enums!$A$20, [1]Enums!$A$31, IF(L8=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Canister</v>
       </c>
       <c r="P8" s="20" t="str">
@@ -19493,7 +19595,7 @@
         <v>Cartridge</v>
       </c>
       <c r="O9" s="20" t="str">
-        <f>IF(L9=[1]Enums!$A$20, [1]Enums!$A$31, IF(N9=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L9=[1]Enums!$A$20, [1]Enums!$A$31, IF(L9=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Canister</v>
       </c>
       <c r="P9" s="20" t="str">
@@ -19555,7 +19657,7 @@
         <v>Cartridge</v>
       </c>
       <c r="O10" s="20" t="str">
-        <f>IF(L10=[1]Enums!$A$20, [1]Enums!$A$31, IF(N10=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L10=[1]Enums!$A$20, [1]Enums!$A$31, IF(L10=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Canister</v>
       </c>
       <c r="P10" s="20" t="str">
@@ -19616,8 +19718,8 @@
         <f>IF(L11=[1]Enums!$A$20, [1]Enums!$A$28, IF(L11=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Cartridge</v>
       </c>
-      <c r="O11" s="24" t="str">
-        <f>IF(L11=[1]Enums!$A$20, [1]Enums!$A$31, IF(N11=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O11" s="20" t="str">
+        <f>IF(L11=[1]Enums!$A$20, [1]Enums!$A$31, IF(L11=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Canister</v>
       </c>
       <c r="P11" s="24" t="str">
@@ -19679,7 +19781,7 @@
         <v>Sack</v>
       </c>
       <c r="O12" s="20" t="str">
-        <f>IF(L12=[1]Enums!$A$20, [1]Enums!$A$31, IF(N12=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L12=[1]Enums!$A$20, [1]Enums!$A$31, IF(L12=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P12" s="20" t="str">
@@ -19741,7 +19843,7 @@
         <v>Sack</v>
       </c>
       <c r="O13" s="20" t="str">
-        <f>IF(L13=[1]Enums!$A$20, [1]Enums!$A$31, IF(N13=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L13=[1]Enums!$A$20, [1]Enums!$A$31, IF(L13=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P13" s="20" t="str">
@@ -19803,7 +19905,7 @@
         <v>Sack</v>
       </c>
       <c r="O14" s="20" t="str">
-        <f>IF(L14=[1]Enums!$A$20, [1]Enums!$A$31, IF(N14=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L14=[1]Enums!$A$20, [1]Enums!$A$31, IF(L14=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P14" s="20" t="str">
@@ -19865,7 +19967,7 @@
         <v>Sack</v>
       </c>
       <c r="O15" s="20" t="str">
-        <f>IF(L15=[1]Enums!$A$20, [1]Enums!$A$31, IF(N15=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L15=[1]Enums!$A$20, [1]Enums!$A$31, IF(L15=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P15" s="20" t="str">
@@ -19927,7 +20029,7 @@
         <v>Sack</v>
       </c>
       <c r="O16" s="20" t="str">
-        <f>IF(L16=[1]Enums!$A$20, [1]Enums!$A$31, IF(N16=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L16=[1]Enums!$A$20, [1]Enums!$A$31, IF(L16=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P16" s="20" t="str">
@@ -19989,7 +20091,7 @@
         <v>Sack</v>
       </c>
       <c r="O17" s="20" t="str">
-        <f>IF(L17=[1]Enums!$A$20, [1]Enums!$A$31, IF(N17=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L17=[1]Enums!$A$20, [1]Enums!$A$31, IF(L17=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P17" s="20" t="str">
@@ -20051,7 +20153,7 @@
         <v>Cartridge</v>
       </c>
       <c r="O18" s="20" t="str">
-        <f>IF(L18=[1]Enums!$A$20, [1]Enums!$A$31, IF(N18=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L18=[1]Enums!$A$20, [1]Enums!$A$31, IF(L18=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Canister</v>
       </c>
       <c r="P18" s="20" t="str">
@@ -20112,8 +20214,8 @@
         <f>IF(L19=[1]Enums!$A$20, [1]Enums!$A$28, IF(L19=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Cartridge</v>
       </c>
-      <c r="O19" s="24" t="str">
-        <f>IF(L19=[1]Enums!$A$20, [1]Enums!$A$31, IF(N19=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O19" s="20" t="str">
+        <f>IF(L19=[1]Enums!$A$20, [1]Enums!$A$31, IF(L19=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Canister</v>
       </c>
       <c r="P19" s="24" t="str">
@@ -20175,7 +20277,7 @@
         <v>Sack</v>
       </c>
       <c r="O20" s="20" t="str">
-        <f>IF(L20=[1]Enums!$A$20, [1]Enums!$A$31, IF(N20=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L20=[1]Enums!$A$20, [1]Enums!$A$31, IF(L20=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P20" s="20" t="str">
@@ -20237,7 +20339,7 @@
         <v>Sack</v>
       </c>
       <c r="O21" s="20" t="str">
-        <f>IF(L21=[1]Enums!$A$20, [1]Enums!$A$31, IF(N21=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L21=[1]Enums!$A$20, [1]Enums!$A$31, IF(L21=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P21" s="20" t="str">
@@ -20299,7 +20401,7 @@
         <v>Sack</v>
       </c>
       <c r="O22" s="20" t="str">
-        <f>IF(L22=[1]Enums!$A$20, [1]Enums!$A$31, IF(N22=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L22=[1]Enums!$A$20, [1]Enums!$A$31, IF(L22=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P22" s="20" t="str">
@@ -20361,7 +20463,7 @@
         <v>Sack</v>
       </c>
       <c r="O23" s="20" t="str">
-        <f>IF(L23=[1]Enums!$A$20, [1]Enums!$A$31, IF(N23=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L23=[1]Enums!$A$20, [1]Enums!$A$31, IF(L23=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P23" s="20" t="str">
@@ -20423,7 +20525,7 @@
         <v>Sack</v>
       </c>
       <c r="O24" s="20" t="str">
-        <f>IF(L24=[1]Enums!$A$20, [1]Enums!$A$31, IF(N24=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L24=[1]Enums!$A$20, [1]Enums!$A$31, IF(L24=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P24" s="20" t="str">
@@ -20485,7 +20587,7 @@
         <v>Sack</v>
       </c>
       <c r="O25" s="20" t="str">
-        <f>IF(L25=[1]Enums!$A$20, [1]Enums!$A$31, IF(N25=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L25=[1]Enums!$A$20, [1]Enums!$A$31, IF(L25=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P25" s="20" t="str">
@@ -20547,7 +20649,7 @@
         <v>Sack</v>
       </c>
       <c r="O26" s="20" t="str">
-        <f>IF(L26=[1]Enums!$A$20, [1]Enums!$A$31, IF(N26=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L26=[1]Enums!$A$20, [1]Enums!$A$31, IF(L26=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P26" s="20" t="str">
@@ -20609,7 +20711,7 @@
         <v>Sack</v>
       </c>
       <c r="O27" s="20" t="str">
-        <f>IF(L27=[1]Enums!$A$20, [1]Enums!$A$31, IF(N27=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L27=[1]Enums!$A$20, [1]Enums!$A$31, IF(L27=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P27" s="20" t="str">
@@ -20671,7 +20773,7 @@
         <v>Sack</v>
       </c>
       <c r="O28" s="20" t="str">
-        <f>IF(L28=[1]Enums!$A$20, [1]Enums!$A$31, IF(N28=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L28=[1]Enums!$A$20, [1]Enums!$A$31, IF(L28=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P28" s="20" t="str">
@@ -20733,7 +20835,7 @@
         <v>Sack</v>
       </c>
       <c r="O29" s="20" t="str">
-        <f>IF(L29=[1]Enums!$A$20, [1]Enums!$A$31, IF(N29=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L29=[1]Enums!$A$20, [1]Enums!$A$31, IF(L29=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P29" s="20" t="str">
@@ -20795,7 +20897,7 @@
         <v>Sack</v>
       </c>
       <c r="O30" s="20" t="str">
-        <f>IF(L30=[1]Enums!$A$20, [1]Enums!$A$31, IF(N30=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L30=[1]Enums!$A$20, [1]Enums!$A$31, IF(L30=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P30" s="20" t="str">
@@ -20857,7 +20959,7 @@
         <v>Sack</v>
       </c>
       <c r="O31" s="20" t="str">
-        <f>IF(L31=[1]Enums!$A$20, [1]Enums!$A$31, IF(N31=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L31=[1]Enums!$A$20, [1]Enums!$A$31, IF(L31=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P31" s="20" t="str">
@@ -20919,7 +21021,7 @@
         <v>Sack</v>
       </c>
       <c r="O32" s="20" t="str">
-        <f>IF(L32=[1]Enums!$A$20, [1]Enums!$A$31, IF(N32=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L32=[1]Enums!$A$20, [1]Enums!$A$31, IF(L32=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P32" s="20" t="str">
@@ -20981,7 +21083,7 @@
         <v>Sack</v>
       </c>
       <c r="O33" s="20" t="str">
-        <f>IF(L33=[1]Enums!$A$20, [1]Enums!$A$31, IF(N33=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L33=[1]Enums!$A$20, [1]Enums!$A$31, IF(L33=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P33" s="20" t="str">
@@ -21043,7 +21145,7 @@
         <v>Sack</v>
       </c>
       <c r="O34" s="20" t="str">
-        <f>IF(L34=[1]Enums!$A$20, [1]Enums!$A$31, IF(N34=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L34=[1]Enums!$A$20, [1]Enums!$A$31, IF(L34=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P34" s="20" t="str">
@@ -21105,7 +21207,7 @@
         <v>Sack</v>
       </c>
       <c r="O35" s="20" t="str">
-        <f>IF(L35=[1]Enums!$A$20, [1]Enums!$A$31, IF(N35=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L35=[1]Enums!$A$20, [1]Enums!$A$31, IF(L35=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P35" s="20" t="str">
@@ -21140,7 +21242,7 @@
       </c>
       <c r="H36" s="16" t="str">
         <f t="shared" si="6"/>
-        <v>Powder Keg (Bromine)</v>
+        <v>Drum (Bromine)</v>
       </c>
       <c r="I36" s="16" t="str">
         <f t="shared" si="7"/>
@@ -21167,8 +21269,8 @@
         <v>Beaker</v>
       </c>
       <c r="O36" s="20" t="str">
-        <f>IF(L36=[1]Enums!$A$20, [1]Enums!$A$31, IF(N36=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
-        <v>Powder Keg</v>
+        <f>IF(L36=[1]Enums!$A$20, [1]Enums!$A$31, IF(L36=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <v>Drum</v>
       </c>
       <c r="P36" s="20" t="str">
         <f>IF(L36=[1]Enums!$A$20, [1]Enums!$A$34, IF(L36=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
@@ -21228,8 +21330,8 @@
         <f>IF(L37=[1]Enums!$A$20, [1]Enums!$A$28, IF(L37=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Cartridge</v>
       </c>
-      <c r="O37" s="24" t="str">
-        <f>IF(L37=[1]Enums!$A$20, [1]Enums!$A$31, IF(N37=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O37" s="20" t="str">
+        <f>IF(L37=[1]Enums!$A$20, [1]Enums!$A$31, IF(L37=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Canister</v>
       </c>
       <c r="P37" s="24" t="str">
@@ -21291,7 +21393,7 @@
         <v>Sack</v>
       </c>
       <c r="O38" s="20" t="str">
-        <f>IF(L38=[1]Enums!$A$20, [1]Enums!$A$31, IF(N38=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L38=[1]Enums!$A$20, [1]Enums!$A$31, IF(L38=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P38" s="20" t="str">
@@ -21353,7 +21455,7 @@
         <v>Sack</v>
       </c>
       <c r="O39" s="20" t="str">
-        <f>IF(L39=[1]Enums!$A$20, [1]Enums!$A$31, IF(N39=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L39=[1]Enums!$A$20, [1]Enums!$A$31, IF(L39=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P39" s="20" t="str">
@@ -21415,7 +21517,7 @@
         <v>Sack</v>
       </c>
       <c r="O40" s="20" t="str">
-        <f>IF(L40=[1]Enums!$A$20, [1]Enums!$A$31, IF(N40=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L40=[1]Enums!$A$20, [1]Enums!$A$31, IF(L40=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P40" s="20" t="str">
@@ -21477,7 +21579,7 @@
         <v>Sack</v>
       </c>
       <c r="O41" s="20" t="str">
-        <f>IF(L41=[1]Enums!$A$20, [1]Enums!$A$31, IF(N41=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L41=[1]Enums!$A$20, [1]Enums!$A$31, IF(L41=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P41" s="20" t="str">
@@ -21539,7 +21641,7 @@
         <v>Sack</v>
       </c>
       <c r="O42" s="20" t="str">
-        <f>IF(L42=[1]Enums!$A$20, [1]Enums!$A$31, IF(N42=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L42=[1]Enums!$A$20, [1]Enums!$A$31, IF(L42=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P42" s="20" t="str">
@@ -21601,7 +21703,7 @@
         <v>Sack</v>
       </c>
       <c r="O43" s="20" t="str">
-        <f>IF(L43=[1]Enums!$A$20, [1]Enums!$A$31, IF(N43=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L43=[1]Enums!$A$20, [1]Enums!$A$31, IF(L43=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P43" s="20" t="str">
@@ -21663,7 +21765,7 @@
         <v>Sack</v>
       </c>
       <c r="O44" s="20" t="str">
-        <f>IF(L44=[1]Enums!$A$20, [1]Enums!$A$31, IF(N44=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L44=[1]Enums!$A$20, [1]Enums!$A$31, IF(L44=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P44" s="20" t="str">
@@ -21725,7 +21827,7 @@
         <v>Sack</v>
       </c>
       <c r="O45" s="20" t="str">
-        <f>IF(L45=[1]Enums!$A$20, [1]Enums!$A$31, IF(N45=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L45=[1]Enums!$A$20, [1]Enums!$A$31, IF(L45=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P45" s="20" t="str">
@@ -21787,7 +21889,7 @@
         <v>Sack</v>
       </c>
       <c r="O46" s="20" t="str">
-        <f>IF(L46=[1]Enums!$A$20, [1]Enums!$A$31, IF(N46=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L46=[1]Enums!$A$20, [1]Enums!$A$31, IF(L46=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P46" s="20" t="str">
@@ -21849,7 +21951,7 @@
         <v>Sack</v>
       </c>
       <c r="O47" s="20" t="str">
-        <f>IF(L47=[1]Enums!$A$20, [1]Enums!$A$31, IF(N47=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L47=[1]Enums!$A$20, [1]Enums!$A$31, IF(L47=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P47" s="20" t="str">
@@ -21911,7 +22013,7 @@
         <v>Sack</v>
       </c>
       <c r="O48" s="20" t="str">
-        <f>IF(L48=[1]Enums!$A$20, [1]Enums!$A$31, IF(N48=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L48=[1]Enums!$A$20, [1]Enums!$A$31, IF(L48=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P48" s="20" t="str">
@@ -21973,7 +22075,7 @@
         <v>Sack</v>
       </c>
       <c r="O49" s="20" t="str">
-        <f>IF(L49=[1]Enums!$A$20, [1]Enums!$A$31, IF(N49=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L49=[1]Enums!$A$20, [1]Enums!$A$31, IF(L49=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P49" s="20" t="str">
@@ -22035,7 +22137,7 @@
         <v>Sack</v>
       </c>
       <c r="O50" s="20" t="str">
-        <f>IF(L50=[1]Enums!$A$20, [1]Enums!$A$31, IF(N50=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L50=[1]Enums!$A$20, [1]Enums!$A$31, IF(L50=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P50" s="20" t="str">
@@ -22097,7 +22199,7 @@
         <v>Sack</v>
       </c>
       <c r="O51" s="20" t="str">
-        <f>IF(L51=[1]Enums!$A$20, [1]Enums!$A$31, IF(N51=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L51=[1]Enums!$A$20, [1]Enums!$A$31, IF(L51=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P51" s="20" t="str">
@@ -22159,7 +22261,7 @@
         <v>Sack</v>
       </c>
       <c r="O52" s="20" t="str">
-        <f>IF(L52=[1]Enums!$A$20, [1]Enums!$A$31, IF(N52=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L52=[1]Enums!$A$20, [1]Enums!$A$31, IF(L52=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P52" s="20" t="str">
@@ -22221,7 +22323,7 @@
         <v>Sack</v>
       </c>
       <c r="O53" s="20" t="str">
-        <f>IF(L53=[1]Enums!$A$20, [1]Enums!$A$31, IF(N53=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L53=[1]Enums!$A$20, [1]Enums!$A$31, IF(L53=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P53" s="20" t="str">
@@ -22283,7 +22385,7 @@
         <v>Sack</v>
       </c>
       <c r="O54" s="20" t="str">
-        <f>IF(L54=[1]Enums!$A$20, [1]Enums!$A$31, IF(N54=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L54=[1]Enums!$A$20, [1]Enums!$A$31, IF(L54=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P54" s="20" t="str">
@@ -22344,8 +22446,8 @@
         <f>IF(L55=[1]Enums!$A$20, [1]Enums!$A$28, IF(L55=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Cartridge</v>
       </c>
-      <c r="O55" s="24" t="str">
-        <f>IF(L55=[1]Enums!$A$20, [1]Enums!$A$31, IF(N55=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O55" s="20" t="str">
+        <f>IF(L55=[1]Enums!$A$20, [1]Enums!$A$31, IF(L55=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Canister</v>
       </c>
       <c r="P55" s="24" t="str">
@@ -22407,7 +22509,7 @@
         <v>Sack</v>
       </c>
       <c r="O56" s="20" t="str">
-        <f>IF(L56=[1]Enums!$A$20, [1]Enums!$A$31, IF(N56=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L56=[1]Enums!$A$20, [1]Enums!$A$31, IF(L56=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P56" s="20" t="str">
@@ -22469,7 +22571,7 @@
         <v>Sack</v>
       </c>
       <c r="O57" s="20" t="str">
-        <f>IF(L57=[1]Enums!$A$20, [1]Enums!$A$31, IF(N57=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L57=[1]Enums!$A$20, [1]Enums!$A$31, IF(L57=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P57" s="20" t="str">
@@ -22531,7 +22633,7 @@
         <v>Sack</v>
       </c>
       <c r="O58" s="20" t="str">
-        <f>IF(L58=[1]Enums!$A$20, [1]Enums!$A$31, IF(N58=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L58=[1]Enums!$A$20, [1]Enums!$A$31, IF(L58=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P58" s="20" t="str">
@@ -22593,7 +22695,7 @@
         <v>Sack</v>
       </c>
       <c r="O59" s="20" t="str">
-        <f>IF(L59=[1]Enums!$A$20, [1]Enums!$A$31, IF(N59=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L59=[1]Enums!$A$20, [1]Enums!$A$31, IF(L59=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P59" s="20" t="str">
@@ -22655,7 +22757,7 @@
         <v>Sack</v>
       </c>
       <c r="O60" s="20" t="str">
-        <f>IF(L60=[1]Enums!$A$20, [1]Enums!$A$31, IF(N60=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L60=[1]Enums!$A$20, [1]Enums!$A$31, IF(L60=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P60" s="20" t="str">
@@ -22717,7 +22819,7 @@
         <v>Sack</v>
       </c>
       <c r="O61" s="20" t="str">
-        <f>IF(L61=[1]Enums!$A$20, [1]Enums!$A$31, IF(N61=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L61=[1]Enums!$A$20, [1]Enums!$A$31, IF(L61=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P61" s="20" t="str">
@@ -22779,7 +22881,7 @@
         <v>Sack</v>
       </c>
       <c r="O62" s="20" t="str">
-        <f>IF(L62=[1]Enums!$A$20, [1]Enums!$A$31, IF(N62=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L62=[1]Enums!$A$20, [1]Enums!$A$31, IF(L62=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P62" s="20" t="str">
@@ -22841,7 +22943,7 @@
         <v>Sack</v>
       </c>
       <c r="O63" s="20" t="str">
-        <f>IF(L63=[1]Enums!$A$20, [1]Enums!$A$31, IF(N63=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L63=[1]Enums!$A$20, [1]Enums!$A$31, IF(L63=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P63" s="20" t="str">
@@ -22903,7 +23005,7 @@
         <v>Sack</v>
       </c>
       <c r="O64" s="20" t="str">
-        <f>IF(L64=[1]Enums!$A$20, [1]Enums!$A$31, IF(N64=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L64=[1]Enums!$A$20, [1]Enums!$A$31, IF(L64=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P64" s="20" t="str">
@@ -22965,7 +23067,7 @@
         <v>Sack</v>
       </c>
       <c r="O65" s="20" t="str">
-        <f>IF(L65=[1]Enums!$A$20, [1]Enums!$A$31, IF(N65=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L65=[1]Enums!$A$20, [1]Enums!$A$31, IF(L65=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P65" s="20" t="str">
@@ -23027,7 +23129,7 @@
         <v>Sack</v>
       </c>
       <c r="O66" s="20" t="str">
-        <f>IF(L66=[1]Enums!$A$20, [1]Enums!$A$31, IF(N66=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L66=[1]Enums!$A$20, [1]Enums!$A$31, IF(L66=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P66" s="20" t="str">
@@ -23089,7 +23191,7 @@
         <v>Sack</v>
       </c>
       <c r="O67" s="20" t="str">
-        <f>IF(L67=[1]Enums!$A$20, [1]Enums!$A$31, IF(N67=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L67=[1]Enums!$A$20, [1]Enums!$A$31, IF(L67=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P67" s="20" t="str">
@@ -23151,7 +23253,7 @@
         <v>Sack</v>
       </c>
       <c r="O68" s="20" t="str">
-        <f>IF(L68=[1]Enums!$A$20, [1]Enums!$A$31, IF(N68=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L68=[1]Enums!$A$20, [1]Enums!$A$31, IF(L68=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P68" s="20" t="str">
@@ -23213,7 +23315,7 @@
         <v>Sack</v>
       </c>
       <c r="O69" s="20" t="str">
-        <f>IF(L69=[1]Enums!$A$20, [1]Enums!$A$31, IF(N69=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L69=[1]Enums!$A$20, [1]Enums!$A$31, IF(L69=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P69" s="20" t="str">
@@ -23275,7 +23377,7 @@
         <v>Sack</v>
       </c>
       <c r="O70" s="20" t="str">
-        <f>IF(L70=[1]Enums!$A$20, [1]Enums!$A$31, IF(N70=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L70=[1]Enums!$A$20, [1]Enums!$A$31, IF(L70=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P70" s="20" t="str">
@@ -23337,7 +23439,7 @@
         <v>Sack</v>
       </c>
       <c r="O71" s="20" t="str">
-        <f>IF(L71=[1]Enums!$A$20, [1]Enums!$A$31, IF(N71=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L71=[1]Enums!$A$20, [1]Enums!$A$31, IF(L71=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P71" s="20" t="str">
@@ -23399,7 +23501,7 @@
         <v>Sack</v>
       </c>
       <c r="O72" s="20" t="str">
-        <f>IF(L72=[1]Enums!$A$20, [1]Enums!$A$31, IF(N72=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L72=[1]Enums!$A$20, [1]Enums!$A$31, IF(L72=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P72" s="20" t="str">
@@ -23461,7 +23563,7 @@
         <v>Sack</v>
       </c>
       <c r="O73" s="20" t="str">
-        <f>IF(L73=[1]Enums!$A$20, [1]Enums!$A$31, IF(N73=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L73=[1]Enums!$A$20, [1]Enums!$A$31, IF(L73=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P73" s="20" t="str">
@@ -23523,7 +23625,7 @@
         <v>Sack</v>
       </c>
       <c r="O74" s="20" t="str">
-        <f>IF(L74=[1]Enums!$A$20, [1]Enums!$A$31, IF(N74=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L74=[1]Enums!$A$20, [1]Enums!$A$31, IF(L74=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P74" s="20" t="str">
@@ -23585,7 +23687,7 @@
         <v>Sack</v>
       </c>
       <c r="O75" s="20" t="str">
-        <f>IF(L75=[1]Enums!$A$20, [1]Enums!$A$31, IF(N75=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L75=[1]Enums!$A$20, [1]Enums!$A$31, IF(L75=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P75" s="20" t="str">
@@ -23647,7 +23749,7 @@
         <v>Sack</v>
       </c>
       <c r="O76" s="20" t="str">
-        <f>IF(L76=[1]Enums!$A$20, [1]Enums!$A$31, IF(N76=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L76=[1]Enums!$A$20, [1]Enums!$A$31, IF(L76=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P76" s="20" t="str">
@@ -23709,7 +23811,7 @@
         <v>Sack</v>
       </c>
       <c r="O77" s="20" t="str">
-        <f>IF(L77=[1]Enums!$A$20, [1]Enums!$A$31, IF(N77=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L77=[1]Enums!$A$20, [1]Enums!$A$31, IF(L77=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P77" s="20" t="str">
@@ -23771,7 +23873,7 @@
         <v>Sack</v>
       </c>
       <c r="O78" s="20" t="str">
-        <f>IF(L78=[1]Enums!$A$20, [1]Enums!$A$31, IF(N78=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L78=[1]Enums!$A$20, [1]Enums!$A$31, IF(L78=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P78" s="20" t="str">
@@ -23833,7 +23935,7 @@
         <v>Sack</v>
       </c>
       <c r="O79" s="20" t="str">
-        <f>IF(L79=[1]Enums!$A$20, [1]Enums!$A$31, IF(N79=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L79=[1]Enums!$A$20, [1]Enums!$A$31, IF(L79=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P79" s="20" t="str">
@@ -23895,7 +23997,7 @@
         <v>Sack</v>
       </c>
       <c r="O80" s="20" t="str">
-        <f>IF(L80=[1]Enums!$A$20, [1]Enums!$A$31, IF(N80=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L80=[1]Enums!$A$20, [1]Enums!$A$31, IF(L80=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P80" s="20" t="str">
@@ -23930,7 +24032,7 @@
       </c>
       <c r="H81" s="16" t="str">
         <f t="shared" si="10"/>
-        <v>Powder Keg (Mercury)</v>
+        <v>Drum (Mercury)</v>
       </c>
       <c r="I81" s="16" t="str">
         <f t="shared" si="11"/>
@@ -23957,8 +24059,8 @@
         <v>Beaker</v>
       </c>
       <c r="O81" s="20" t="str">
-        <f>IF(L81=[1]Enums!$A$20, [1]Enums!$A$31, IF(N81=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
-        <v>Powder Keg</v>
+        <f>IF(L81=[1]Enums!$A$20, [1]Enums!$A$31, IF(L81=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <v>Drum</v>
       </c>
       <c r="P81" s="20" t="str">
         <f>IF(L81=[1]Enums!$A$20, [1]Enums!$A$34, IF(L81=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
@@ -24019,7 +24121,7 @@
         <v>Sack</v>
       </c>
       <c r="O82" s="20" t="str">
-        <f>IF(L82=[1]Enums!$A$20, [1]Enums!$A$31, IF(N82=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L82=[1]Enums!$A$20, [1]Enums!$A$31, IF(L82=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P82" s="20" t="str">
@@ -24081,7 +24183,7 @@
         <v>Sack</v>
       </c>
       <c r="O83" s="20" t="str">
-        <f>IF(L83=[1]Enums!$A$20, [1]Enums!$A$31, IF(N83=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L83=[1]Enums!$A$20, [1]Enums!$A$31, IF(L83=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P83" s="20" t="str">
@@ -24143,7 +24245,7 @@
         <v>Sack</v>
       </c>
       <c r="O84" s="20" t="str">
-        <f>IF(L84=[1]Enums!$A$20, [1]Enums!$A$31, IF(N84=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L84=[1]Enums!$A$20, [1]Enums!$A$31, IF(L84=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P84" s="20" t="str">
@@ -24205,7 +24307,7 @@
         <v>Sack</v>
       </c>
       <c r="O85" s="20" t="str">
-        <f>IF(L85=[1]Enums!$A$20, [1]Enums!$A$31, IF(N85=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L85=[1]Enums!$A$20, [1]Enums!$A$31, IF(L85=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P85" s="20" t="str">
@@ -24267,7 +24369,7 @@
         <v>Sack</v>
       </c>
       <c r="O86" s="20" t="str">
-        <f>IF(L86=[1]Enums!$A$20, [1]Enums!$A$31, IF(N86=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <f>IF(L86=[1]Enums!$A$20, [1]Enums!$A$31, IF(L86=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P86" s="20" t="str">
@@ -24328,8 +24430,8 @@
         <f>IF(L87=[1]Enums!$A$20, [1]Enums!$A$28, IF(L87=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Cartridge</v>
       </c>
-      <c r="O87" s="24" t="str">
-        <f>IF(L87=[1]Enums!$A$20, [1]Enums!$A$31, IF(N87=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O87" s="20" t="str">
+        <f>IF(L87=[1]Enums!$A$20, [1]Enums!$A$31, IF(L87=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Canister</v>
       </c>
       <c r="P87" s="24" t="str">
@@ -24390,8 +24492,8 @@
         <f>IF(L88=[1]Enums!$A$20, [1]Enums!$A$28, IF(L88=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O88" s="4" t="str">
-        <f>IF(L88=[1]Enums!$A$20, [1]Enums!$A$31, IF(N88=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O88" s="20" t="str">
+        <f>IF(L88=[1]Enums!$A$20, [1]Enums!$A$31, IF(L88=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P88" s="4" t="str">
@@ -24452,8 +24554,8 @@
         <f>IF(L89=[1]Enums!$A$20, [1]Enums!$A$28, IF(L89=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O89" s="4" t="str">
-        <f>IF(L89=[1]Enums!$A$20, [1]Enums!$A$31, IF(N89=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O89" s="20" t="str">
+        <f>IF(L89=[1]Enums!$A$20, [1]Enums!$A$31, IF(L89=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P89" s="4" t="str">
@@ -24514,8 +24616,8 @@
         <f>IF(L90=[1]Enums!$A$20, [1]Enums!$A$28, IF(L90=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O90" s="4" t="str">
-        <f>IF(L90=[1]Enums!$A$20, [1]Enums!$A$31, IF(N90=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O90" s="20" t="str">
+        <f>IF(L90=[1]Enums!$A$20, [1]Enums!$A$31, IF(L90=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P90" s="4" t="str">
@@ -24576,8 +24678,8 @@
         <f>IF(L91=[1]Enums!$A$20, [1]Enums!$A$28, IF(L91=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O91" s="4" t="str">
-        <f>IF(L91=[1]Enums!$A$20, [1]Enums!$A$31, IF(N91=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O91" s="20" t="str">
+        <f>IF(L91=[1]Enums!$A$20, [1]Enums!$A$31, IF(L91=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P91" s="4" t="str">
@@ -24638,8 +24740,8 @@
         <f>IF(L92=[1]Enums!$A$20, [1]Enums!$A$28, IF(L92=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O92" s="4" t="str">
-        <f>IF(L92=[1]Enums!$A$20, [1]Enums!$A$31, IF(N92=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O92" s="20" t="str">
+        <f>IF(L92=[1]Enums!$A$20, [1]Enums!$A$31, IF(L92=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P92" s="4" t="str">
@@ -24700,8 +24802,8 @@
         <f>IF(L93=[1]Enums!$A$20, [1]Enums!$A$28, IF(L93=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O93" s="4" t="str">
-        <f>IF(L93=[1]Enums!$A$20, [1]Enums!$A$31, IF(N93=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O93" s="20" t="str">
+        <f>IF(L93=[1]Enums!$A$20, [1]Enums!$A$31, IF(L93=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P93" s="4" t="str">
@@ -24762,8 +24864,8 @@
         <f>IF(L94=[1]Enums!$A$20, [1]Enums!$A$28, IF(L94=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O94" s="4" t="str">
-        <f>IF(L94=[1]Enums!$A$20, [1]Enums!$A$31, IF(N94=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O94" s="20" t="str">
+        <f>IF(L94=[1]Enums!$A$20, [1]Enums!$A$31, IF(L94=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P94" s="4" t="str">
@@ -24824,8 +24926,8 @@
         <f>IF(L95=[1]Enums!$A$20, [1]Enums!$A$28, IF(L95=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O95" s="4" t="str">
-        <f>IF(L95=[1]Enums!$A$20, [1]Enums!$A$31, IF(N95=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O95" s="20" t="str">
+        <f>IF(L95=[1]Enums!$A$20, [1]Enums!$A$31, IF(L95=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P95" s="4" t="str">
@@ -24886,8 +24988,8 @@
         <f>IF(L96=[1]Enums!$A$20, [1]Enums!$A$28, IF(L96=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O96" s="4" t="str">
-        <f>IF(L96=[1]Enums!$A$20, [1]Enums!$A$31, IF(N96=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O96" s="20" t="str">
+        <f>IF(L96=[1]Enums!$A$20, [1]Enums!$A$31, IF(L96=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P96" s="4" t="str">
@@ -24948,8 +25050,8 @@
         <f>IF(L97=[1]Enums!$A$20, [1]Enums!$A$28, IF(L97=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O97" s="4" t="str">
-        <f>IF(L97=[1]Enums!$A$20, [1]Enums!$A$31, IF(N97=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O97" s="20" t="str">
+        <f>IF(L97=[1]Enums!$A$20, [1]Enums!$A$31, IF(L97=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P97" s="4" t="str">
@@ -25010,8 +25112,8 @@
         <f>IF(L98=[1]Enums!$A$20, [1]Enums!$A$28, IF(L98=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O98" s="4" t="str">
-        <f>IF(L98=[1]Enums!$A$20, [1]Enums!$A$31, IF(N98=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O98" s="20" t="str">
+        <f>IF(L98=[1]Enums!$A$20, [1]Enums!$A$31, IF(L98=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P98" s="4" t="str">
@@ -25072,8 +25174,8 @@
         <f>IF(L99=[1]Enums!$A$20, [1]Enums!$A$28, IF(L99=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O99" s="4" t="str">
-        <f>IF(L99=[1]Enums!$A$20, [1]Enums!$A$31, IF(N99=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O99" s="20" t="str">
+        <f>IF(L99=[1]Enums!$A$20, [1]Enums!$A$31, IF(L99=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P99" s="4" t="str">
@@ -25134,8 +25236,8 @@
         <f>IF(L100=[1]Enums!$A$20, [1]Enums!$A$28, IF(L100=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O100" s="4" t="str">
-        <f>IF(L100=[1]Enums!$A$20, [1]Enums!$A$31, IF(N100=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O100" s="20" t="str">
+        <f>IF(L100=[1]Enums!$A$20, [1]Enums!$A$31, IF(L100=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P100" s="4" t="str">
@@ -25196,8 +25298,8 @@
         <f>IF(L101=[1]Enums!$A$20, [1]Enums!$A$28, IF(L101=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O101" s="4" t="str">
-        <f>IF(L101=[1]Enums!$A$20, [1]Enums!$A$31, IF(N101=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O101" s="20" t="str">
+        <f>IF(L101=[1]Enums!$A$20, [1]Enums!$A$31, IF(L101=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P101" s="4" t="str">
@@ -25258,8 +25360,8 @@
         <f>IF(L102=[1]Enums!$A$20, [1]Enums!$A$28, IF(L102=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O102" s="4" t="str">
-        <f>IF(L102=[1]Enums!$A$20, [1]Enums!$A$31, IF(N102=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O102" s="20" t="str">
+        <f>IF(L102=[1]Enums!$A$20, [1]Enums!$A$31, IF(L102=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P102" s="4" t="str">
@@ -25320,8 +25422,8 @@
         <f>IF(L103=[1]Enums!$A$20, [1]Enums!$A$28, IF(L103=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O103" s="4" t="str">
-        <f>IF(L103=[1]Enums!$A$20, [1]Enums!$A$31, IF(N103=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O103" s="20" t="str">
+        <f>IF(L103=[1]Enums!$A$20, [1]Enums!$A$31, IF(L103=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P103" s="4" t="str">
@@ -25382,8 +25484,8 @@
         <f>IF(L104=[1]Enums!$A$20, [1]Enums!$A$28, IF(L104=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O104" s="4" t="str">
-        <f>IF(L104=[1]Enums!$A$20, [1]Enums!$A$31, IF(N104=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O104" s="20" t="str">
+        <f>IF(L104=[1]Enums!$A$20, [1]Enums!$A$31, IF(L104=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P104" s="4" t="str">
@@ -25444,8 +25546,8 @@
         <f>IF(L105=[1]Enums!$A$20, [1]Enums!$A$28, IF(L105=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O105" s="4" t="str">
-        <f>IF(L105=[1]Enums!$A$20, [1]Enums!$A$31, IF(N105=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O105" s="20" t="str">
+        <f>IF(L105=[1]Enums!$A$20, [1]Enums!$A$31, IF(L105=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P105" s="4" t="str">
@@ -25506,8 +25608,8 @@
         <f>IF(L106=[1]Enums!$A$20, [1]Enums!$A$28, IF(L106=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O106" s="4" t="str">
-        <f>IF(L106=[1]Enums!$A$20, [1]Enums!$A$31, IF(N106=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O106" s="20" t="str">
+        <f>IF(L106=[1]Enums!$A$20, [1]Enums!$A$31, IF(L106=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P106" s="4" t="str">
@@ -25568,8 +25670,8 @@
         <f>IF(L107=[1]Enums!$A$20, [1]Enums!$A$28, IF(L107=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O107" s="4" t="str">
-        <f>IF(L107=[1]Enums!$A$20, [1]Enums!$A$31, IF(N107=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O107" s="20" t="str">
+        <f>IF(L107=[1]Enums!$A$20, [1]Enums!$A$31, IF(L107=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P107" s="4" t="str">
@@ -25630,8 +25732,8 @@
         <f>IF(L108=[1]Enums!$A$20, [1]Enums!$A$28, IF(L108=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O108" s="4" t="str">
-        <f>IF(L108=[1]Enums!$A$20, [1]Enums!$A$31, IF(N108=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O108" s="20" t="str">
+        <f>IF(L108=[1]Enums!$A$20, [1]Enums!$A$31, IF(L108=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P108" s="4" t="str">
@@ -25692,8 +25794,8 @@
         <f>IF(L109=[1]Enums!$A$20, [1]Enums!$A$28, IF(L109=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O109" s="4" t="str">
-        <f>IF(L109=[1]Enums!$A$20, [1]Enums!$A$31, IF(N109=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O109" s="20" t="str">
+        <f>IF(L109=[1]Enums!$A$20, [1]Enums!$A$31, IF(L109=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P109" s="4" t="str">
@@ -25754,8 +25856,8 @@
         <f>IF(L110=[1]Enums!$A$20, [1]Enums!$A$28, IF(L110=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O110" s="4" t="str">
-        <f>IF(L110=[1]Enums!$A$20, [1]Enums!$A$31, IF(N110=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O110" s="20" t="str">
+        <f>IF(L110=[1]Enums!$A$20, [1]Enums!$A$31, IF(L110=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P110" s="4" t="str">
@@ -25816,8 +25918,8 @@
         <f>IF(L111=[1]Enums!$A$20, [1]Enums!$A$28, IF(L111=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O111" s="4" t="str">
-        <f>IF(L111=[1]Enums!$A$20, [1]Enums!$A$31, IF(N111=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O111" s="20" t="str">
+        <f>IF(L111=[1]Enums!$A$20, [1]Enums!$A$31, IF(L111=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P111" s="4" t="str">
@@ -25878,8 +25980,8 @@
         <f>IF(L112=[1]Enums!$A$20, [1]Enums!$A$28, IF(L112=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O112" s="4" t="str">
-        <f>IF(L112=[1]Enums!$A$20, [1]Enums!$A$31, IF(N112=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O112" s="20" t="str">
+        <f>IF(L112=[1]Enums!$A$20, [1]Enums!$A$31, IF(L112=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P112" s="4" t="str">
@@ -25940,8 +26042,8 @@
         <f>IF(L113=[1]Enums!$A$20, [1]Enums!$A$28, IF(L113=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O113" s="4" t="str">
-        <f>IF(L113=[1]Enums!$A$20, [1]Enums!$A$31, IF(N113=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O113" s="20" t="str">
+        <f>IF(L113=[1]Enums!$A$20, [1]Enums!$A$31, IF(L113=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P113" s="4" t="str">
@@ -26002,8 +26104,8 @@
         <f>IF(L114=[1]Enums!$A$20, [1]Enums!$A$28, IF(L114=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O114" s="4" t="str">
-        <f>IF(L114=[1]Enums!$A$20, [1]Enums!$A$31, IF(N114=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O114" s="20" t="str">
+        <f>IF(L114=[1]Enums!$A$20, [1]Enums!$A$31, IF(L114=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P114" s="4" t="str">
@@ -26064,8 +26166,8 @@
         <f>IF(L115=[1]Enums!$A$20, [1]Enums!$A$28, IF(L115=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O115" s="4" t="str">
-        <f>IF(L115=[1]Enums!$A$20, [1]Enums!$A$31, IF(N115=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O115" s="20" t="str">
+        <f>IF(L115=[1]Enums!$A$20, [1]Enums!$A$31, IF(L115=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P115" s="4" t="str">
@@ -26126,8 +26228,8 @@
         <f>IF(L116=[1]Enums!$A$20, [1]Enums!$A$28, IF(L116=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O116" s="4" t="str">
-        <f>IF(L116=[1]Enums!$A$20, [1]Enums!$A$31, IF(N116=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O116" s="20" t="str">
+        <f>IF(L116=[1]Enums!$A$20, [1]Enums!$A$31, IF(L116=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P116" s="4" t="str">
@@ -26188,8 +26290,8 @@
         <f>IF(L117=[1]Enums!$A$20, [1]Enums!$A$28, IF(L117=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O117" s="4" t="str">
-        <f>IF(L117=[1]Enums!$A$20, [1]Enums!$A$31, IF(N117=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O117" s="20" t="str">
+        <f>IF(L117=[1]Enums!$A$20, [1]Enums!$A$31, IF(L117=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P117" s="4" t="str">
@@ -26250,8 +26352,8 @@
         <f>IF(L118=[1]Enums!$A$20, [1]Enums!$A$28, IF(L118=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O118" s="4" t="str">
-        <f>IF(L118=[1]Enums!$A$20, [1]Enums!$A$31, IF(N118=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O118" s="20" t="str">
+        <f>IF(L118=[1]Enums!$A$20, [1]Enums!$A$31, IF(L118=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P118" s="4" t="str">
@@ -26312,8 +26414,8 @@
         <f>IF(L119=[1]Enums!$A$20, [1]Enums!$A$28, IF(L119=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
         <v>Sack</v>
       </c>
-      <c r="O119" s="4" t="str">
-        <f>IF(L119=[1]Enums!$A$20, [1]Enums!$A$31, IF(N119=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+      <c r="O119" s="20" t="str">
+        <f>IF(L119=[1]Enums!$A$20, [1]Enums!$A$31, IF(L119=[1]Enums!$B$30, [1]Enums!$A$30, [1]Enums!$A$29))</f>
         <v>Powder Keg</v>
       </c>
       <c r="P119" s="4" t="str">
@@ -26334,8 +26436,8 @@
   </sheetPr>
   <dimension ref="A1:O390"/>
   <sheetViews>
-    <sheetView topLeftCell="A355" workbookViewId="0">
-      <selection activeCell="J380" sqref="J380"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="A167" sqref="A167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -35462,7 +35564,10 @@
       </c>
     </row>
     <row r="162" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A162" s="4"/>
+      <c r="A162" s="4" t="str">
+        <f>[1]Enums!$A$14</f>
+        <v>1.1.2</v>
+      </c>
       <c r="B162" s="13" t="s">
         <v>778</v>
       </c>
@@ -41579,19 +41684,19 @@
       </c>
       <c r="F270" s="16" t="str">
         <f t="shared" si="16"/>
-        <v>Vial (Sodium Hydroxide)</v>
+        <v>Bag (Sodium Hydroxide)</v>
       </c>
       <c r="G270" s="16" t="str">
         <f t="shared" si="17"/>
-        <v>Beaker (Sodium Hydroxide)</v>
+        <v>Sack (Sodium Hydroxide)</v>
       </c>
       <c r="H270" s="16" t="str">
         <f t="shared" si="18"/>
-        <v>Drum (Sodium Hydroxide)</v>
+        <v>Powder Keg (Sodium Hydroxide)</v>
       </c>
       <c r="I270" s="16" t="str">
         <f t="shared" si="19"/>
-        <v>Chemical Vat (Sodium Hydroxide)</v>
+        <v>Chemical Silo (Sodium Hydroxide)</v>
       </c>
       <c r="J270" s="16" t="str">
         <f>[1]Compounds!$B260</f>
@@ -41599,23 +41704,23 @@
       </c>
       <c r="K270" t="str">
         <f>[1]Compounds!$D260</f>
-        <v>Liquid</v>
+        <v>Solid</v>
       </c>
       <c r="L270" s="4" t="str">
         <f>IF(K270=[1]Enums!$A$20, [1]Enums!$A$25, IF(K270=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
-        <v>Vial</v>
+        <v>Bag</v>
       </c>
       <c r="M270" s="4" t="str">
         <f>IF(K270=[1]Enums!$A$20, [1]Enums!$A$28, IF(K270=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
-        <v>Beaker</v>
+        <v>Sack</v>
       </c>
       <c r="N270" s="4" t="str">
         <f>IF(K270=[1]Enums!$A$20, [1]Enums!$A$31, IF(K270=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
-        <v>Drum</v>
+        <v>Powder Keg</v>
       </c>
       <c r="O270" s="4" t="str">
         <f>IF(K270=[1]Enums!$A$20, [1]Enums!$A$34, IF(K270=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
-        <v>Chemical Vat</v>
+        <v>Chemical Silo</v>
       </c>
     </row>
     <row r="271" spans="1:15" x14ac:dyDescent="0.2">
@@ -47918,6 +48023,10 @@
       </c>
     </row>
     <row r="381" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A381" s="4" t="str">
+        <f>[1]Enums!$A$14</f>
+        <v>1.1.2</v>
+      </c>
       <c r="B381" s="13" t="s">
         <v>2302</v>
       </c>
@@ -47932,46 +48041,50 @@
       </c>
       <c r="F381" s="16" t="str">
         <f t="shared" si="45"/>
-        <v>Bag (0)</v>
+        <v>Flask (Nitrogen Dioxide)</v>
       </c>
       <c r="G381" s="16" t="str">
         <f t="shared" si="46"/>
-        <v>Sack (0)</v>
+        <v>Cartridge (Nitrogen Dioxide)</v>
       </c>
       <c r="H381" s="16" t="str">
         <f t="shared" si="47"/>
-        <v>Powder Keg (0)</v>
+        <v>Canister (Nitrogen Dioxide)</v>
       </c>
       <c r="I381" s="16" t="str">
         <f t="shared" si="48"/>
-        <v>Chemical Silo (0)</v>
-      </c>
-      <c r="J381" s="16">
+        <v>Chemical Tank (Nitrogen Dioxide)</v>
+      </c>
+      <c r="J381" s="16" t="str">
         <f>[1]Compounds!$B389</f>
-        <v>0</v>
-      </c>
-      <c r="K381">
+        <v>Nitrogen Dioxide</v>
+      </c>
+      <c r="K381" t="str">
         <f>[1]Compounds!$D389</f>
-        <v>0</v>
+        <v>Gas</v>
       </c>
       <c r="L381" s="4" t="str">
         <f>IF(K381=[1]Enums!$A$20, [1]Enums!$A$25, IF(K381=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
-        <v>Bag</v>
+        <v>Flask</v>
       </c>
       <c r="M381" s="4" t="str">
         <f>IF(K381=[1]Enums!$A$20, [1]Enums!$A$28, IF(K381=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
-        <v>Sack</v>
+        <v>Cartridge</v>
       </c>
       <c r="N381" s="4" t="str">
         <f>IF(K381=[1]Enums!$A$20, [1]Enums!$A$31, IF(K381=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
-        <v>Powder Keg</v>
+        <v>Canister</v>
       </c>
       <c r="O381" s="4" t="str">
         <f>IF(K381=[1]Enums!$A$20, [1]Enums!$A$34, IF(K381=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
-        <v>Chemical Silo</v>
+        <v>Chemical Tank</v>
       </c>
     </row>
     <row r="382" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A382" s="4" t="str">
+        <f>[1]Enums!$A$14</f>
+        <v>1.1.2</v>
+      </c>
       <c r="B382" s="13" t="s">
         <v>2298</v>
       </c>
@@ -47986,27 +48099,27 @@
       </c>
       <c r="F382" s="16" t="str">
         <f t="shared" si="45"/>
-        <v>Bag (0)</v>
+        <v>Bag (Sodium Nitrite)</v>
       </c>
       <c r="G382" s="16" t="str">
         <f t="shared" si="46"/>
-        <v>Sack (0)</v>
+        <v>Sack (Sodium Nitrite)</v>
       </c>
       <c r="H382" s="16" t="str">
         <f t="shared" si="47"/>
-        <v>Powder Keg (0)</v>
+        <v>Powder Keg (Sodium Nitrite)</v>
       </c>
       <c r="I382" s="16" t="str">
         <f t="shared" si="48"/>
-        <v>Chemical Silo (0)</v>
-      </c>
-      <c r="J382" s="16">
+        <v>Chemical Silo (Sodium Nitrite)</v>
+      </c>
+      <c r="J382" s="16" t="str">
         <f>[1]Compounds!$B390</f>
-        <v>0</v>
-      </c>
-      <c r="K382">
+        <v>Sodium Nitrite</v>
+      </c>
+      <c r="K382" t="str">
         <f>[1]Compounds!$D390</f>
-        <v>0</v>
+        <v>Solid</v>
       </c>
       <c r="L382" s="4" t="str">
         <f>IF(K382=[1]Enums!$A$20, [1]Enums!$A$25, IF(K382=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
@@ -48026,6 +48139,10 @@
       </c>
     </row>
     <row r="383" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A383" s="4" t="str">
+        <f>[1]Enums!$A$14</f>
+        <v>1.1.2</v>
+      </c>
       <c r="B383" s="13" t="s">
         <v>2294</v>
       </c>
@@ -48040,43 +48157,43 @@
       </c>
       <c r="F383" s="16" t="str">
         <f t="shared" si="45"/>
-        <v>Bag (0)</v>
+        <v>Vial (Dicyclopentadiene)</v>
       </c>
       <c r="G383" s="16" t="str">
         <f t="shared" si="46"/>
-        <v>Sack (0)</v>
+        <v>Beaker (Dicyclopentadiene)</v>
       </c>
       <c r="H383" s="16" t="str">
         <f t="shared" si="47"/>
-        <v>Powder Keg (0)</v>
+        <v>Drum (Dicyclopentadiene)</v>
       </c>
       <c r="I383" s="16" t="str">
         <f t="shared" si="48"/>
-        <v>Chemical Silo (0)</v>
-      </c>
-      <c r="J383" s="16">
+        <v>Chemical Vat (Dicyclopentadiene)</v>
+      </c>
+      <c r="J383" s="16" t="str">
         <f>[1]Compounds!$B391</f>
-        <v>0</v>
-      </c>
-      <c r="K383">
+        <v>Dicyclopentadiene</v>
+      </c>
+      <c r="K383" t="str">
         <f>[1]Compounds!$D391</f>
-        <v>0</v>
+        <v>Liquid</v>
       </c>
       <c r="L383" s="4" t="str">
         <f>IF(K383=[1]Enums!$A$20, [1]Enums!$A$25, IF(K383=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
-        <v>Bag</v>
+        <v>Vial</v>
       </c>
       <c r="M383" s="4" t="str">
         <f>IF(K383=[1]Enums!$A$20, [1]Enums!$A$28, IF(K383=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
-        <v>Sack</v>
+        <v>Beaker</v>
       </c>
       <c r="N383" s="4" t="str">
         <f>IF(K383=[1]Enums!$A$20, [1]Enums!$A$31, IF(K383=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
-        <v>Powder Keg</v>
+        <v>Drum</v>
       </c>
       <c r="O383" s="4" t="str">
         <f>IF(K383=[1]Enums!$A$20, [1]Enums!$A$34, IF(K383=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
-        <v>Chemical Silo</v>
+        <v>Chemical Vat</v>
       </c>
     </row>
     <row r="384" spans="1:15" x14ac:dyDescent="0.2">
@@ -50927,7 +51044,7 @@
       </c>
       <c r="B137" t="str">
         <f t="shared" si="7"/>
-        <v>Vial (Sodium Hydroxide)</v>
+        <v>Bag (Sodium Hydroxide)</v>
       </c>
       <c r="C137" t="str">
         <f>[1]Compounds!$B$260</f>
@@ -50935,7 +51052,7 @@
       </c>
       <c r="D137" t="str">
         <f>IF(VLOOKUP(C137,[1]Compounds!B:D,3,FALSE)=[1]Enums!$A$18,[1]Enums!$A$23,IF(VLOOKUP(C137,[1]Compounds!B:D,3,FALSE)=[1]Enums!$A$19,[1]Enums!$A$24,[1]Enums!$A$25))</f>
-        <v>Vial</v>
+        <v>Bag</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
@@ -50945,7 +51062,7 @@
       </c>
       <c r="B138" t="str">
         <f t="shared" si="7"/>
-        <v>Beaker (Sodium Hydroxide)</v>
+        <v>Sack (Sodium Hydroxide)</v>
       </c>
       <c r="C138" t="str">
         <f>[1]Compounds!$B$260</f>
@@ -50953,7 +51070,7 @@
       </c>
       <c r="D138" t="str">
         <f>IF(VLOOKUP(C138,[1]Compounds!B:D,3,FALSE)=[1]Enums!$A$18,[1]Enums!$A$26,IF(VLOOKUP(C138,[1]Compounds!B:D,3,FALSE)=[1]Enums!$A$19,[1]Enums!$A$27,[1]Enums!$A$28))</f>
-        <v>Beaker</v>
+        <v>Sack</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
@@ -50963,7 +51080,7 @@
       </c>
       <c r="B139" t="str">
         <f t="shared" si="7"/>
-        <v>Drum (Sodium Hydroxide)</v>
+        <v>Powder Keg (Sodium Hydroxide)</v>
       </c>
       <c r="C139" t="str">
         <f>[1]Compounds!$B$260</f>
@@ -50971,7 +51088,7 @@
       </c>
       <c r="D139" t="str">
         <f>IF(VLOOKUP(C139,[1]Compounds!B:D,3,FALSE)=[1]Enums!$A$18,[1]Enums!$A$29,IF(VLOOKUP(C139,[1]Compounds!B:D,3,FALSE)=[1]Enums!$A$19,[1]Enums!$A$30,[1]Enums!$A$31))</f>
-        <v>Drum</v>
+        <v>Powder Keg</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
1.1.13 Updates on Recipes and 3D rendering code
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2373" uniqueCount="2338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2416" uniqueCount="2380">
   <si>
     <t>Ore</t>
   </si>
@@ -7051,6 +7051,132 @@
   </si>
   <si>
     <t>19T</t>
+  </si>
+  <si>
+    <t>16w</t>
+  </si>
+  <si>
+    <t>15r</t>
+  </si>
+  <si>
+    <t>14m</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>16v</t>
+  </si>
+  <si>
+    <t>15q</t>
+  </si>
+  <si>
+    <t>14l</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>16u</t>
+  </si>
+  <si>
+    <t>15p</t>
+  </si>
+  <si>
+    <t>14k</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>16t</t>
+  </si>
+  <si>
+    <t>15o</t>
+  </si>
+  <si>
+    <t>14j</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>16s</t>
+  </si>
+  <si>
+    <t>15n</t>
+  </si>
+  <si>
+    <t>14i</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>16r</t>
+  </si>
+  <si>
+    <t>15m</t>
+  </si>
+  <si>
+    <t>14h</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>16q</t>
+  </si>
+  <si>
+    <t>15l</t>
+  </si>
+  <si>
+    <t>14g</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>16p</t>
+  </si>
+  <si>
+    <t>15k</t>
+  </si>
+  <si>
+    <t>14f</t>
+  </si>
+  <si>
+    <t>5Z</t>
+  </si>
+  <si>
+    <t>16o</t>
+  </si>
+  <si>
+    <t>15j</t>
+  </si>
+  <si>
+    <t>14e</t>
+  </si>
+  <si>
+    <t>5Y</t>
+  </si>
+  <si>
+    <t>16n</t>
+  </si>
+  <si>
+    <t>15i</t>
+  </si>
+  <si>
+    <t>14d</t>
+  </si>
+  <si>
+    <t>5X</t>
+  </si>
+  <si>
+    <t>Carbon Fiber Weave</t>
+  </si>
+  <si>
+    <t>1bz</t>
   </si>
 </sst>
 </file>
@@ -12827,7 +12953,7 @@
         </row>
         <row r="371">
           <cell r="B371" t="str">
-            <v>Terephthaloyl chloride</v>
+            <v>Terephthaloyl Chloride</v>
           </cell>
           <cell r="D371" t="str">
             <v>Solid</v>
@@ -12835,7 +12961,7 @@
         </row>
         <row r="372">
           <cell r="B372" t="str">
-            <v>Isophthaloyl chloride</v>
+            <v>Isophthaloyl Chloride</v>
           </cell>
           <cell r="D372" t="str">
             <v>Solid</v>
@@ -12859,7 +12985,7 @@
         </row>
         <row r="375">
           <cell r="B375" t="str">
-            <v>Anilene</v>
+            <v>Aniline</v>
           </cell>
           <cell r="D375" t="str">
             <v>Liquid</v>
@@ -12993,6 +13119,79 @@
             <v>Dicyclopentadiene</v>
           </cell>
           <cell r="D391" t="str">
+            <v>Liquid</v>
+          </cell>
+        </row>
+        <row r="392">
+          <cell r="B392" t="str">
+            <v>Tetrafluoroboric Acid</v>
+          </cell>
+          <cell r="C392" t="str">
+            <v>HBF4</v>
+          </cell>
+          <cell r="D392" t="str">
+            <v>Liquid</v>
+          </cell>
+        </row>
+        <row r="393">
+          <cell r="B393" t="str">
+            <v>Fluorobenzene</v>
+          </cell>
+          <cell r="C393" t="str">
+            <v>C6H5F</v>
+          </cell>
+          <cell r="D393" t="str">
+            <v>Liquid</v>
+          </cell>
+        </row>
+        <row r="394">
+          <cell r="B394" t="str">
+            <v>p-Fluorobenzoyl Chloride</v>
+          </cell>
+          <cell r="C394" t="str">
+            <v>C7H4ClFO</v>
+          </cell>
+          <cell r="D394" t="str">
+            <v>Liquid</v>
+          </cell>
+        </row>
+        <row r="395">
+          <cell r="B395" t="str">
+            <v>p-Nitrotoluene</v>
+          </cell>
+          <cell r="D395" t="str">
+            <v>Liquid</v>
+          </cell>
+        </row>
+        <row r="396">
+          <cell r="B396" t="str">
+            <v>p-Aminotoluene</v>
+          </cell>
+          <cell r="D396" t="str">
+            <v>Liquid</v>
+          </cell>
+        </row>
+        <row r="397">
+          <cell r="B397" t="str">
+            <v>p-Fluorotoluene</v>
+          </cell>
+          <cell r="D397" t="str">
+            <v>Liquid</v>
+          </cell>
+        </row>
+        <row r="398">
+          <cell r="B398" t="str">
+            <v>1-(Trichloromethyl)-4-Fluorobenzene</v>
+          </cell>
+          <cell r="D398" t="str">
+            <v>Liquid</v>
+          </cell>
+        </row>
+        <row r="399">
+          <cell r="B399" t="str">
+            <v>4,4-Difluorobenzophenone</v>
+          </cell>
+          <cell r="D399" t="str">
             <v>Liquid</v>
           </cell>
         </row>
@@ -13296,8 +13495,8 @@
   </sheetPr>
   <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14930,8 +15129,29 @@
       </c>
     </row>
     <row r="56" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+      <c r="A56" s="29" t="str">
+        <f>[1]Enums!$A$14</f>
+        <v>1.1.2</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>2379</v>
+      </c>
+      <c r="C56" s="26" t="s">
+        <v>2378</v>
+      </c>
+      <c r="D56" s="26" t="s">
+        <v>1965</v>
+      </c>
+      <c r="E56" s="26">
+        <v>8</v>
+      </c>
+      <c r="F56" s="26" t="b">
+        <v>0</v>
+      </c>
       <c r="G56" s="28"/>
-      <c r="H56" s="28"/>
+      <c r="H56" s="28">
+        <v>64</v>
+      </c>
       <c r="I56" s="28"/>
     </row>
     <row r="57" spans="1:15" ht="15" x14ac:dyDescent="0.2">
@@ -26434,10 +26654,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:O390"/>
+  <dimension ref="A1:O399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="A167" sqref="A167"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="A234" sqref="A234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -39546,7 +39766,10 @@
       </c>
     </row>
     <row r="232" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A232" s="4"/>
+      <c r="A232" s="4" t="str">
+        <f>[1]Enums!$A$14</f>
+        <v>1.1.2</v>
+      </c>
       <c r="B232" s="13" t="s">
         <v>708</v>
       </c>
@@ -46997,23 +47220,23 @@
       </c>
       <c r="F363" s="16" t="str">
         <f t="shared" si="33"/>
-        <v>Bag (Terephthaloyl chloride)</v>
+        <v>Bag (Terephthaloyl Chloride)</v>
       </c>
       <c r="G363" s="16" t="str">
         <f t="shared" si="34"/>
-        <v>Sack (Terephthaloyl chloride)</v>
+        <v>Sack (Terephthaloyl Chloride)</v>
       </c>
       <c r="H363" s="16" t="str">
         <f t="shared" si="35"/>
-        <v>Powder Keg (Terephthaloyl chloride)</v>
+        <v>Powder Keg (Terephthaloyl Chloride)</v>
       </c>
       <c r="I363" s="16" t="str">
         <f t="shared" si="36"/>
-        <v>Chemical Silo (Terephthaloyl chloride)</v>
+        <v>Chemical Silo (Terephthaloyl Chloride)</v>
       </c>
       <c r="J363" s="16" t="str">
         <f>[1]Compounds!$B371</f>
-        <v>Terephthaloyl chloride</v>
+        <v>Terephthaloyl Chloride</v>
       </c>
       <c r="K363" t="str">
         <f>[1]Compounds!$D371</f>
@@ -47055,23 +47278,23 @@
       </c>
       <c r="F364" s="16" t="str">
         <f t="shared" si="33"/>
-        <v>Bag (Isophthaloyl chloride)</v>
+        <v>Bag (Isophthaloyl Chloride)</v>
       </c>
       <c r="G364" s="16" t="str">
         <f t="shared" si="34"/>
-        <v>Sack (Isophthaloyl chloride)</v>
+        <v>Sack (Isophthaloyl Chloride)</v>
       </c>
       <c r="H364" s="16" t="str">
         <f t="shared" si="35"/>
-        <v>Powder Keg (Isophthaloyl chloride)</v>
+        <v>Powder Keg (Isophthaloyl Chloride)</v>
       </c>
       <c r="I364" s="16" t="str">
         <f t="shared" si="36"/>
-        <v>Chemical Silo (Isophthaloyl chloride)</v>
+        <v>Chemical Silo (Isophthaloyl Chloride)</v>
       </c>
       <c r="J364" s="16" t="str">
         <f>[1]Compounds!$B372</f>
-        <v>Isophthaloyl chloride</v>
+        <v>Isophthaloyl Chloride</v>
       </c>
       <c r="K364" t="str">
         <f>[1]Compounds!$D372</f>
@@ -47229,23 +47452,23 @@
       </c>
       <c r="F367" s="16" t="str">
         <f t="shared" ref="F367" si="37">L367&amp;" ("&amp;$J367&amp;")"</f>
-        <v>Vial (Anilene)</v>
+        <v>Vial (Aniline)</v>
       </c>
       <c r="G367" s="16" t="str">
         <f t="shared" ref="G367" si="38">M367&amp;" ("&amp;$J367&amp;")"</f>
-        <v>Beaker (Anilene)</v>
+        <v>Beaker (Aniline)</v>
       </c>
       <c r="H367" s="16" t="str">
         <f t="shared" ref="H367" si="39">N367&amp;" ("&amp;$J367&amp;")"</f>
-        <v>Drum (Anilene)</v>
+        <v>Drum (Aniline)</v>
       </c>
       <c r="I367" s="16" t="str">
         <f t="shared" ref="I367" si="40">O367&amp;" ("&amp;$J367&amp;")"</f>
-        <v>Chemical Vat (Anilene)</v>
+        <v>Chemical Vat (Aniline)</v>
       </c>
       <c r="J367" s="16" t="str">
         <f>[1]Compounds!$B375</f>
-        <v>Anilene</v>
+        <v>Aniline</v>
       </c>
       <c r="K367" t="str">
         <f>[1]Compounds!$D375</f>
@@ -48197,6 +48420,10 @@
       </c>
     </row>
     <row r="384" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A384" s="4" t="str">
+        <f>[1]Enums!$A$14</f>
+        <v>1.1.2</v>
+      </c>
       <c r="B384" s="13" t="s">
         <v>2290</v>
       </c>
@@ -48211,46 +48438,50 @@
       </c>
       <c r="F384" s="16" t="str">
         <f t="shared" si="45"/>
-        <v>Bag (0)</v>
+        <v>Vial (Tetrafluoroboric Acid)</v>
       </c>
       <c r="G384" s="16" t="str">
         <f t="shared" si="46"/>
-        <v>Sack (0)</v>
+        <v>Beaker (Tetrafluoroboric Acid)</v>
       </c>
       <c r="H384" s="16" t="str">
         <f t="shared" si="47"/>
-        <v>Powder Keg (0)</v>
+        <v>Drum (Tetrafluoroboric Acid)</v>
       </c>
       <c r="I384" s="16" t="str">
         <f t="shared" si="48"/>
-        <v>Chemical Silo (0)</v>
-      </c>
-      <c r="J384" s="16">
+        <v>Chemical Vat (Tetrafluoroboric Acid)</v>
+      </c>
+      <c r="J384" s="16" t="str">
         <f>[1]Compounds!$B392</f>
-        <v>0</v>
-      </c>
-      <c r="K384">
+        <v>Tetrafluoroboric Acid</v>
+      </c>
+      <c r="K384" t="str">
         <f>[1]Compounds!$D392</f>
-        <v>0</v>
+        <v>Liquid</v>
       </c>
       <c r="L384" s="4" t="str">
         <f>IF(K384=[1]Enums!$A$20, [1]Enums!$A$25, IF(K384=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
-        <v>Bag</v>
+        <v>Vial</v>
       </c>
       <c r="M384" s="4" t="str">
         <f>IF(K384=[1]Enums!$A$20, [1]Enums!$A$28, IF(K384=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
-        <v>Sack</v>
+        <v>Beaker</v>
       </c>
       <c r="N384" s="4" t="str">
         <f>IF(K384=[1]Enums!$A$20, [1]Enums!$A$31, IF(K384=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
-        <v>Powder Keg</v>
+        <v>Drum</v>
       </c>
       <c r="O384" s="4" t="str">
         <f>IF(K384=[1]Enums!$A$20, [1]Enums!$A$34, IF(K384=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
-        <v>Chemical Silo</v>
-      </c>
-    </row>
-    <row r="385" spans="2:15" x14ac:dyDescent="0.2">
+        <v>Chemical Vat</v>
+      </c>
+    </row>
+    <row r="385" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A385" s="4" t="str">
+        <f>[1]Enums!$A$14</f>
+        <v>1.1.2</v>
+      </c>
       <c r="B385" s="13" t="s">
         <v>2286</v>
       </c>
@@ -48265,46 +48496,50 @@
       </c>
       <c r="F385" s="16" t="str">
         <f t="shared" si="45"/>
-        <v>Bag (0)</v>
+        <v>Vial (Fluorobenzene)</v>
       </c>
       <c r="G385" s="16" t="str">
         <f t="shared" si="46"/>
-        <v>Sack (0)</v>
+        <v>Beaker (Fluorobenzene)</v>
       </c>
       <c r="H385" s="16" t="str">
         <f t="shared" si="47"/>
-        <v>Powder Keg (0)</v>
+        <v>Drum (Fluorobenzene)</v>
       </c>
       <c r="I385" s="16" t="str">
         <f t="shared" si="48"/>
-        <v>Chemical Silo (0)</v>
-      </c>
-      <c r="J385" s="16">
+        <v>Chemical Vat (Fluorobenzene)</v>
+      </c>
+      <c r="J385" s="16" t="str">
         <f>[1]Compounds!$B393</f>
-        <v>0</v>
-      </c>
-      <c r="K385">
+        <v>Fluorobenzene</v>
+      </c>
+      <c r="K385" t="str">
         <f>[1]Compounds!$D393</f>
-        <v>0</v>
+        <v>Liquid</v>
       </c>
       <c r="L385" s="4" t="str">
         <f>IF(K385=[1]Enums!$A$20, [1]Enums!$A$25, IF(K385=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
-        <v>Bag</v>
+        <v>Vial</v>
       </c>
       <c r="M385" s="4" t="str">
         <f>IF(K385=[1]Enums!$A$20, [1]Enums!$A$28, IF(K385=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
-        <v>Sack</v>
+        <v>Beaker</v>
       </c>
       <c r="N385" s="4" t="str">
         <f>IF(K385=[1]Enums!$A$20, [1]Enums!$A$31, IF(K385=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
-        <v>Powder Keg</v>
+        <v>Drum</v>
       </c>
       <c r="O385" s="4" t="str">
         <f>IF(K385=[1]Enums!$A$20, [1]Enums!$A$34, IF(K385=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
-        <v>Chemical Silo</v>
-      </c>
-    </row>
-    <row r="386" spans="2:15" x14ac:dyDescent="0.2">
+        <v>Chemical Vat</v>
+      </c>
+    </row>
+    <row r="386" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A386" s="4" t="str">
+        <f>[1]Enums!$A$14</f>
+        <v>1.1.2</v>
+      </c>
       <c r="B386" s="13" t="s">
         <v>2282</v>
       </c>
@@ -48319,46 +48554,50 @@
       </c>
       <c r="F386" s="16" t="str">
         <f t="shared" si="45"/>
-        <v>Bag (0)</v>
+        <v>Vial (p-Fluorobenzoyl Chloride)</v>
       </c>
       <c r="G386" s="16" t="str">
         <f t="shared" si="46"/>
-        <v>Sack (0)</v>
+        <v>Beaker (p-Fluorobenzoyl Chloride)</v>
       </c>
       <c r="H386" s="16" t="str">
         <f t="shared" si="47"/>
-        <v>Powder Keg (0)</v>
+        <v>Drum (p-Fluorobenzoyl Chloride)</v>
       </c>
       <c r="I386" s="16" t="str">
         <f t="shared" si="48"/>
-        <v>Chemical Silo (0)</v>
-      </c>
-      <c r="J386" s="16">
+        <v>Chemical Vat (p-Fluorobenzoyl Chloride)</v>
+      </c>
+      <c r="J386" s="16" t="str">
         <f>[1]Compounds!$B394</f>
-        <v>0</v>
-      </c>
-      <c r="K386">
+        <v>p-Fluorobenzoyl Chloride</v>
+      </c>
+      <c r="K386" t="str">
         <f>[1]Compounds!$D394</f>
-        <v>0</v>
+        <v>Liquid</v>
       </c>
       <c r="L386" s="4" t="str">
         <f>IF(K386=[1]Enums!$A$20, [1]Enums!$A$25, IF(K386=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
-        <v>Bag</v>
+        <v>Vial</v>
       </c>
       <c r="M386" s="4" t="str">
         <f>IF(K386=[1]Enums!$A$20, [1]Enums!$A$28, IF(K386=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
-        <v>Sack</v>
+        <v>Beaker</v>
       </c>
       <c r="N386" s="4" t="str">
         <f>IF(K386=[1]Enums!$A$20, [1]Enums!$A$31, IF(K386=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
-        <v>Powder Keg</v>
+        <v>Drum</v>
       </c>
       <c r="O386" s="4" t="str">
         <f>IF(K386=[1]Enums!$A$20, [1]Enums!$A$34, IF(K386=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
-        <v>Chemical Silo</v>
-      </c>
-    </row>
-    <row r="387" spans="2:15" x14ac:dyDescent="0.2">
+        <v>Chemical Vat</v>
+      </c>
+    </row>
+    <row r="387" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A387" s="4" t="str">
+        <f>[1]Enums!$A$14</f>
+        <v>1.1.2</v>
+      </c>
       <c r="B387" s="13" t="s">
         <v>2278</v>
       </c>
@@ -48373,46 +48612,50 @@
       </c>
       <c r="F387" s="16" t="str">
         <f t="shared" si="45"/>
-        <v>Bag (0)</v>
+        <v>Vial (p-Nitrotoluene)</v>
       </c>
       <c r="G387" s="16" t="str">
         <f t="shared" si="46"/>
-        <v>Sack (0)</v>
+        <v>Beaker (p-Nitrotoluene)</v>
       </c>
       <c r="H387" s="16" t="str">
         <f t="shared" si="47"/>
-        <v>Powder Keg (0)</v>
+        <v>Drum (p-Nitrotoluene)</v>
       </c>
       <c r="I387" s="16" t="str">
         <f t="shared" si="48"/>
-        <v>Chemical Silo (0)</v>
-      </c>
-      <c r="J387" s="16">
+        <v>Chemical Vat (p-Nitrotoluene)</v>
+      </c>
+      <c r="J387" s="16" t="str">
         <f>[1]Compounds!$B395</f>
-        <v>0</v>
-      </c>
-      <c r="K387">
+        <v>p-Nitrotoluene</v>
+      </c>
+      <c r="K387" t="str">
         <f>[1]Compounds!$D395</f>
-        <v>0</v>
+        <v>Liquid</v>
       </c>
       <c r="L387" s="4" t="str">
         <f>IF(K387=[1]Enums!$A$20, [1]Enums!$A$25, IF(K387=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
-        <v>Bag</v>
+        <v>Vial</v>
       </c>
       <c r="M387" s="4" t="str">
         <f>IF(K387=[1]Enums!$A$20, [1]Enums!$A$28, IF(K387=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
-        <v>Sack</v>
+        <v>Beaker</v>
       </c>
       <c r="N387" s="4" t="str">
         <f>IF(K387=[1]Enums!$A$20, [1]Enums!$A$31, IF(K387=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
-        <v>Powder Keg</v>
+        <v>Drum</v>
       </c>
       <c r="O387" s="4" t="str">
         <f>IF(K387=[1]Enums!$A$20, [1]Enums!$A$34, IF(K387=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
-        <v>Chemical Silo</v>
-      </c>
-    </row>
-    <row r="388" spans="2:15" x14ac:dyDescent="0.2">
+        <v>Chemical Vat</v>
+      </c>
+    </row>
+    <row r="388" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A388" s="4" t="str">
+        <f>[1]Enums!$A$14</f>
+        <v>1.1.2</v>
+      </c>
       <c r="B388" s="13" t="s">
         <v>2274</v>
       </c>
@@ -48427,46 +48670,50 @@
       </c>
       <c r="F388" s="16" t="str">
         <f t="shared" si="45"/>
-        <v>Bag (0)</v>
+        <v>Vial (p-Aminotoluene)</v>
       </c>
       <c r="G388" s="16" t="str">
         <f t="shared" si="46"/>
-        <v>Sack (0)</v>
+        <v>Beaker (p-Aminotoluene)</v>
       </c>
       <c r="H388" s="16" t="str">
         <f t="shared" si="47"/>
-        <v>Powder Keg (0)</v>
+        <v>Drum (p-Aminotoluene)</v>
       </c>
       <c r="I388" s="16" t="str">
         <f t="shared" si="48"/>
-        <v>Chemical Silo (0)</v>
-      </c>
-      <c r="J388" s="16">
+        <v>Chemical Vat (p-Aminotoluene)</v>
+      </c>
+      <c r="J388" s="16" t="str">
         <f>[1]Compounds!$B396</f>
-        <v>0</v>
-      </c>
-      <c r="K388">
+        <v>p-Aminotoluene</v>
+      </c>
+      <c r="K388" t="str">
         <f>[1]Compounds!$D396</f>
-        <v>0</v>
+        <v>Liquid</v>
       </c>
       <c r="L388" s="4" t="str">
         <f>IF(K388=[1]Enums!$A$20, [1]Enums!$A$25, IF(K388=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
-        <v>Bag</v>
+        <v>Vial</v>
       </c>
       <c r="M388" s="4" t="str">
         <f>IF(K388=[1]Enums!$A$20, [1]Enums!$A$28, IF(K388=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
-        <v>Sack</v>
+        <v>Beaker</v>
       </c>
       <c r="N388" s="4" t="str">
         <f>IF(K388=[1]Enums!$A$20, [1]Enums!$A$31, IF(K388=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
-        <v>Powder Keg</v>
+        <v>Drum</v>
       </c>
       <c r="O388" s="4" t="str">
         <f>IF(K388=[1]Enums!$A$20, [1]Enums!$A$34, IF(K388=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
-        <v>Chemical Silo</v>
-      </c>
-    </row>
-    <row r="389" spans="2:15" x14ac:dyDescent="0.2">
+        <v>Chemical Vat</v>
+      </c>
+    </row>
+    <row r="389" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A389" s="4" t="str">
+        <f>[1]Enums!$A$14</f>
+        <v>1.1.2</v>
+      </c>
       <c r="B389" s="13" t="s">
         <v>2270</v>
       </c>
@@ -48481,84 +48728,590 @@
       </c>
       <c r="F389" s="16" t="str">
         <f t="shared" si="45"/>
-        <v>Bag (0)</v>
+        <v>Vial (p-Fluorotoluene)</v>
       </c>
       <c r="G389" s="16" t="str">
         <f t="shared" si="46"/>
-        <v>Sack (0)</v>
+        <v>Beaker (p-Fluorotoluene)</v>
       </c>
       <c r="H389" s="16" t="str">
         <f t="shared" si="47"/>
-        <v>Powder Keg (0)</v>
+        <v>Drum (p-Fluorotoluene)</v>
       </c>
       <c r="I389" s="16" t="str">
         <f t="shared" si="48"/>
-        <v>Chemical Silo (0)</v>
-      </c>
-      <c r="J389" s="16">
+        <v>Chemical Vat (p-Fluorotoluene)</v>
+      </c>
+      <c r="J389" s="16" t="str">
         <f>[1]Compounds!$B397</f>
-        <v>0</v>
-      </c>
-      <c r="K389">
+        <v>p-Fluorotoluene</v>
+      </c>
+      <c r="K389" t="str">
         <f>[1]Compounds!$D397</f>
-        <v>0</v>
+        <v>Liquid</v>
       </c>
       <c r="L389" s="4" t="str">
         <f>IF(K389=[1]Enums!$A$20, [1]Enums!$A$25, IF(K389=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
-        <v>Bag</v>
+        <v>Vial</v>
       </c>
       <c r="M389" s="4" t="str">
         <f>IF(K389=[1]Enums!$A$20, [1]Enums!$A$28, IF(K389=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
-        <v>Sack</v>
+        <v>Beaker</v>
       </c>
       <c r="N389" s="4" t="str">
         <f>IF(K389=[1]Enums!$A$20, [1]Enums!$A$31, IF(K389=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
-        <v>Powder Keg</v>
+        <v>Drum</v>
       </c>
       <c r="O389" s="4" t="str">
         <f>IF(K389=[1]Enums!$A$20, [1]Enums!$A$34, IF(K389=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
-        <v>Chemical Silo</v>
-      </c>
-    </row>
-    <row r="390" spans="2:15" x14ac:dyDescent="0.2">
+        <v>Chemical Vat</v>
+      </c>
+    </row>
+    <row r="390" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A390" s="4" t="str">
+        <f>[1]Enums!$A$14</f>
+        <v>1.1.2</v>
+      </c>
+      <c r="B390" s="13" t="s">
+        <v>2377</v>
+      </c>
+      <c r="C390" s="13" t="s">
+        <v>2376</v>
+      </c>
+      <c r="D390" s="13" t="s">
+        <v>2375</v>
+      </c>
+      <c r="E390" s="13" t="s">
+        <v>2374</v>
+      </c>
       <c r="F390" s="16" t="str">
         <f t="shared" si="45"/>
-        <v>Bag (0)</v>
+        <v>Vial (1-(Trichloromethyl)-4-Fluorobenzene)</v>
       </c>
       <c r="G390" s="16" t="str">
         <f t="shared" si="46"/>
-        <v>Sack (0)</v>
+        <v>Beaker (1-(Trichloromethyl)-4-Fluorobenzene)</v>
       </c>
       <c r="H390" s="16" t="str">
         <f t="shared" si="47"/>
-        <v>Powder Keg (0)</v>
+        <v>Drum (1-(Trichloromethyl)-4-Fluorobenzene)</v>
       </c>
       <c r="I390" s="16" t="str">
         <f t="shared" si="48"/>
-        <v>Chemical Silo (0)</v>
-      </c>
-      <c r="J390" s="16">
+        <v>Chemical Vat (1-(Trichloromethyl)-4-Fluorobenzene)</v>
+      </c>
+      <c r="J390" s="16" t="str">
         <f>[1]Compounds!$B398</f>
-        <v>0</v>
-      </c>
-      <c r="K390">
+        <v>1-(Trichloromethyl)-4-Fluorobenzene</v>
+      </c>
+      <c r="K390" t="str">
         <f>[1]Compounds!$D398</f>
-        <v>0</v>
+        <v>Liquid</v>
       </c>
       <c r="L390" s="4" t="str">
         <f>IF(K390=[1]Enums!$A$20, [1]Enums!$A$25, IF(K390=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
-        <v>Bag</v>
+        <v>Vial</v>
       </c>
       <c r="M390" s="4" t="str">
         <f>IF(K390=[1]Enums!$A$20, [1]Enums!$A$28, IF(K390=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
-        <v>Sack</v>
+        <v>Beaker</v>
       </c>
       <c r="N390" s="4" t="str">
         <f>IF(K390=[1]Enums!$A$20, [1]Enums!$A$31, IF(K390=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
-        <v>Powder Keg</v>
+        <v>Drum</v>
       </c>
       <c r="O390" s="4" t="str">
         <f>IF(K390=[1]Enums!$A$20, [1]Enums!$A$34, IF(K390=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
+        <v>Chemical Vat</v>
+      </c>
+    </row>
+    <row r="391" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A391" s="4" t="str">
+        <f>[1]Enums!$A$14</f>
+        <v>1.1.2</v>
+      </c>
+      <c r="B391" s="13" t="s">
+        <v>2373</v>
+      </c>
+      <c r="C391" s="13" t="s">
+        <v>2372</v>
+      </c>
+      <c r="D391" s="13" t="s">
+        <v>2371</v>
+      </c>
+      <c r="E391" s="13" t="s">
+        <v>2370</v>
+      </c>
+      <c r="F391" s="16" t="str">
+        <f t="shared" ref="F391:F399" si="49">L391&amp;" ("&amp;$J391&amp;")"</f>
+        <v>Vial (4,4-Difluorobenzophenone)</v>
+      </c>
+      <c r="G391" s="16" t="str">
+        <f t="shared" ref="G391:G399" si="50">M391&amp;" ("&amp;$J391&amp;")"</f>
+        <v>Beaker (4,4-Difluorobenzophenone)</v>
+      </c>
+      <c r="H391" s="16" t="str">
+        <f t="shared" ref="H391:H399" si="51">N391&amp;" ("&amp;$J391&amp;")"</f>
+        <v>Drum (4,4-Difluorobenzophenone)</v>
+      </c>
+      <c r="I391" s="16" t="str">
+        <f t="shared" ref="I391:I399" si="52">O391&amp;" ("&amp;$J391&amp;")"</f>
+        <v>Chemical Vat (4,4-Difluorobenzophenone)</v>
+      </c>
+      <c r="J391" s="16" t="str">
+        <f>[1]Compounds!$B399</f>
+        <v>4,4-Difluorobenzophenone</v>
+      </c>
+      <c r="K391" t="str">
+        <f>[1]Compounds!$D399</f>
+        <v>Liquid</v>
+      </c>
+      <c r="L391" s="4" t="str">
+        <f>IF(K391=[1]Enums!$A$20, [1]Enums!$A$25, IF(K391=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
+        <v>Vial</v>
+      </c>
+      <c r="M391" s="4" t="str">
+        <f>IF(K391=[1]Enums!$A$20, [1]Enums!$A$28, IF(K391=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
+        <v>Beaker</v>
+      </c>
+      <c r="N391" s="4" t="str">
+        <f>IF(K391=[1]Enums!$A$20, [1]Enums!$A$31, IF(K391=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <v>Drum</v>
+      </c>
+      <c r="O391" s="4" t="str">
+        <f>IF(K391=[1]Enums!$A$20, [1]Enums!$A$34, IF(K391=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
+        <v>Chemical Vat</v>
+      </c>
+    </row>
+    <row r="392" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B392" s="13" t="s">
+        <v>2369</v>
+      </c>
+      <c r="C392" s="13" t="s">
+        <v>2368</v>
+      </c>
+      <c r="D392" s="13" t="s">
+        <v>2367</v>
+      </c>
+      <c r="E392" s="13" t="s">
+        <v>2366</v>
+      </c>
+      <c r="F392" s="16" t="str">
+        <f t="shared" si="49"/>
+        <v>Bag (0)</v>
+      </c>
+      <c r="G392" s="16" t="str">
+        <f t="shared" si="50"/>
+        <v>Sack (0)</v>
+      </c>
+      <c r="H392" s="16" t="str">
+        <f t="shared" si="51"/>
+        <v>Powder Keg (0)</v>
+      </c>
+      <c r="I392" s="16" t="str">
+        <f t="shared" si="52"/>
+        <v>Chemical Silo (0)</v>
+      </c>
+      <c r="J392" s="16">
+        <f>[1]Compounds!$B400</f>
+        <v>0</v>
+      </c>
+      <c r="K392">
+        <f>[1]Compounds!$D400</f>
+        <v>0</v>
+      </c>
+      <c r="L392" s="4" t="str">
+        <f>IF(K392=[1]Enums!$A$20, [1]Enums!$A$25, IF(K392=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M392" s="4" t="str">
+        <f>IF(K392=[1]Enums!$A$20, [1]Enums!$A$28, IF(K392=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N392" s="4" t="str">
+        <f>IF(K392=[1]Enums!$A$20, [1]Enums!$A$31, IF(K392=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O392" s="4" t="str">
+        <f>IF(K392=[1]Enums!$A$20, [1]Enums!$A$34, IF(K392=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
+        <v>Chemical Silo</v>
+      </c>
+    </row>
+    <row r="393" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B393" s="13" t="s">
+        <v>2365</v>
+      </c>
+      <c r="C393" s="13" t="s">
+        <v>2364</v>
+      </c>
+      <c r="D393" s="13" t="s">
+        <v>2363</v>
+      </c>
+      <c r="E393" s="13" t="s">
+        <v>2362</v>
+      </c>
+      <c r="F393" s="16" t="str">
+        <f t="shared" si="49"/>
+        <v>Bag (0)</v>
+      </c>
+      <c r="G393" s="16" t="str">
+        <f t="shared" si="50"/>
+        <v>Sack (0)</v>
+      </c>
+      <c r="H393" s="16" t="str">
+        <f t="shared" si="51"/>
+        <v>Powder Keg (0)</v>
+      </c>
+      <c r="I393" s="16" t="str">
+        <f t="shared" si="52"/>
+        <v>Chemical Silo (0)</v>
+      </c>
+      <c r="J393" s="16">
+        <f>[1]Compounds!$B401</f>
+        <v>0</v>
+      </c>
+      <c r="K393">
+        <f>[1]Compounds!$D401</f>
+        <v>0</v>
+      </c>
+      <c r="L393" s="4" t="str">
+        <f>IF(K393=[1]Enums!$A$20, [1]Enums!$A$25, IF(K393=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M393" s="4" t="str">
+        <f>IF(K393=[1]Enums!$A$20, [1]Enums!$A$28, IF(K393=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N393" s="4" t="str">
+        <f>IF(K393=[1]Enums!$A$20, [1]Enums!$A$31, IF(K393=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O393" s="4" t="str">
+        <f>IF(K393=[1]Enums!$A$20, [1]Enums!$A$34, IF(K393=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
+        <v>Chemical Silo</v>
+      </c>
+    </row>
+    <row r="394" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B394" s="13" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C394" s="13" t="s">
+        <v>2360</v>
+      </c>
+      <c r="D394" s="13" t="s">
+        <v>2359</v>
+      </c>
+      <c r="E394" s="13" t="s">
+        <v>2358</v>
+      </c>
+      <c r="F394" s="16" t="str">
+        <f t="shared" si="49"/>
+        <v>Bag (0)</v>
+      </c>
+      <c r="G394" s="16" t="str">
+        <f t="shared" si="50"/>
+        <v>Sack (0)</v>
+      </c>
+      <c r="H394" s="16" t="str">
+        <f t="shared" si="51"/>
+        <v>Powder Keg (0)</v>
+      </c>
+      <c r="I394" s="16" t="str">
+        <f t="shared" si="52"/>
+        <v>Chemical Silo (0)</v>
+      </c>
+      <c r="J394" s="16">
+        <f>[1]Compounds!$B402</f>
+        <v>0</v>
+      </c>
+      <c r="K394">
+        <f>[1]Compounds!$D402</f>
+        <v>0</v>
+      </c>
+      <c r="L394" s="4" t="str">
+        <f>IF(K394=[1]Enums!$A$20, [1]Enums!$A$25, IF(K394=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M394" s="4" t="str">
+        <f>IF(K394=[1]Enums!$A$20, [1]Enums!$A$28, IF(K394=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N394" s="4" t="str">
+        <f>IF(K394=[1]Enums!$A$20, [1]Enums!$A$31, IF(K394=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O394" s="4" t="str">
+        <f>IF(K394=[1]Enums!$A$20, [1]Enums!$A$34, IF(K394=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
+        <v>Chemical Silo</v>
+      </c>
+    </row>
+    <row r="395" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B395" s="13" t="s">
+        <v>2357</v>
+      </c>
+      <c r="C395" s="13" t="s">
+        <v>2356</v>
+      </c>
+      <c r="D395" s="13" t="s">
+        <v>2355</v>
+      </c>
+      <c r="E395" s="13" t="s">
+        <v>2354</v>
+      </c>
+      <c r="F395" s="16" t="str">
+        <f t="shared" si="49"/>
+        <v>Bag (0)</v>
+      </c>
+      <c r="G395" s="16" t="str">
+        <f t="shared" si="50"/>
+        <v>Sack (0)</v>
+      </c>
+      <c r="H395" s="16" t="str">
+        <f t="shared" si="51"/>
+        <v>Powder Keg (0)</v>
+      </c>
+      <c r="I395" s="16" t="str">
+        <f t="shared" si="52"/>
+        <v>Chemical Silo (0)</v>
+      </c>
+      <c r="J395" s="16">
+        <f>[1]Compounds!$B403</f>
+        <v>0</v>
+      </c>
+      <c r="K395">
+        <f>[1]Compounds!$D403</f>
+        <v>0</v>
+      </c>
+      <c r="L395" s="4" t="str">
+        <f>IF(K395=[1]Enums!$A$20, [1]Enums!$A$25, IF(K395=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M395" s="4" t="str">
+        <f>IF(K395=[1]Enums!$A$20, [1]Enums!$A$28, IF(K395=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N395" s="4" t="str">
+        <f>IF(K395=[1]Enums!$A$20, [1]Enums!$A$31, IF(K395=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O395" s="4" t="str">
+        <f>IF(K395=[1]Enums!$A$20, [1]Enums!$A$34, IF(K395=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
+        <v>Chemical Silo</v>
+      </c>
+    </row>
+    <row r="396" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B396" s="13" t="s">
+        <v>2353</v>
+      </c>
+      <c r="C396" s="13" t="s">
+        <v>2352</v>
+      </c>
+      <c r="D396" s="13" t="s">
+        <v>2351</v>
+      </c>
+      <c r="E396" s="13" t="s">
+        <v>2350</v>
+      </c>
+      <c r="F396" s="16" t="str">
+        <f t="shared" si="49"/>
+        <v>Bag (0)</v>
+      </c>
+      <c r="G396" s="16" t="str">
+        <f t="shared" si="50"/>
+        <v>Sack (0)</v>
+      </c>
+      <c r="H396" s="16" t="str">
+        <f t="shared" si="51"/>
+        <v>Powder Keg (0)</v>
+      </c>
+      <c r="I396" s="16" t="str">
+        <f t="shared" si="52"/>
+        <v>Chemical Silo (0)</v>
+      </c>
+      <c r="J396" s="16">
+        <f>[1]Compounds!$B404</f>
+        <v>0</v>
+      </c>
+      <c r="K396">
+        <f>[1]Compounds!$D404</f>
+        <v>0</v>
+      </c>
+      <c r="L396" s="4" t="str">
+        <f>IF(K396=[1]Enums!$A$20, [1]Enums!$A$25, IF(K396=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M396" s="4" t="str">
+        <f>IF(K396=[1]Enums!$A$20, [1]Enums!$A$28, IF(K396=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N396" s="4" t="str">
+        <f>IF(K396=[1]Enums!$A$20, [1]Enums!$A$31, IF(K396=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O396" s="4" t="str">
+        <f>IF(K396=[1]Enums!$A$20, [1]Enums!$A$34, IF(K396=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
+        <v>Chemical Silo</v>
+      </c>
+    </row>
+    <row r="397" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B397" s="13" t="s">
+        <v>2349</v>
+      </c>
+      <c r="C397" s="13" t="s">
+        <v>2348</v>
+      </c>
+      <c r="D397" s="13" t="s">
+        <v>2347</v>
+      </c>
+      <c r="E397" s="13" t="s">
+        <v>2346</v>
+      </c>
+      <c r="F397" s="16" t="str">
+        <f t="shared" si="49"/>
+        <v>Bag (0)</v>
+      </c>
+      <c r="G397" s="16" t="str">
+        <f t="shared" si="50"/>
+        <v>Sack (0)</v>
+      </c>
+      <c r="H397" s="16" t="str">
+        <f t="shared" si="51"/>
+        <v>Powder Keg (0)</v>
+      </c>
+      <c r="I397" s="16" t="str">
+        <f t="shared" si="52"/>
+        <v>Chemical Silo (0)</v>
+      </c>
+      <c r="J397" s="16">
+        <f>[1]Compounds!$B405</f>
+        <v>0</v>
+      </c>
+      <c r="K397">
+        <f>[1]Compounds!$D405</f>
+        <v>0</v>
+      </c>
+      <c r="L397" s="4" t="str">
+        <f>IF(K397=[1]Enums!$A$20, [1]Enums!$A$25, IF(K397=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M397" s="4" t="str">
+        <f>IF(K397=[1]Enums!$A$20, [1]Enums!$A$28, IF(K397=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N397" s="4" t="str">
+        <f>IF(K397=[1]Enums!$A$20, [1]Enums!$A$31, IF(K397=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O397" s="4" t="str">
+        <f>IF(K397=[1]Enums!$A$20, [1]Enums!$A$34, IF(K397=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
+        <v>Chemical Silo</v>
+      </c>
+    </row>
+    <row r="398" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B398" s="13" t="s">
+        <v>2345</v>
+      </c>
+      <c r="C398" s="13" t="s">
+        <v>2344</v>
+      </c>
+      <c r="D398" s="13" t="s">
+        <v>2343</v>
+      </c>
+      <c r="E398" s="13" t="s">
+        <v>2342</v>
+      </c>
+      <c r="F398" s="16" t="str">
+        <f t="shared" si="49"/>
+        <v>Bag (0)</v>
+      </c>
+      <c r="G398" s="16" t="str">
+        <f t="shared" si="50"/>
+        <v>Sack (0)</v>
+      </c>
+      <c r="H398" s="16" t="str">
+        <f t="shared" si="51"/>
+        <v>Powder Keg (0)</v>
+      </c>
+      <c r="I398" s="16" t="str">
+        <f t="shared" si="52"/>
+        <v>Chemical Silo (0)</v>
+      </c>
+      <c r="J398" s="16">
+        <f>[1]Compounds!$B406</f>
+        <v>0</v>
+      </c>
+      <c r="K398">
+        <f>[1]Compounds!$D406</f>
+        <v>0</v>
+      </c>
+      <c r="L398" s="4" t="str">
+        <f>IF(K398=[1]Enums!$A$20, [1]Enums!$A$25, IF(K398=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M398" s="4" t="str">
+        <f>IF(K398=[1]Enums!$A$20, [1]Enums!$A$28, IF(K398=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N398" s="4" t="str">
+        <f>IF(K398=[1]Enums!$A$20, [1]Enums!$A$31, IF(K398=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O398" s="4" t="str">
+        <f>IF(K398=[1]Enums!$A$20, [1]Enums!$A$34, IF(K398=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
+        <v>Chemical Silo</v>
+      </c>
+    </row>
+    <row r="399" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B399" s="13" t="s">
+        <v>2341</v>
+      </c>
+      <c r="C399" s="13" t="s">
+        <v>2340</v>
+      </c>
+      <c r="D399" s="13" t="s">
+        <v>2339</v>
+      </c>
+      <c r="E399" s="13" t="s">
+        <v>2338</v>
+      </c>
+      <c r="F399" s="16" t="str">
+        <f t="shared" si="49"/>
+        <v>Bag (0)</v>
+      </c>
+      <c r="G399" s="16" t="str">
+        <f t="shared" si="50"/>
+        <v>Sack (0)</v>
+      </c>
+      <c r="H399" s="16" t="str">
+        <f t="shared" si="51"/>
+        <v>Powder Keg (0)</v>
+      </c>
+      <c r="I399" s="16" t="str">
+        <f t="shared" si="52"/>
+        <v>Chemical Silo (0)</v>
+      </c>
+      <c r="J399" s="16">
+        <f>[1]Compounds!$B407</f>
+        <v>0</v>
+      </c>
+      <c r="K399">
+        <f>[1]Compounds!$D407</f>
+        <v>0</v>
+      </c>
+      <c r="L399" s="4" t="str">
+        <f>IF(K399=[1]Enums!$A$20, [1]Enums!$A$25, IF(K399=[1]Enums!$B$24, [1]Enums!$A$24, [1]Enums!$A$23))</f>
+        <v>Bag</v>
+      </c>
+      <c r="M399" s="4" t="str">
+        <f>IF(K399=[1]Enums!$A$20, [1]Enums!$A$28, IF(K399=[1]Enums!$B$27, [1]Enums!$A$27, [1]Enums!$A$26))</f>
+        <v>Sack</v>
+      </c>
+      <c r="N399" s="4" t="str">
+        <f>IF(K399=[1]Enums!$A$20, [1]Enums!$A$31, IF(K399=[1]Enums!$B$24, [1]Enums!$A$30, [1]Enums!$A$29))</f>
+        <v>Powder Keg</v>
+      </c>
+      <c r="O399" s="4" t="str">
+        <f>IF(K399=[1]Enums!$A$20, [1]Enums!$A$34, IF(K399=[1]Enums!$B$24, [1]Enums!$A$33, [1]Enums!$A$32))</f>
         <v>Chemical Silo</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Build Version 1.2.3 with updated Lights and Oilfield Texture
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="71445" yWindow="495" windowWidth="19200" windowHeight="19455" tabRatio="877"/>
+    <workbookView xWindow="72375" yWindow="495" windowWidth="19200" windowHeight="19455" tabRatio="877" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Custom Objects" sheetId="41" r:id="rId1"/>
@@ -7754,8 +7754,19 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Minecraft Item</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="3">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Minecraft Block</v>
+          </cell>
+        </row>
         <row r="22">
           <cell r="A22" t="str">
             <v>1.0.0</v>
@@ -13201,8 +13212,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -13500,7 +13511,7 @@
   </sheetPr>
   <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -15264,7 +15275,7 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Moved cleanroom to its own class; minor tweaks and bug fixes
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="877" activeTab="1"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="877"/>
   </bookViews>
   <sheets>
     <sheet name="Custom Objects" sheetId="41" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2475" uniqueCount="2430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2477" uniqueCount="2432">
   <si>
     <t>Ore</t>
   </si>
@@ -7259,9 +7259,6 @@
     <t>Bars (Copper)</t>
   </si>
   <si>
-    <t>Loads (Copper)</t>
-  </si>
-  <si>
     <t>1eP</t>
   </si>
   <si>
@@ -7326,6 +7323,15 @@
   </si>
   <si>
     <t>SpeechDistance</t>
+  </si>
+  <si>
+    <t>1eq</t>
+  </si>
+  <si>
+    <t>Smart Phone</t>
+  </si>
+  <si>
+    <t>Stacks (Copper)</t>
   </si>
 </sst>
 </file>
@@ -13694,10 +13700,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:S75"/>
+  <dimension ref="A1:S76"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="H87" sqref="H87"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15789,7 +15795,7 @@
         <v>1.3.2</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
       <c r="C66" s="26" t="s">
         <v>2405</v>
@@ -15816,7 +15822,7 @@
         <v>1.3.2</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>2409</v>
+        <v>2408</v>
       </c>
       <c r="C67" s="26" t="s">
         <v>2406</v>
@@ -15843,10 +15849,10 @@
         <v>1.3.2</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>2408</v>
+        <v>2407</v>
       </c>
       <c r="C68" s="26" t="s">
-        <v>2407</v>
+        <v>2431</v>
       </c>
       <c r="D68" s="28" t="str">
         <f>[1]Enums!$A$52</f>
@@ -15870,10 +15876,10 @@
         <v>1.3.2</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
       <c r="C69" s="26" t="s">
-        <v>2411</v>
+        <v>2410</v>
       </c>
       <c r="D69" s="28" t="str">
         <f>[1]Enums!$A$49</f>
@@ -15897,10 +15903,10 @@
         <v>1.3.2</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="C70" s="26" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="D70" s="28" t="str">
         <f>[1]Enums!$A$49</f>
@@ -15924,10 +15930,10 @@
         <v>1.3.2</v>
       </c>
       <c r="B71" s="13" t="s">
+        <v>2422</v>
+      </c>
+      <c r="C71" s="26" t="s">
         <v>2423</v>
-      </c>
-      <c r="C71" s="26" t="s">
-        <v>2424</v>
       </c>
       <c r="D71" s="28" t="str">
         <f>[1]Enums!$A$49</f>
@@ -15945,7 +15951,7 @@
       </c>
       <c r="I71" s="28"/>
       <c r="J71" s="26" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="K71" s="26">
         <v>64</v>
@@ -15957,10 +15963,10 @@
         <v>1.3.2</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
       <c r="C72" s="26" t="s">
-        <v>2425</v>
+        <v>2424</v>
       </c>
       <c r="D72" s="28" t="str">
         <f>[1]Enums!$A$49</f>
@@ -15978,7 +15984,7 @@
       </c>
       <c r="I72" s="28"/>
       <c r="J72" s="26" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="K72" s="26">
         <v>128</v>
@@ -15990,10 +15996,10 @@
         <v>1.3.2</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>2421</v>
+        <v>2420</v>
       </c>
       <c r="C73" s="26" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
       <c r="D73" s="28" t="str">
         <f>[1]Enums!$A$49</f>
@@ -16011,7 +16017,7 @@
       </c>
       <c r="I73" s="28"/>
       <c r="J73" s="26" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="K73" s="26">
         <v>512</v>
@@ -16023,10 +16029,10 @@
         <v>1.3.2</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="C74" s="26" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
       <c r="D74" s="28" t="str">
         <f>[1]Enums!$A$49</f>
@@ -16042,7 +16048,7 @@
         <v>1</v>
       </c>
       <c r="J74" s="26" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="K74" s="26">
         <v>512</v>
@@ -16054,10 +16060,10 @@
         <v>1.3.2</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>2419</v>
+        <v>2418</v>
       </c>
       <c r="C75" s="26" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
       <c r="D75" s="28" t="str">
         <f>[1]Enums!$A$49</f>
@@ -16070,6 +16076,31 @@
         <v>0</v>
       </c>
       <c r="H75" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A76" s="29" t="str">
+        <f>[1]Enums!$A$21</f>
+        <v>1.3.2</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>2429</v>
+      </c>
+      <c r="C76" s="26" t="s">
+        <v>2430</v>
+      </c>
+      <c r="D76" s="28" t="str">
+        <f>[1]Enums!$A$49</f>
+        <v>PC Item</v>
+      </c>
+      <c r="E76" s="26">
+        <v>8</v>
+      </c>
+      <c r="F76" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H76" s="26">
         <v>1</v>
       </c>
     </row>
@@ -16085,7 +16116,7 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -16253,7 +16284,7 @@
   <dimension ref="A1:R120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="J20" sqref="J20:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17666,7 +17697,7 @@
         <v>1.3.2</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>2415</v>
+        <v>2414</v>
       </c>
       <c r="C27" t="str">
         <f xml:space="preserve"> E27</f>
@@ -18827,10 +18858,10 @@
         <v>1.3.2</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>2417</v>
+        <v>2416</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>2416</v>
+        <v>2415</v>
       </c>
       <c r="D27" t="str">
         <f>[1]Minerals!$B$1</f>
@@ -19500,7 +19531,7 @@
         <v>1.3.2</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
       <c r="C30" t="str">
         <f>"Block of "&amp;Ingots!E27</f>

</xml_diff>

<commit_message>
Update to fewer items for serverside compatibility
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="877" activeTab="2"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="877" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Custom Objects" sheetId="41" r:id="rId1"/>
@@ -19516,7 +19516,7 @@
   </sheetPr>
   <dimension ref="A1:R120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -31513,8 +31513,8 @@
   </sheetPr>
   <dimension ref="A1:O399"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A234" sqref="A234"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -31523,7 +31523,7 @@
     <col min="3" max="3" width="3.7109375" customWidth="1"/>
     <col min="4" max="4" width="4.28515625" customWidth="1"/>
     <col min="5" max="5" width="4.140625" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="16" customWidth="1"/>
     <col min="7" max="7" width="6.7109375" style="16" customWidth="1"/>
     <col min="8" max="8" width="6.85546875" style="16" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" style="16" customWidth="1"/>

</xml_diff>

<commit_message>
Fixed recipe issues and tree tap not dropping its items upon destroy
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="877" activeTab="6"/>
+    <workbookView xWindow="13020" yWindow="0" windowWidth="20670" windowHeight="10035" tabRatio="877" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Custom Objects" sheetId="41" r:id="rId1"/>
@@ -49930,8 +49930,8 @@
   </sheetPr>
   <dimension ref="A1:R120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -53768,8 +53768,8 @@
   </sheetPr>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated version number to 1.4.4
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15810" yWindow="0" windowWidth="6450" windowHeight="9045" tabRatio="877" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="15810" yWindow="0" windowWidth="6450" windowHeight="9045" tabRatio="877" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Custom Objects" sheetId="41" r:id="rId1"/>
@@ -14098,8 +14098,8 @@
   </sheetPr>
   <dimension ref="A1:S80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="E60" workbookViewId="0">
+      <selection activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -24018,8 +24018,8 @@
   </sheetPr>
   <dimension ref="A1:O399"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="Q101" sqref="Q101"/>
+    <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
+      <selection activeCell="B244" sqref="B244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -52577,7 +52577,7 @@
   </sheetPr>
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Beginning of work on computer GUI
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15810" yWindow="0" windowWidth="6450" windowHeight="9045" tabRatio="877" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="15810" yWindow="0" windowWidth="6450" windowHeight="9045" tabRatio="877" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Custom Objects" sheetId="41" r:id="rId1"/>
@@ -24018,8 +24018,8 @@
   </sheetPr>
   <dimension ref="A1:O399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
-      <selection activeCell="B244" sqref="B244"/>
+    <sheetView topLeftCell="A324" workbookViewId="0">
+      <selection activeCell="J235" sqref="J235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -46692,7 +46692,7 @@
   </sheetPr>
   <dimension ref="A1:D334"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E141" sqref="E141"/>
     </sheetView>

</xml_diff>

<commit_message>
Added DevTool, needs work
Added ChallengeBlock, unimplemented

Added Dev Commands and Shematics
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Debra\Desktop\PolyCraftForge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195B9431-EA04-466D-B77E-A7763E50D43E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C40BE9-207E-4D2F-A909-7FB191859342}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17112" yWindow="0" windowWidth="6456" windowHeight="9048" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2609" uniqueCount="2557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2617" uniqueCount="2561">
   <si>
     <t>Ore</t>
   </si>
@@ -7713,6 +7713,18 @@
   </si>
   <si>
     <t>1hX</t>
+  </si>
+  <si>
+    <t>1hn</t>
+  </si>
+  <si>
+    <t>Dev Tool</t>
+  </si>
+  <si>
+    <t>1ho</t>
+  </si>
+  <si>
+    <t>Challenge Block</t>
   </si>
 </sst>
 </file>
@@ -14143,10 +14155,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:S83"/>
+  <dimension ref="A1:S85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="I85" sqref="I85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -16723,6 +16735,46 @@
       </c>
       <c r="K83" s="26" t="s">
         <v>2556</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="27" t="s">
+        <v>2549</v>
+      </c>
+      <c r="B84" s="26" t="s">
+        <v>2557</v>
+      </c>
+      <c r="C84" s="26" t="s">
+        <v>2558</v>
+      </c>
+      <c r="D84" s="26" t="s">
+        <v>1963</v>
+      </c>
+      <c r="F84" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H84" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" s="27" t="s">
+        <v>2549</v>
+      </c>
+      <c r="B85" s="26" t="s">
+        <v>2559</v>
+      </c>
+      <c r="C85" s="26" t="s">
+        <v>2560</v>
+      </c>
+      <c r="D85" s="26" t="s">
+        <v>2554</v>
+      </c>
+      <c r="F85" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H85" s="26">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed GameBlock and cleaned KillWall
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Debra\Desktop\PolyCraftForge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E76283-42F8-4F8D-B898-5801A526C715}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59E04A9-B292-4482-95BA-019D8A37D091}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17112" yWindow="0" windowWidth="6456" windowHeight="9048" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2607" uniqueCount="2554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2603" uniqueCount="2552">
   <si>
     <t>Ore</t>
   </si>
@@ -7698,12 +7698,6 @@
   </si>
   <si>
     <t>Oil Slime Ball</t>
-  </si>
-  <si>
-    <t>1hA</t>
-  </si>
-  <si>
-    <t>Game Block</t>
   </si>
 </sst>
 </file>
@@ -14134,10 +14128,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:S83"/>
+  <dimension ref="A1:S82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="I83" sqref="I83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C82" sqref="A1:S82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -16688,26 +16682,6 @@
       </c>
       <c r="H82" s="26">
         <v>64</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="27" t="s">
-        <v>2549</v>
-      </c>
-      <c r="B83" s="26" t="s">
-        <v>2552</v>
-      </c>
-      <c r="C83" s="26" t="s">
-        <v>2553</v>
-      </c>
-      <c r="D83" s="26" t="s">
-        <v>1963</v>
-      </c>
-      <c r="F83" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="H83" s="26">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
now Can only get Dev Tool with Command /dev tool
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Debra\Desktop\PolyCraftForge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59E04A9-B292-4482-95BA-019D8A37D091}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6605CEF-8106-41BA-8910-EDAC61FD86FA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17112" yWindow="0" windowWidth="6456" windowHeight="9048" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,11 +38,18 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="179021" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2603" uniqueCount="2552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2775" uniqueCount="2576">
   <si>
     <t>Ore</t>
   </si>
@@ -7698,6 +7705,78 @@
   </si>
   <si>
     <t>Oil Slime Ball</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>1.1.0</t>
+  </si>
+  <si>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>1.0.3</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
+  </si>
+  <si>
+    <t>1.2.3</t>
+  </si>
+  <si>
+    <t>1.3.2</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>1.3.5</t>
+  </si>
+  <si>
+    <t>1.3.6</t>
+  </si>
+  <si>
+    <t>1.3.8</t>
+  </si>
+  <si>
+    <t>1hY</t>
+  </si>
+  <si>
+    <t>Password Door</t>
+  </si>
+  <si>
+    <t>PC Block</t>
+  </si>
+  <si>
+    <t>ItemID</t>
+  </si>
+  <si>
+    <t>1hX</t>
+  </si>
+  <si>
+    <t>1hn</t>
+  </si>
+  <si>
+    <t>Dev Tool</t>
+  </si>
+  <si>
+    <t>1ho</t>
+  </si>
+  <si>
+    <t>Challenge Block</t>
   </si>
 </sst>
 </file>
@@ -8202,36 +8281,6 @@
             <v>Chemical Tank</v>
           </cell>
         </row>
-        <row r="21">
-          <cell r="A21" t="str">
-            <v>Armor</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22" t="str">
-            <v>Weapon</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24" t="str">
-            <v>Tool</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26" t="str">
-            <v>PC Item</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28" t="str">
-            <v>Food</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29" t="str">
-            <v>Currency</v>
-          </cell>
-        </row>
         <row r="133">
           <cell r="A133" t="str">
             <v>Version</v>
@@ -8242,11 +8291,6 @@
             <v>1.0.0</v>
           </cell>
         </row>
-        <row r="137">
-          <cell r="A137" t="str">
-            <v>1.0.3</v>
-          </cell>
-        </row>
         <row r="138">
           <cell r="A138" t="str">
             <v>1.0.4</v>
@@ -8267,24 +8311,9 @@
             <v>1.1.2</v>
           </cell>
         </row>
-        <row r="149">
-          <cell r="A149" t="str">
-            <v>1.2.3</v>
-          </cell>
-        </row>
         <row r="153">
           <cell r="A153" t="str">
             <v>1.3.2</v>
-          </cell>
-        </row>
-        <row r="156">
-          <cell r="A156" t="str">
-            <v>1.3.5</v>
-          </cell>
-        </row>
-        <row r="157">
-          <cell r="A157" t="str">
-            <v>1.3.6</v>
           </cell>
         </row>
         <row r="159">
@@ -8306,13 +8335,7 @@
         </row>
       </sheetData>
       <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
-        <row r="22">
-          <cell r="A22" t="str">
-            <v>1.0.0</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="3"/>
       <sheetData sheetId="4">
         <row r="1">
           <cell r="B1" t="str">
@@ -14128,10 +14151,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:S82"/>
+  <dimension ref="A1:S85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C82" sqref="A1:S82"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -14152,13 +14175,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="str">
-        <f>[1]Enums!$A$133</f>
-        <v>Version</v>
-      </c>
-      <c r="B1" s="37" t="str">
-        <f xml:space="preserve"> '[1]Game IDs'!A1</f>
-        <v>Game ID</v>
+      <c r="A1" s="38" t="s">
+        <v>2552</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>2521</v>
       </c>
       <c r="C1" s="36" t="s">
         <v>2146</v>
@@ -14213,9 +14234,8 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A2" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>2027</v>
@@ -14223,9 +14243,8 @@
       <c r="C2" s="31" t="s">
         <v>2026</v>
       </c>
-      <c r="D2" s="32" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D2" s="32" t="s">
+        <v>1963</v>
       </c>
       <c r="E2" s="26">
         <v>2</v>
@@ -14238,9 +14257,8 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A3" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>2025</v>
@@ -14248,9 +14266,8 @@
       <c r="C3" s="32" t="s">
         <v>2024</v>
       </c>
-      <c r="D3" s="32" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D3" s="32" t="s">
+        <v>1963</v>
       </c>
       <c r="E3" s="32">
         <v>1</v>
@@ -14263,9 +14280,8 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A4" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B4" s="33" t="s">
         <v>2023</v>
@@ -14273,9 +14289,8 @@
       <c r="C4" s="34" t="s">
         <v>2153</v>
       </c>
-      <c r="D4" s="32" t="str">
-        <f>[1]Enums!$A$22</f>
-        <v>Weapon</v>
+      <c r="D4" s="32" t="s">
+        <v>2554</v>
       </c>
       <c r="E4" s="32">
         <v>7</v>
@@ -14309,9 +14324,8 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A5" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>2147</v>
@@ -14319,9 +14333,8 @@
       <c r="C5" s="34" t="s">
         <v>2154</v>
       </c>
-      <c r="D5" s="32" t="str">
-        <f>[1]Enums!$A$22</f>
-        <v>Weapon</v>
+      <c r="D5" s="32" t="s">
+        <v>2554</v>
       </c>
       <c r="E5" s="32">
         <v>7</v>
@@ -14358,9 +14371,8 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A6" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>2148</v>
@@ -14368,9 +14380,8 @@
       <c r="C6" s="34" t="s">
         <v>2155</v>
       </c>
-      <c r="D6" s="32" t="str">
-        <f>[1]Enums!$A$22</f>
-        <v>Weapon</v>
+      <c r="D6" s="32" t="s">
+        <v>2554</v>
       </c>
       <c r="E6" s="32">
         <v>7</v>
@@ -14407,9 +14418,8 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A7" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>2149</v>
@@ -14417,9 +14427,8 @@
       <c r="C7" s="34" t="s">
         <v>2022</v>
       </c>
-      <c r="D7" s="32" t="str">
-        <f>[1]Enums!$A$22</f>
-        <v>Weapon</v>
+      <c r="D7" s="32" t="s">
+        <v>2554</v>
       </c>
       <c r="E7" s="32">
         <v>7</v>
@@ -14456,9 +14465,8 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A8" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B8" s="33" t="s">
         <v>2020</v>
@@ -14466,9 +14474,8 @@
       <c r="C8" s="32" t="s">
         <v>2019</v>
       </c>
-      <c r="D8" s="32" t="str">
-        <f>[1]Enums!$A$24</f>
-        <v>Tool</v>
+      <c r="D8" s="32" t="s">
+        <v>2556</v>
       </c>
       <c r="E8" s="32"/>
       <c r="F8" s="26" t="b">
@@ -14482,9 +14489,8 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A9" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B9" s="33" t="s">
         <v>2018</v>
@@ -14492,9 +14498,8 @@
       <c r="C9" s="34" t="s">
         <v>2325</v>
       </c>
-      <c r="D9" s="32" t="str">
-        <f>[1]Enums!$A$21</f>
-        <v>Armor</v>
+      <c r="D9" s="32" t="s">
+        <v>2557</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="26" t="b">
@@ -14523,9 +14528,8 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A10" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>2017</v>
@@ -14533,9 +14537,8 @@
       <c r="C10" s="34" t="s">
         <v>2016</v>
       </c>
-      <c r="D10" s="32" t="str">
-        <f>[1]Enums!$A$24</f>
-        <v>Tool</v>
+      <c r="D10" s="32" t="s">
+        <v>2556</v>
       </c>
       <c r="E10" s="32"/>
       <c r="F10" s="26" t="b">
@@ -14552,9 +14555,8 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A11" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B11" s="33" t="s">
         <v>2014</v>
@@ -14562,9 +14564,8 @@
       <c r="C11" s="32" t="s">
         <v>2013</v>
       </c>
-      <c r="D11" s="32" t="str">
-        <f>[1]Enums!$A$24</f>
-        <v>Tool</v>
+      <c r="D11" s="32" t="s">
+        <v>2556</v>
       </c>
       <c r="E11" s="32"/>
       <c r="F11" s="26" t="b">
@@ -14575,9 +14576,8 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A12" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B12" s="33" t="s">
         <v>2012</v>
@@ -14585,9 +14585,8 @@
       <c r="C12" s="32" t="s">
         <v>2011</v>
       </c>
-      <c r="D12" s="32" t="str">
-        <f>[1]Enums!$A$24</f>
-        <v>Tool</v>
+      <c r="D12" s="32" t="s">
+        <v>2556</v>
       </c>
       <c r="E12" s="32">
         <v>7</v>
@@ -14607,15 +14606,13 @@
       <c r="L12" s="26">
         <v>0.6</v>
       </c>
-      <c r="M12" s="26" t="str">
-        <f>'[1]Blocks (MC)'!$A$22</f>
-        <v>1.0.0</v>
+      <c r="M12" s="26" t="s">
+        <v>2553</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A13" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B13" s="33" t="s">
         <v>2009</v>
@@ -14623,9 +14620,8 @@
       <c r="C13" s="32" t="s">
         <v>2163</v>
       </c>
-      <c r="D13" s="32" t="str">
-        <f>[1]Enums!$A$21</f>
-        <v>Armor</v>
+      <c r="D13" s="32" t="s">
+        <v>2557</v>
       </c>
       <c r="E13" s="32"/>
       <c r="F13" s="26" t="b">
@@ -14645,9 +14641,8 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A14" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>2160</v>
@@ -14655,9 +14650,8 @@
       <c r="C14" s="32" t="s">
         <v>2164</v>
       </c>
-      <c r="D14" s="32" t="str">
-        <f>[1]Enums!$A$21</f>
-        <v>Armor</v>
+      <c r="D14" s="32" t="s">
+        <v>2557</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="26" t="b">
@@ -14677,9 +14671,8 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A15" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>2161</v>
@@ -14687,9 +14680,8 @@
       <c r="C15" s="32" t="s">
         <v>2165</v>
       </c>
-      <c r="D15" s="32" t="str">
-        <f>[1]Enums!$A$21</f>
-        <v>Armor</v>
+      <c r="D15" s="32" t="s">
+        <v>2557</v>
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="26" t="b">
@@ -14709,9 +14701,8 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A16" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>2162</v>
@@ -14719,9 +14710,8 @@
       <c r="C16" s="32" t="s">
         <v>2166</v>
       </c>
-      <c r="D16" s="32" t="str">
-        <f>[1]Enums!$A$21</f>
-        <v>Armor</v>
+      <c r="D16" s="32" t="s">
+        <v>2557</v>
       </c>
       <c r="E16" s="32"/>
       <c r="F16" s="26" t="b">
@@ -14741,9 +14731,8 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A17" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B17" s="33" t="s">
         <v>2007</v>
@@ -14751,9 +14740,8 @@
       <c r="C17" s="32" t="s">
         <v>2006</v>
       </c>
-      <c r="D17" s="32" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D17" s="32" t="s">
+        <v>1963</v>
       </c>
       <c r="F17" s="26" t="b">
         <v>1</v>
@@ -14763,9 +14751,8 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A18" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B18" s="33" t="s">
         <v>2005</v>
@@ -14773,9 +14760,8 @@
       <c r="C18" s="34" t="s">
         <v>2004</v>
       </c>
-      <c r="D18" s="34" t="str">
-        <f>[1]Enums!$A$28</f>
-        <v>Food</v>
+      <c r="D18" s="34" t="s">
+        <v>2558</v>
       </c>
       <c r="F18" s="26" t="b">
         <v>1</v>
@@ -14785,9 +14771,8 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A19" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B19" s="33" t="s">
         <v>2003</v>
@@ -14795,9 +14780,8 @@
       <c r="C19" s="34" t="s">
         <v>2002</v>
       </c>
-      <c r="D19" s="34" t="str">
-        <f>[1]Enums!$A$28</f>
-        <v>Food</v>
+      <c r="D19" s="34" t="s">
+        <v>2558</v>
       </c>
       <c r="F19" s="26" t="b">
         <v>1</v>
@@ -14807,9 +14791,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A20" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B20" s="33" t="s">
         <v>2001</v>
@@ -14817,9 +14800,8 @@
       <c r="C20" s="28" t="s">
         <v>2380</v>
       </c>
-      <c r="D20" s="34" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D20" s="34" t="s">
+        <v>1963</v>
       </c>
       <c r="F20" s="26" t="b">
         <v>1</v>
@@ -14829,9 +14811,8 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A21" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B21" s="33" t="s">
         <v>2000</v>
@@ -14839,9 +14820,8 @@
       <c r="C21" s="28" t="s">
         <v>2156</v>
       </c>
-      <c r="D21" s="34" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D21" s="34" t="s">
+        <v>1963</v>
       </c>
       <c r="F21" s="26" t="b">
         <v>1</v>
@@ -14853,9 +14833,8 @@
       <c r="I21" s="28"/>
     </row>
     <row r="22" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A22" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>2150</v>
@@ -14863,9 +14842,8 @@
       <c r="C22" s="28" t="s">
         <v>2157</v>
       </c>
-      <c r="D22" s="34" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D22" s="34" t="s">
+        <v>1963</v>
       </c>
       <c r="F22" s="26" t="b">
         <v>0</v>
@@ -14877,9 +14855,8 @@
       <c r="I22" s="28"/>
     </row>
     <row r="23" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A23" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>2151</v>
@@ -14887,9 +14864,8 @@
       <c r="C23" s="28" t="s">
         <v>2158</v>
       </c>
-      <c r="D23" s="34" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D23" s="34" t="s">
+        <v>1963</v>
       </c>
       <c r="F23" s="26" t="b">
         <v>0</v>
@@ -14901,9 +14877,8 @@
       <c r="I23" s="28"/>
     </row>
     <row r="24" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A24" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>2152</v>
@@ -14911,9 +14886,8 @@
       <c r="C24" s="28" t="s">
         <v>2159</v>
       </c>
-      <c r="D24" s="34" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D24" s="34" t="s">
+        <v>1963</v>
       </c>
       <c r="F24" s="26" t="b">
         <v>0</v>
@@ -14925,9 +14899,8 @@
       <c r="I24" s="28"/>
     </row>
     <row r="25" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A25" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B25" s="33" t="s">
         <v>1999</v>
@@ -14935,9 +14908,8 @@
       <c r="C25" s="28" t="s">
         <v>1998</v>
       </c>
-      <c r="D25" s="28" t="str">
-        <f>[1]Enums!$A$24</f>
-        <v>Tool</v>
+      <c r="D25" s="28" t="s">
+        <v>2556</v>
       </c>
       <c r="E25" s="26">
         <v>4</v>
@@ -14950,9 +14922,8 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A26" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B26" s="33" t="s">
         <v>1997</v>
@@ -14960,9 +14931,8 @@
       <c r="C26" s="28" t="s">
         <v>1996</v>
       </c>
-      <c r="D26" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D26" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="F26" s="26" t="b">
         <v>1</v>
@@ -14972,9 +14942,8 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A27" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B27" s="33" t="s">
         <v>1995</v>
@@ -14982,9 +14951,8 @@
       <c r="C27" s="28" t="s">
         <v>1994</v>
       </c>
-      <c r="D27" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D27" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="F27" s="26" t="b">
         <v>1</v>
@@ -14994,9 +14962,8 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A28" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B28" s="33" t="s">
         <v>1993</v>
@@ -15004,9 +14971,8 @@
       <c r="C28" s="28" t="s">
         <v>1992</v>
       </c>
-      <c r="D28" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D28" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="F28" s="26" t="b">
         <v>1</v>
@@ -15016,9 +14982,8 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A29" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B29" s="33" t="s">
         <v>1991</v>
@@ -15026,9 +14991,8 @@
       <c r="C29" s="28" t="s">
         <v>1990</v>
       </c>
-      <c r="D29" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D29" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="F29" s="26" t="b">
         <v>1</v>
@@ -15044,9 +15008,8 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A30" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B30" s="33" t="s">
         <v>1988</v>
@@ -15054,9 +15017,8 @@
       <c r="C30" s="28" t="s">
         <v>1987</v>
       </c>
-      <c r="D30" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D30" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E30" s="26">
         <v>4</v>
@@ -15069,9 +15031,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A31" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B31" s="13" t="s">
         <v>1986</v>
@@ -15079,9 +15040,8 @@
       <c r="C31" s="26" t="s">
         <v>1985</v>
       </c>
-      <c r="D31" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D31" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E31" s="28"/>
       <c r="F31" s="28" t="b">
@@ -15092,9 +15052,8 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A32" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A32" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B32" s="13" t="s">
         <v>1984</v>
@@ -15102,9 +15061,8 @@
       <c r="C32" s="26" t="s">
         <v>1983</v>
       </c>
-      <c r="D32" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D32" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="F32" s="26" t="b">
         <v>1</v>
@@ -15114,9 +15072,8 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A33" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A33" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B33" s="13" t="s">
         <v>1982</v>
@@ -15124,9 +15081,8 @@
       <c r="C33" s="26" t="s">
         <v>1981</v>
       </c>
-      <c r="D33" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D33" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E33" s="26">
         <v>4</v>
@@ -15139,9 +15095,8 @@
       </c>
     </row>
     <row r="34" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A34" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>1980</v>
@@ -15149,9 +15104,8 @@
       <c r="C34" s="26" t="s">
         <v>1979</v>
       </c>
-      <c r="D34" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D34" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E34" s="26">
         <v>8</v>
@@ -15164,9 +15118,8 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="str">
-        <f>[1]Enums!$A$137</f>
-        <v>1.0.3</v>
+      <c r="A35" s="29" t="s">
+        <v>2559</v>
       </c>
       <c r="B35" s="13" t="s">
         <v>1978</v>
@@ -15174,9 +15127,8 @@
       <c r="C35" s="31" t="s">
         <v>1977</v>
       </c>
-      <c r="D35" s="28" t="str">
-        <f>[1]Enums!$A$24</f>
-        <v>Tool</v>
+      <c r="D35" s="28" t="s">
+        <v>2556</v>
       </c>
       <c r="E35" s="26">
         <v>4</v>
@@ -15197,9 +15149,8 @@
       </c>
     </row>
     <row r="36" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A36" s="29" t="str">
-        <f>[1]Enums!$A$137</f>
-        <v>1.0.3</v>
+      <c r="A36" s="29" t="s">
+        <v>2559</v>
       </c>
       <c r="B36" s="13" t="s">
         <v>1976</v>
@@ -15207,9 +15158,8 @@
       <c r="C36" s="31" t="s">
         <v>1975</v>
       </c>
-      <c r="D36" s="28" t="str">
-        <f>[1]Enums!$A$24</f>
-        <v>Tool</v>
+      <c r="D36" s="28" t="s">
+        <v>2556</v>
       </c>
       <c r="E36" s="26">
         <v>4</v>
@@ -15230,9 +15180,8 @@
       </c>
     </row>
     <row r="37" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A37" s="29" t="str">
-        <f>[1]Enums!$A$137</f>
-        <v>1.0.3</v>
+      <c r="A37" s="29" t="s">
+        <v>2559</v>
       </c>
       <c r="B37" s="13" t="s">
         <v>1974</v>
@@ -15240,9 +15189,8 @@
       <c r="C37" s="31" t="s">
         <v>1973</v>
       </c>
-      <c r="D37" s="28" t="str">
-        <f>[1]Enums!$A$24</f>
-        <v>Tool</v>
+      <c r="D37" s="28" t="s">
+        <v>2556</v>
       </c>
       <c r="E37" s="26">
         <v>4</v>
@@ -15263,9 +15211,8 @@
       </c>
     </row>
     <row r="38" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A38" s="29" t="str">
-        <f>[1]Enums!$A$137</f>
-        <v>1.0.3</v>
+      <c r="A38" s="29" t="s">
+        <v>2559</v>
       </c>
       <c r="B38" s="13" t="s">
         <v>1972</v>
@@ -15273,9 +15220,8 @@
       <c r="C38" s="31" t="s">
         <v>1971</v>
       </c>
-      <c r="D38" s="28" t="str">
-        <f>[1]Enums!$A$24</f>
-        <v>Tool</v>
+      <c r="D38" s="28" t="s">
+        <v>2556</v>
       </c>
       <c r="E38" s="26">
         <v>4</v>
@@ -15296,9 +15242,8 @@
       </c>
     </row>
     <row r="39" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A39" s="29" t="str">
-        <f>[1]Enums!$A$137</f>
-        <v>1.0.3</v>
+      <c r="A39" s="29" t="s">
+        <v>2559</v>
       </c>
       <c r="B39" s="13" t="s">
         <v>1970</v>
@@ -15306,9 +15251,8 @@
       <c r="C39" s="31" t="s">
         <v>1969</v>
       </c>
-      <c r="D39" s="28" t="str">
-        <f>[1]Enums!$A$24</f>
-        <v>Tool</v>
+      <c r="D39" s="28" t="s">
+        <v>2556</v>
       </c>
       <c r="E39" s="26">
         <v>4</v>
@@ -15329,9 +15273,8 @@
       </c>
     </row>
     <row r="40" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A40" s="29" t="str">
-        <f>[1]Enums!$A$137</f>
-        <v>1.0.3</v>
+      <c r="A40" s="29" t="s">
+        <v>2559</v>
       </c>
       <c r="B40" s="13" t="s">
         <v>1968</v>
@@ -15339,9 +15282,8 @@
       <c r="C40" s="31" t="s">
         <v>1967</v>
       </c>
-      <c r="D40" s="28" t="str">
-        <f>[1]Enums!$A$24</f>
-        <v>Tool</v>
+      <c r="D40" s="28" t="s">
+        <v>2556</v>
       </c>
       <c r="E40" s="26">
         <v>4</v>
@@ -15362,9 +15304,8 @@
       </c>
     </row>
     <row r="41" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A41" s="29" t="str">
-        <f>[1]Enums!$A$137</f>
-        <v>1.0.3</v>
+      <c r="A41" s="29" t="s">
+        <v>2559</v>
       </c>
       <c r="B41" s="31" t="s">
         <v>1965</v>
@@ -15372,9 +15313,8 @@
       <c r="C41" s="31" t="s">
         <v>1964</v>
       </c>
-      <c r="D41" s="28" t="str">
-        <f>[1]Enums!$A$24</f>
-        <v>Tool</v>
+      <c r="D41" s="28" t="s">
+        <v>2556</v>
       </c>
       <c r="E41" s="26">
         <v>4</v>
@@ -15389,9 +15329,8 @@
       <c r="I41" s="28"/>
     </row>
     <row r="42" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A42" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A42" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B42" s="26" t="s">
         <v>1962</v>
@@ -15399,9 +15338,8 @@
       <c r="C42" s="31" t="s">
         <v>1961</v>
       </c>
-      <c r="D42" s="32" t="str">
-        <f>[1]Enums!$A$21</f>
-        <v>Armor</v>
+      <c r="D42" s="32" t="s">
+        <v>2557</v>
       </c>
       <c r="E42" s="26">
         <v>8</v>
@@ -15425,9 +15363,8 @@
       </c>
     </row>
     <row r="43" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A43" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A43" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B43" s="13" t="s">
         <v>2143</v>
@@ -15435,9 +15372,8 @@
       <c r="C43" s="28" t="s">
         <v>2133</v>
       </c>
-      <c r="D43" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D43" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E43" s="26">
         <v>8</v>
@@ -15452,9 +15388,8 @@
       <c r="I43" s="28"/>
     </row>
     <row r="44" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A44" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A44" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B44" s="13" t="s">
         <v>2142</v>
@@ -15462,9 +15397,8 @@
       <c r="C44" s="28" t="s">
         <v>2134</v>
       </c>
-      <c r="D44" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D44" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E44" s="26">
         <v>8</v>
@@ -15479,9 +15413,8 @@
       <c r="I44" s="28"/>
     </row>
     <row r="45" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A45" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A45" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B45" s="13" t="s">
         <v>2141</v>
@@ -15489,9 +15422,8 @@
       <c r="C45" s="28" t="s">
         <v>2135</v>
       </c>
-      <c r="D45" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D45" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E45" s="26">
         <v>8</v>
@@ -15506,9 +15438,8 @@
       <c r="I45" s="28"/>
     </row>
     <row r="46" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A46" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A46" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B46" s="13" t="s">
         <v>2140</v>
@@ -15516,9 +15447,8 @@
       <c r="C46" s="28" t="s">
         <v>2136</v>
       </c>
-      <c r="D46" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D46" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E46" s="26">
         <v>8</v>
@@ -15533,9 +15463,8 @@
       <c r="I46" s="28"/>
     </row>
     <row r="47" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A47" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A47" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B47" s="13" t="s">
         <v>2139</v>
@@ -15543,9 +15472,8 @@
       <c r="C47" s="26" t="s">
         <v>2137</v>
       </c>
-      <c r="D47" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D47" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E47" s="26">
         <v>8</v>
@@ -15560,9 +15488,8 @@
       <c r="I47" s="28"/>
     </row>
     <row r="48" spans="1:12" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A48" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A48" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B48" s="13" t="s">
         <v>2138</v>
@@ -15570,9 +15497,8 @@
       <c r="C48" s="26" t="s">
         <v>2145</v>
       </c>
-      <c r="D48" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D48" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E48" s="26">
         <v>8</v>
@@ -15587,9 +15513,8 @@
       <c r="I48" s="28"/>
     </row>
     <row r="49" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A49" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A49" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B49" s="13" t="s">
         <v>2173</v>
@@ -15597,9 +15522,8 @@
       <c r="C49" s="26" t="s">
         <v>2174</v>
       </c>
-      <c r="D49" s="32" t="str">
-        <f>[1]Enums!$A$21</f>
-        <v>Armor</v>
+      <c r="D49" s="32" t="s">
+        <v>2557</v>
       </c>
       <c r="E49" s="26">
         <v>8</v>
@@ -15618,9 +15542,8 @@
       <c r="K49" s="30"/>
     </row>
     <row r="50" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A50" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A50" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B50" s="13" t="s">
         <v>2172</v>
@@ -15628,9 +15551,8 @@
       <c r="C50" s="26" t="s">
         <v>2175</v>
       </c>
-      <c r="D50" s="32" t="str">
-        <f>[1]Enums!$A$21</f>
-        <v>Armor</v>
+      <c r="D50" s="32" t="s">
+        <v>2557</v>
       </c>
       <c r="E50" s="26">
         <v>8</v>
@@ -15649,9 +15571,8 @@
       <c r="K50" s="30"/>
     </row>
     <row r="51" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A51" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A51" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B51" s="13" t="s">
         <v>2171</v>
@@ -15659,9 +15580,8 @@
       <c r="C51" s="26" t="s">
         <v>2176</v>
       </c>
-      <c r="D51" s="32" t="str">
-        <f>[1]Enums!$A$21</f>
-        <v>Armor</v>
+      <c r="D51" s="32" t="s">
+        <v>2557</v>
       </c>
       <c r="E51" s="26">
         <v>8</v>
@@ -15680,9 +15600,8 @@
       <c r="K51" s="30"/>
     </row>
     <row r="52" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A52" s="29" t="str">
-        <f>[1]Enums!$A$144</f>
-        <v>1.1.0</v>
+      <c r="A52" s="29" t="s">
+        <v>2555</v>
       </c>
       <c r="B52" s="13" t="s">
         <v>2170</v>
@@ -15690,9 +15609,8 @@
       <c r="C52" s="26" t="s">
         <v>2177</v>
       </c>
-      <c r="D52" s="32" t="str">
-        <f>[1]Enums!$A$21</f>
-        <v>Armor</v>
+      <c r="D52" s="32" t="s">
+        <v>2557</v>
       </c>
       <c r="E52" s="26">
         <v>8</v>
@@ -15711,9 +15629,8 @@
       <c r="K52" s="30"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A53" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B53" s="13" t="s">
         <v>2331</v>
@@ -15721,9 +15638,8 @@
       <c r="C53" s="34" t="s">
         <v>2326</v>
       </c>
-      <c r="D53" s="32" t="str">
-        <f>[1]Enums!$A$21</f>
-        <v>Armor</v>
+      <c r="D53" s="32" t="s">
+        <v>2557</v>
       </c>
       <c r="E53" s="32">
         <v>8</v>
@@ -15754,9 +15670,8 @@
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A54" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B54" s="13" t="s">
         <v>2330</v>
@@ -15764,9 +15679,8 @@
       <c r="C54" s="34" t="s">
         <v>2327</v>
       </c>
-      <c r="D54" s="32" t="str">
-        <f>[1]Enums!$A$21</f>
-        <v>Armor</v>
+      <c r="D54" s="32" t="s">
+        <v>2557</v>
       </c>
       <c r="E54" s="32">
         <v>8</v>
@@ -15797,9 +15711,8 @@
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="29" t="str">
-        <f>[1]Enums!$A$134</f>
-        <v>1.0.0</v>
+      <c r="A55" s="29" t="s">
+        <v>2553</v>
       </c>
       <c r="B55" s="13" t="s">
         <v>2329</v>
@@ -15807,9 +15720,8 @@
       <c r="C55" s="34" t="s">
         <v>2328</v>
       </c>
-      <c r="D55" s="32" t="str">
-        <f>[1]Enums!$A$21</f>
-        <v>Armor</v>
+      <c r="D55" s="32" t="s">
+        <v>2557</v>
       </c>
       <c r="E55" s="32">
         <v>8</v>
@@ -15840,9 +15752,8 @@
       </c>
     </row>
     <row r="56" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A56" s="29" t="str">
-        <f>[1]Enums!$A$146</f>
-        <v>1.1.2</v>
+      <c r="A56" s="29" t="s">
+        <v>2560</v>
       </c>
       <c r="B56" s="13" t="s">
         <v>2375</v>
@@ -15850,9 +15761,8 @@
       <c r="C56" s="26" t="s">
         <v>2374</v>
       </c>
-      <c r="D56" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D56" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E56" s="26">
         <v>8</v>
@@ -15867,9 +15777,8 @@
       <c r="I56" s="28"/>
     </row>
     <row r="57" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A57" s="29" t="str">
-        <f>[1]Enums!$A$149</f>
-        <v>1.2.3</v>
+      <c r="A57" s="29" t="s">
+        <v>2561</v>
       </c>
       <c r="B57" s="13" t="s">
         <v>2398</v>
@@ -15877,9 +15786,8 @@
       <c r="C57" s="26" t="s">
         <v>2381</v>
       </c>
-      <c r="D57" s="32" t="str">
-        <f>[1]Enums!$A$22</f>
-        <v>Weapon</v>
+      <c r="D57" s="32" t="s">
+        <v>2554</v>
       </c>
       <c r="E57" s="26">
         <v>8</v>
@@ -15912,9 +15820,8 @@
       </c>
     </row>
     <row r="58" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A58" s="29" t="str">
-        <f>[1]Enums!$A$149</f>
-        <v>1.2.3</v>
+      <c r="A58" s="29" t="s">
+        <v>2561</v>
       </c>
       <c r="B58" s="13" t="s">
         <v>2397</v>
@@ -15922,9 +15829,8 @@
       <c r="C58" s="26" t="s">
         <v>2382</v>
       </c>
-      <c r="D58" s="32" t="str">
-        <f>[1]Enums!$A$22</f>
-        <v>Weapon</v>
+      <c r="D58" s="32" t="s">
+        <v>2554</v>
       </c>
       <c r="E58" s="26">
         <v>8</v>
@@ -15957,9 +15863,8 @@
       </c>
     </row>
     <row r="59" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A59" s="29" t="str">
-        <f>[1]Enums!$A$149</f>
-        <v>1.2.3</v>
+      <c r="A59" s="29" t="s">
+        <v>2561</v>
       </c>
       <c r="B59" s="13" t="s">
         <v>2396</v>
@@ -15967,9 +15872,8 @@
       <c r="C59" s="26" t="s">
         <v>2383</v>
       </c>
-      <c r="D59" s="32" t="str">
-        <f>[1]Enums!$A$22</f>
-        <v>Weapon</v>
+      <c r="D59" s="32" t="s">
+        <v>2554</v>
       </c>
       <c r="E59" s="26">
         <v>8</v>
@@ -16002,9 +15906,8 @@
       </c>
     </row>
     <row r="60" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A60" s="29" t="str">
-        <f>[1]Enums!$A$149</f>
-        <v>1.2.3</v>
+      <c r="A60" s="29" t="s">
+        <v>2561</v>
       </c>
       <c r="B60" s="13" t="s">
         <v>2395</v>
@@ -16012,9 +15915,8 @@
       <c r="C60" s="26" t="s">
         <v>2384</v>
       </c>
-      <c r="D60" s="32" t="str">
-        <f>[1]Enums!$A$22</f>
-        <v>Weapon</v>
+      <c r="D60" s="32" t="s">
+        <v>2554</v>
       </c>
       <c r="E60" s="26">
         <v>8</v>
@@ -16047,9 +15949,8 @@
       </c>
     </row>
     <row r="61" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A61" s="29" t="str">
-        <f>[1]Enums!$A$149</f>
-        <v>1.2.3</v>
+      <c r="A61" s="29" t="s">
+        <v>2561</v>
       </c>
       <c r="B61" s="13" t="s">
         <v>2394</v>
@@ -16057,9 +15958,8 @@
       <c r="C61" s="26" t="s">
         <v>2385</v>
       </c>
-      <c r="D61" s="32" t="str">
-        <f>[1]Enums!$A$22</f>
-        <v>Weapon</v>
+      <c r="D61" s="32" t="s">
+        <v>2554</v>
       </c>
       <c r="E61" s="26">
         <v>8</v>
@@ -16086,9 +15986,8 @@
       </c>
     </row>
     <row r="62" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A62" s="29" t="str">
-        <f>[1]Enums!$A$149</f>
-        <v>1.2.3</v>
+      <c r="A62" s="29" t="s">
+        <v>2561</v>
       </c>
       <c r="B62" s="13" t="s">
         <v>2393</v>
@@ -16096,9 +15995,8 @@
       <c r="C62" s="26" t="s">
         <v>2386</v>
       </c>
-      <c r="D62" s="32" t="str">
-        <f>[1]Enums!$A$22</f>
-        <v>Weapon</v>
+      <c r="D62" s="32" t="s">
+        <v>2554</v>
       </c>
       <c r="E62" s="26">
         <v>8</v>
@@ -16125,9 +16023,8 @@
       </c>
     </row>
     <row r="63" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A63" s="29" t="str">
-        <f>[1]Enums!$A$149</f>
-        <v>1.2.3</v>
+      <c r="A63" s="29" t="s">
+        <v>2561</v>
       </c>
       <c r="B63" s="13" t="s">
         <v>2392</v>
@@ -16135,9 +16032,8 @@
       <c r="C63" s="26" t="s">
         <v>2387</v>
       </c>
-      <c r="D63" s="32" t="str">
-        <f>[1]Enums!$A$22</f>
-        <v>Weapon</v>
+      <c r="D63" s="32" t="s">
+        <v>2554</v>
       </c>
       <c r="E63" s="26">
         <v>8</v>
@@ -16164,9 +16060,8 @@
       </c>
     </row>
     <row r="64" spans="1:15" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A64" s="29" t="str">
-        <f>[1]Enums!$A$149</f>
-        <v>1.2.3</v>
+      <c r="A64" s="29" t="s">
+        <v>2561</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>2391</v>
@@ -16174,9 +16069,8 @@
       <c r="C64" s="26" t="s">
         <v>2388</v>
       </c>
-      <c r="D64" s="32" t="str">
-        <f>[1]Enums!$A$22</f>
-        <v>Weapon</v>
+      <c r="D64" s="32" t="s">
+        <v>2554</v>
       </c>
       <c r="E64" s="26">
         <v>8</v>
@@ -16203,9 +16097,8 @@
       </c>
     </row>
     <row r="65" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A65" s="29" t="str">
-        <f>[1]Enums!$A$153</f>
-        <v>1.3.2</v>
+      <c r="A65" s="29" t="s">
+        <v>2562</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>2403</v>
@@ -16213,9 +16106,8 @@
       <c r="C65" s="26" t="s">
         <v>2404</v>
       </c>
-      <c r="D65" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D65" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E65" s="26">
         <v>4</v>
@@ -16230,9 +16122,8 @@
       <c r="I65" s="28"/>
     </row>
     <row r="66" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A66" s="29" t="str">
-        <f>[1]Enums!$A$153</f>
-        <v>1.3.2</v>
+      <c r="A66" s="29" t="s">
+        <v>2562</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>2409</v>
@@ -16240,9 +16131,8 @@
       <c r="C66" s="26" t="s">
         <v>2405</v>
       </c>
-      <c r="D66" s="28" t="str">
-        <f>[1]Enums!$A$29</f>
-        <v>Currency</v>
+      <c r="D66" s="28" t="s">
+        <v>2563</v>
       </c>
       <c r="E66" s="26">
         <v>2</v>
@@ -16257,9 +16147,8 @@
       <c r="I66" s="28"/>
     </row>
     <row r="67" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A67" s="29" t="str">
-        <f>[1]Enums!$A$153</f>
-        <v>1.3.2</v>
+      <c r="A67" s="29" t="s">
+        <v>2562</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>2408</v>
@@ -16267,9 +16156,8 @@
       <c r="C67" s="26" t="s">
         <v>2406</v>
       </c>
-      <c r="D67" s="28" t="str">
-        <f>[1]Enums!$A$29</f>
-        <v>Currency</v>
+      <c r="D67" s="28" t="s">
+        <v>2563</v>
       </c>
       <c r="E67" s="26">
         <v>2</v>
@@ -16284,9 +16172,8 @@
       <c r="I67" s="28"/>
     </row>
     <row r="68" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A68" s="29" t="str">
-        <f>[1]Enums!$A$153</f>
-        <v>1.3.2</v>
+      <c r="A68" s="29" t="s">
+        <v>2562</v>
       </c>
       <c r="B68" s="13" t="s">
         <v>2407</v>
@@ -16294,9 +16181,8 @@
       <c r="C68" s="26" t="s">
         <v>2431</v>
       </c>
-      <c r="D68" s="28" t="str">
-        <f>[1]Enums!$A$29</f>
-        <v>Currency</v>
+      <c r="D68" s="28" t="s">
+        <v>2563</v>
       </c>
       <c r="E68" s="26">
         <v>2</v>
@@ -16311,9 +16197,8 @@
       <c r="I68" s="28"/>
     </row>
     <row r="69" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A69" s="29" t="str">
-        <f>[1]Enums!$A$153</f>
-        <v>1.3.2</v>
+      <c r="A69" s="29" t="s">
+        <v>2562</v>
       </c>
       <c r="B69" s="13" t="s">
         <v>2412</v>
@@ -16321,9 +16206,8 @@
       <c r="C69" s="26" t="s">
         <v>2410</v>
       </c>
-      <c r="D69" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D69" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E69" s="26">
         <v>8</v>
@@ -16338,9 +16222,8 @@
       <c r="I69" s="28"/>
     </row>
     <row r="70" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A70" s="29" t="str">
-        <f>[1]Enums!$A$153</f>
-        <v>1.3.2</v>
+      <c r="A70" s="29" t="s">
+        <v>2562</v>
       </c>
       <c r="B70" s="13" t="s">
         <v>2411</v>
@@ -16348,9 +16231,8 @@
       <c r="C70" s="26" t="s">
         <v>2413</v>
       </c>
-      <c r="D70" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D70" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E70" s="26">
         <v>8</v>
@@ -16365,9 +16247,8 @@
       <c r="I70" s="28"/>
     </row>
     <row r="71" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A71" s="29" t="str">
-        <f>[1]Enums!$A$153</f>
-        <v>1.3.2</v>
+      <c r="A71" s="29" t="s">
+        <v>2562</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>2422</v>
@@ -16375,9 +16256,8 @@
       <c r="C71" s="26" t="s">
         <v>2423</v>
       </c>
-      <c r="D71" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D71" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E71" s="26">
         <v>2</v>
@@ -16398,9 +16278,8 @@
       </c>
     </row>
     <row r="72" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A72" s="29" t="str">
-        <f>[1]Enums!$A$153</f>
-        <v>1.3.2</v>
+      <c r="A72" s="29" t="s">
+        <v>2562</v>
       </c>
       <c r="B72" s="13" t="s">
         <v>2421</v>
@@ -16408,9 +16287,8 @@
       <c r="C72" s="26" t="s">
         <v>2424</v>
       </c>
-      <c r="D72" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D72" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E72" s="26">
         <v>4</v>
@@ -16431,9 +16309,8 @@
       </c>
     </row>
     <row r="73" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A73" s="29" t="str">
-        <f>[1]Enums!$A$153</f>
-        <v>1.3.2</v>
+      <c r="A73" s="29" t="s">
+        <v>2562</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>2420</v>
@@ -16441,9 +16318,8 @@
       <c r="C73" s="26" t="s">
         <v>2425</v>
       </c>
-      <c r="D73" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D73" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E73" s="26">
         <v>8</v>
@@ -16464,9 +16340,8 @@
       </c>
     </row>
     <row r="74" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A74" s="29" t="str">
-        <f>[1]Enums!$A$153</f>
-        <v>1.3.2</v>
+      <c r="A74" s="29" t="s">
+        <v>2562</v>
       </c>
       <c r="B74" s="13" t="s">
         <v>2419</v>
@@ -16474,9 +16349,8 @@
       <c r="C74" s="26" t="s">
         <v>2426</v>
       </c>
-      <c r="D74" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D74" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E74" s="26">
         <v>8</v>
@@ -16495,9 +16369,8 @@
       </c>
     </row>
     <row r="75" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A75" s="29" t="str">
-        <f>[1]Enums!$A$153</f>
-        <v>1.3.2</v>
+      <c r="A75" s="29" t="s">
+        <v>2562</v>
       </c>
       <c r="B75" s="13" t="s">
         <v>2418</v>
@@ -16505,9 +16378,8 @@
       <c r="C75" s="26" t="s">
         <v>2427</v>
       </c>
-      <c r="D75" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D75" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E75" s="26">
         <v>8</v>
@@ -16520,9 +16392,8 @@
       </c>
     </row>
     <row r="76" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A76" s="29" t="str">
-        <f>[1]Enums!$A$153</f>
-        <v>1.3.2</v>
+      <c r="A76" s="29" t="s">
+        <v>2562</v>
       </c>
       <c r="B76" s="13" t="s">
         <v>2429</v>
@@ -16530,9 +16401,8 @@
       <c r="C76" s="26" t="s">
         <v>2430</v>
       </c>
-      <c r="D76" s="28" t="str">
-        <f>[1]Enums!$A$26</f>
-        <v>PC Item</v>
+      <c r="D76" s="28" t="s">
+        <v>1963</v>
       </c>
       <c r="E76" s="26">
         <v>8</v>
@@ -16545,9 +16415,8 @@
       </c>
     </row>
     <row r="77" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A77" s="29" t="str">
-        <f>[1]Enums!$A$153</f>
-        <v>1.3.2</v>
+      <c r="A77" s="29" t="s">
+        <v>2562</v>
       </c>
       <c r="B77" s="13" t="s">
         <v>2399</v>
@@ -16555,9 +16424,8 @@
       <c r="C77" s="26" t="s">
         <v>2460</v>
       </c>
-      <c r="D77" s="28" t="str">
-        <f>[1]Enums!$A$29</f>
-        <v>Currency</v>
+      <c r="D77" s="28" t="s">
+        <v>2563</v>
       </c>
       <c r="E77" s="26">
         <v>2</v>
@@ -16570,9 +16438,8 @@
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="29" t="str">
-        <f>[1]Enums!$A$156</f>
-        <v>1.3.5</v>
+      <c r="A78" s="29" t="s">
+        <v>2564</v>
       </c>
       <c r="B78" s="13" t="s">
         <v>2462</v>
@@ -16594,9 +16461,8 @@
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" s="29" t="str">
-        <f>[1]Enums!$A$157</f>
-        <v>1.3.6</v>
+      <c r="A79" s="29" t="s">
+        <v>2565</v>
       </c>
       <c r="B79" s="13" t="s">
         <v>2464</v>
@@ -16618,9 +16484,8 @@
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="str">
-        <f>[1]Enums!$A$159</f>
-        <v>1.3.8</v>
+      <c r="A80" s="4" t="s">
+        <v>2566</v>
       </c>
       <c r="B80" s="13" t="s">
         <v>2496</v>
@@ -16641,7 +16506,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="27" t="s">
         <v>2546</v>
       </c>
@@ -16664,7 +16529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="27" t="s">
         <v>2549</v>
       </c>
@@ -16681,6 +16546,72 @@
         <v>0</v>
       </c>
       <c r="H82" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="27" t="s">
+        <v>2549</v>
+      </c>
+      <c r="B83" s="26" t="s">
+        <v>2567</v>
+      </c>
+      <c r="C83" s="26" t="s">
+        <v>2568</v>
+      </c>
+      <c r="D83" s="26" t="s">
+        <v>2569</v>
+      </c>
+      <c r="F83" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H83" s="26">
+        <v>64</v>
+      </c>
+      <c r="J83" s="26" t="s">
+        <v>2570</v>
+      </c>
+      <c r="K83" s="26" t="s">
+        <v>2571</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="27" t="s">
+        <v>2549</v>
+      </c>
+      <c r="B84" s="26" t="s">
+        <v>2572</v>
+      </c>
+      <c r="C84" s="26" t="s">
+        <v>2573</v>
+      </c>
+      <c r="D84" s="26" t="s">
+        <v>1963</v>
+      </c>
+      <c r="F84" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H84" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" s="27" t="s">
+        <v>2549</v>
+      </c>
+      <c r="B85" s="26" t="s">
+        <v>2574</v>
+      </c>
+      <c r="C85" s="26" t="s">
+        <v>2575</v>
+      </c>
+      <c r="D85" s="26" t="s">
+        <v>2569</v>
+      </c>
+      <c r="F85" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H85" s="26">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Raid Games Excel files
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Debra\Desktop\PolyCraftForge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6605CEF-8106-41BA-8910-EDAC61FD86FA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE150D5-3766-4C86-A184-E8B9878FF93F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17112" yWindow="0" windowWidth="6456" windowHeight="9048" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14153,7 +14153,7 @@
   </sheetPr>
   <dimension ref="A1:S85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
       <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changed text wall to inventory instead of custom object
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Polycraft\Documents\Polycraft Forge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7C77B1FE-6FF0-4602-BA90-1B66004C1758}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2F670B8F-E833-4FBC-AE1C-53290611334A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17115" yWindow="0" windowWidth="6450" windowHeight="9045" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2633" uniqueCount="2574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2630" uniqueCount="2572">
   <si>
     <t>Ore</t>
   </si>
@@ -7758,12 +7758,6 @@
   </si>
   <si>
     <t>Armor</t>
-  </si>
-  <si>
-    <t>1hy</t>
-  </si>
-  <si>
-    <t>TextWall</t>
   </si>
 </sst>
 </file>
@@ -14216,10 +14210,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:S92"/>
+  <dimension ref="A1:S91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="H92" sqref="H92"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B91" sqref="B89:B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16967,27 +16961,6 @@
       </c>
       <c r="H91" s="26">
         <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A92" s="4" t="str">
-        <f>[1]Enums!$A$169</f>
-        <v>1.4.10</v>
-      </c>
-      <c r="B92" s="13" t="s">
-        <v>2572</v>
-      </c>
-      <c r="C92" s="26" t="s">
-        <v>2573</v>
-      </c>
-      <c r="D92" s="26" t="s">
-        <v>1963</v>
-      </c>
-      <c r="F92" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="H92" s="26">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed Polycraft TextWallEntity Files & References
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Triforce\Documents\polycraftworld\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C93DB08E-EEB5-48FB-8749-A6BC09F89E02}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3A3E0FE8-D4C7-444A-BFD0-32F9E4E78E1D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17115" yWindow="0" windowWidth="6450" windowHeight="9045" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14212,8 +14212,8 @@
   </sheetPr>
   <dimension ref="A1:S91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="I82" sqref="I82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added HPBlock in Excel File
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2638" uniqueCount="2578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2642" uniqueCount="2581">
   <si>
     <t>Ore</t>
   </si>
@@ -7775,6 +7775,15 @@
   </si>
   <si>
     <t>Tool</t>
+  </si>
+  <si>
+    <t>1.4.13</t>
+  </si>
+  <si>
+    <t>1hH</t>
+  </si>
+  <si>
+    <t>HPBlock</t>
   </si>
 </sst>
 </file>
@@ -14197,10 +14206,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:S93"/>
+  <dimension ref="A1:S94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+      <selection activeCell="I94" sqref="I94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16988,6 +16997,26 @@
       </c>
       <c r="H93" s="43">
         <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A94" s="27" t="s">
+        <v>2578</v>
+      </c>
+      <c r="B94" s="26" t="s">
+        <v>2579</v>
+      </c>
+      <c r="C94" s="26" t="s">
+        <v>2580</v>
+      </c>
+      <c r="D94" s="26" t="s">
+        <v>2552</v>
+      </c>
+      <c r="F94" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H94" s="26">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HPBlock created. Has values, textures, and is editable by the physics experiment creator.
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjg150230\PolycraftForge\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DRZ170000\Desktop\polycraftforge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2642" uniqueCount="2581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2642" uniqueCount="2580">
   <si>
     <t>Ore</t>
   </si>
@@ -7775,9 +7775,6 @@
   </si>
   <si>
     <t>Tool</t>
-  </si>
-  <si>
-    <t>1.4.13</t>
   </si>
   <si>
     <t>1hH</t>
@@ -14208,8 +14205,8 @@
   </sheetPr>
   <dimension ref="A1:S94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="I94" sqref="I94"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17001,13 +16998,13 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="27" t="s">
+        <v>2572</v>
+      </c>
+      <c r="B94" s="26" t="s">
         <v>2578</v>
       </c>
-      <c r="B94" s="26" t="s">
+      <c r="C94" s="26" t="s">
         <v>2579</v>
-      </c>
-      <c r="C94" s="26" t="s">
-        <v>2580</v>
       </c>
       <c r="D94" s="26" t="s">
         <v>2552</v>

</xml_diff>

<commit_message>
Added 3 Gravel Cannon Types
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DRZ170000\Desktop\polycraftforge\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjg150230\PolycraftForge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2642" uniqueCount="2580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2646" uniqueCount="2582">
   <si>
     <t>Ore</t>
   </si>
@@ -7781,6 +7781,12 @@
   </si>
   <si>
     <t>HPBlock</t>
+  </si>
+  <si>
+    <t>1hS</t>
+  </si>
+  <si>
+    <t>GravelCannonBall</t>
   </si>
 </sst>
 </file>
@@ -14203,10 +14209,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:S94"/>
+  <dimension ref="A1:S95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+      <selection activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17013,6 +17019,26 @@
         <v>0</v>
       </c>
       <c r="H94" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A95" s="27" t="s">
+        <v>2572</v>
+      </c>
+      <c r="B95" s="26" t="s">
+        <v>2580</v>
+      </c>
+      <c r="C95" s="26" t="s">
+        <v>2581</v>
+      </c>
+      <c r="D95" s="26" t="s">
+        <v>1963</v>
+      </c>
+      <c r="F95" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H95" s="26">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reserve Game ID for special permission blocks
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2642" uniqueCount="2581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2650" uniqueCount="2585">
   <si>
     <t>Ore</t>
   </si>
@@ -7784,6 +7784,18 @@
   </si>
   <si>
     <t>HPBlock</t>
+  </si>
+  <si>
+    <t>1jB</t>
+  </si>
+  <si>
+    <t>1jA</t>
+  </si>
+  <si>
+    <t>PlaceBlockPP</t>
+  </si>
+  <si>
+    <t>BreakBlockPP</t>
   </si>
 </sst>
 </file>
@@ -14206,10 +14218,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:S94"/>
+  <dimension ref="A1:S96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="I94" sqref="I94"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17016,6 +17028,46 @@
         <v>0</v>
       </c>
       <c r="H94" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A95" s="27" t="s">
+        <v>2578</v>
+      </c>
+      <c r="B95" s="13" t="s">
+        <v>2582</v>
+      </c>
+      <c r="C95" s="26" t="s">
+        <v>2583</v>
+      </c>
+      <c r="D95" s="26" t="s">
+        <v>2552</v>
+      </c>
+      <c r="F95" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H95" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A96" s="27" t="s">
+        <v>2578</v>
+      </c>
+      <c r="B96" s="13" t="s">
+        <v>2581</v>
+      </c>
+      <c r="C96" s="26" t="s">
+        <v>2584</v>
+      </c>
+      <c r="D96" s="26" t="s">
+        <v>2552</v>
+      </c>
+      <c r="F96" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H96" s="26">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added BreakBlock and PlaceBlock
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2650" uniqueCount="2585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2650" uniqueCount="2584">
   <si>
     <t>Ore</t>
   </si>
@@ -7777,9 +7777,6 @@
     <t>Tool</t>
   </si>
   <si>
-    <t>1.4.13</t>
-  </si>
-  <si>
     <t>1hH</t>
   </si>
   <si>
@@ -7792,10 +7789,10 @@
     <t>1jA</t>
   </si>
   <si>
-    <t>PlaceBlockPP</t>
-  </si>
-  <si>
-    <t>BreakBlockPP</t>
+    <t>Place Block</t>
+  </si>
+  <si>
+    <t>Break Block</t>
   </si>
 </sst>
 </file>
@@ -14221,7 +14218,7 @@
   <dimension ref="A1:S96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="F90" sqref="F90"/>
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17013,13 +17010,13 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="27" t="s">
+        <v>2572</v>
+      </c>
+      <c r="B94" s="26" t="s">
         <v>2578</v>
       </c>
-      <c r="B94" s="26" t="s">
+      <c r="C94" s="26" t="s">
         <v>2579</v>
-      </c>
-      <c r="C94" s="26" t="s">
-        <v>2580</v>
       </c>
       <c r="D94" s="26" t="s">
         <v>2552</v>
@@ -17033,13 +17030,13 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="27" t="s">
-        <v>2578</v>
+        <v>2572</v>
       </c>
       <c r="B95" s="13" t="s">
+        <v>2581</v>
+      </c>
+      <c r="C95" s="26" t="s">
         <v>2582</v>
-      </c>
-      <c r="C95" s="26" t="s">
-        <v>2583</v>
       </c>
       <c r="D95" s="26" t="s">
         <v>2552</v>
@@ -17053,13 +17050,13 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="27" t="s">
-        <v>2578</v>
+        <v>2572</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>2581</v>
+        <v>2580</v>
       </c>
       <c r="C96" s="26" t="s">
-        <v>2584</v>
+        <v>2583</v>
       </c>
       <c r="D96" s="26" t="s">
         <v>2552</v>

</xml_diff>

<commit_message>
Fixed config merge conflicts
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjg150230\PolycraftForge\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjg150230\Desktop\New folder (5)\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2650" uniqueCount="2584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2692" uniqueCount="2605">
   <si>
     <t>Ore</t>
   </si>
@@ -7793,6 +7793,69 @@
   </si>
   <si>
     <t>Break Block</t>
+  </si>
+  <si>
+    <t>1hJ</t>
+  </si>
+  <si>
+    <t>Paintpellet</t>
+  </si>
+  <si>
+    <t>1hK</t>
+  </si>
+  <si>
+    <t>Wood Slingshot</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>Velocity, Cooldown, PelletTypeUsed, NumberOfPelletsUsed, Damage</t>
+  </si>
+  <si>
+    <t>1.4.13</t>
+  </si>
+  <si>
+    <t>1hM</t>
+  </si>
+  <si>
+    <t>Tactical Slingshot</t>
+  </si>
+  <si>
+    <t>1hN</t>
+  </si>
+  <si>
+    <t>Scatter Slingshot</t>
+  </si>
+  <si>
+    <t>1hO</t>
+  </si>
+  <si>
+    <t>Burst Slingshot</t>
+  </si>
+  <si>
+    <t>1hP</t>
+  </si>
+  <si>
+    <t>Gravity Slingshot</t>
+  </si>
+  <si>
+    <t>1hQ</t>
+  </si>
+  <si>
+    <t>Ice Slingshot</t>
+  </si>
+  <si>
+    <t>1hL</t>
+  </si>
+  <si>
+    <t>Paintball</t>
+  </si>
+  <si>
+    <t>1hS</t>
+  </si>
+  <si>
+    <t>GravelCannonBall</t>
   </si>
 </sst>
 </file>
@@ -14215,10 +14278,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:S96"/>
+  <dimension ref="A1:S105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17065,6 +17128,294 @@
         <v>0</v>
       </c>
       <c r="H96" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A97" s="27" t="s">
+        <v>2572</v>
+      </c>
+      <c r="B97" s="26" t="s">
+        <v>2603</v>
+      </c>
+      <c r="C97" s="26" t="s">
+        <v>2604</v>
+      </c>
+      <c r="D97" s="26" t="s">
+        <v>1963</v>
+      </c>
+      <c r="F97" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H97" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A98" s="27" t="s">
+        <v>2572</v>
+      </c>
+      <c r="B98" s="26" t="s">
+        <v>2584</v>
+      </c>
+      <c r="C98" s="26" t="s">
+        <v>2585</v>
+      </c>
+      <c r="D98" s="26" t="s">
+        <v>1963</v>
+      </c>
+      <c r="F98" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H98" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A99" s="27" t="s">
+        <v>2572</v>
+      </c>
+      <c r="B99" s="26" t="s">
+        <v>2586</v>
+      </c>
+      <c r="C99" s="26" t="s">
+        <v>2587</v>
+      </c>
+      <c r="D99" s="26" t="s">
+        <v>2588</v>
+      </c>
+      <c r="F99" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H99" s="26">
+        <v>1</v>
+      </c>
+      <c r="J99" s="26" t="s">
+        <v>2589</v>
+      </c>
+      <c r="K99" s="26">
+        <v>1</v>
+      </c>
+      <c r="L99" s="26">
+        <v>0</v>
+      </c>
+      <c r="M99" s="26">
+        <v>0</v>
+      </c>
+      <c r="N99" s="26">
+        <v>1</v>
+      </c>
+      <c r="O99" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A100" s="27" t="s">
+        <v>2590</v>
+      </c>
+      <c r="B100" s="26" t="s">
+        <v>2591</v>
+      </c>
+      <c r="C100" s="26" t="s">
+        <v>2592</v>
+      </c>
+      <c r="D100" s="26" t="s">
+        <v>2588</v>
+      </c>
+      <c r="F100" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H100" s="26">
+        <v>1</v>
+      </c>
+      <c r="J100" s="26" t="s">
+        <v>2589</v>
+      </c>
+      <c r="K100" s="26">
+        <v>2</v>
+      </c>
+      <c r="L100" s="26">
+        <v>3</v>
+      </c>
+      <c r="M100" s="26">
+        <v>1</v>
+      </c>
+      <c r="N100" s="26">
+        <v>1</v>
+      </c>
+      <c r="O100" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A101" s="27" t="s">
+        <v>2590</v>
+      </c>
+      <c r="B101" s="26" t="s">
+        <v>2593</v>
+      </c>
+      <c r="C101" s="26" t="s">
+        <v>2594</v>
+      </c>
+      <c r="D101" s="26" t="s">
+        <v>2588</v>
+      </c>
+      <c r="F101" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H101" s="26">
+        <v>1</v>
+      </c>
+      <c r="J101" s="26" t="s">
+        <v>2589</v>
+      </c>
+      <c r="K101" s="26">
+        <v>1</v>
+      </c>
+      <c r="L101" s="26">
+        <v>2</v>
+      </c>
+      <c r="M101" s="26">
+        <v>1</v>
+      </c>
+      <c r="N101" s="26">
+        <v>3</v>
+      </c>
+      <c r="O101" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A102" s="27" t="s">
+        <v>2590</v>
+      </c>
+      <c r="B102" s="26" t="s">
+        <v>2595</v>
+      </c>
+      <c r="C102" s="26" t="s">
+        <v>2596</v>
+      </c>
+      <c r="D102" s="26" t="s">
+        <v>2588</v>
+      </c>
+      <c r="F102" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H102" s="26">
+        <v>1</v>
+      </c>
+      <c r="J102" s="26" t="s">
+        <v>2589</v>
+      </c>
+      <c r="K102" s="26">
+        <v>1.25</v>
+      </c>
+      <c r="L102" s="26">
+        <v>2</v>
+      </c>
+      <c r="M102" s="26">
+        <v>1</v>
+      </c>
+      <c r="N102" s="26">
+        <v>3</v>
+      </c>
+      <c r="O102" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A103" s="27" t="s">
+        <v>2590</v>
+      </c>
+      <c r="B103" s="26" t="s">
+        <v>2597</v>
+      </c>
+      <c r="C103" s="26" t="s">
+        <v>2598</v>
+      </c>
+      <c r="D103" s="26" t="s">
+        <v>2588</v>
+      </c>
+      <c r="F103" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H103" s="26">
+        <v>1</v>
+      </c>
+      <c r="J103" s="26" t="s">
+        <v>2589</v>
+      </c>
+      <c r="K103" s="26">
+        <v>0.85</v>
+      </c>
+      <c r="L103" s="26">
+        <v>3</v>
+      </c>
+      <c r="M103" s="26">
+        <v>0</v>
+      </c>
+      <c r="N103" s="26">
+        <v>1</v>
+      </c>
+      <c r="O103" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A104" s="27" t="s">
+        <v>2590</v>
+      </c>
+      <c r="B104" s="26" t="s">
+        <v>2599</v>
+      </c>
+      <c r="C104" s="26" t="s">
+        <v>2600</v>
+      </c>
+      <c r="D104" s="26" t="s">
+        <v>2588</v>
+      </c>
+      <c r="F104" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H104" s="26">
+        <v>1</v>
+      </c>
+      <c r="J104" s="26" t="s">
+        <v>2589</v>
+      </c>
+      <c r="K104" s="26">
+        <v>1</v>
+      </c>
+      <c r="L104" s="26">
+        <v>3</v>
+      </c>
+      <c r="M104" s="26">
+        <v>0</v>
+      </c>
+      <c r="N104" s="26">
+        <v>1</v>
+      </c>
+      <c r="O104" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A105" s="27" t="s">
+        <v>2590</v>
+      </c>
+      <c r="B105" s="26" t="s">
+        <v>2601</v>
+      </c>
+      <c r="C105" s="26" t="s">
+        <v>2602</v>
+      </c>
+      <c r="D105" s="26" t="s">
+        <v>1963</v>
+      </c>
+      <c r="F105" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H105" s="26">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Registering AI Tool ID
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjg150230\Desktop\New folder (5)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjg150230\1.8.9 PolycraftForge\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2692" uniqueCount="2605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="2607">
   <si>
     <t>Ore</t>
   </si>
@@ -7856,6 +7856,12 @@
   </si>
   <si>
     <t>GravelCannonBall</t>
+  </si>
+  <si>
+    <t>1k0</t>
+  </si>
+  <si>
+    <t>AI Tool</t>
   </si>
 </sst>
 </file>
@@ -14278,10 +14284,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:S105"/>
+  <dimension ref="A1:S106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17417,6 +17423,26 @@
       </c>
       <c r="H105" s="26">
         <v>64</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A106" s="27" t="s">
+        <v>2590</v>
+      </c>
+      <c r="B106" s="26" t="s">
+        <v>2605</v>
+      </c>
+      <c r="C106" s="26" t="s">
+        <v>2606</v>
+      </c>
+      <c r="D106" s="26" t="s">
+        <v>1963</v>
+      </c>
+      <c r="F106" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H106" s="26">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add geometric resoning game blocks
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjg150230\1.8.9 PolycraftForge\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxg115630\Desktop\Polycraft forge 1.8.9\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="2607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2723" uniqueCount="2634">
   <si>
     <t>Ore</t>
   </si>
@@ -7759,9 +7759,6 @@
     <t>Armor</t>
   </si>
   <si>
-    <t>1.4.12</t>
-  </si>
-  <si>
     <t>1hF</t>
   </si>
   <si>
@@ -7813,9 +7810,6 @@
     <t>Velocity, Cooldown, PelletTypeUsed, NumberOfPelletsUsed, Damage</t>
   </si>
   <si>
-    <t>1.4.13</t>
-  </si>
-  <si>
     <t>1hM</t>
   </si>
   <si>
@@ -7862,6 +7856,93 @@
   </si>
   <si>
     <t>AI Tool</t>
+  </si>
+  <si>
+    <t>1ke</t>
+  </si>
+  <si>
+    <t>1kd</t>
+  </si>
+  <si>
+    <t>1kc</t>
+  </si>
+  <si>
+    <t>1kb</t>
+  </si>
+  <si>
+    <t>1ka</t>
+  </si>
+  <si>
+    <t>1k9</t>
+  </si>
+  <si>
+    <t>1k8</t>
+  </si>
+  <si>
+    <t>1k7</t>
+  </si>
+  <si>
+    <t>1k6</t>
+  </si>
+  <si>
+    <t>1k5</t>
+  </si>
+  <si>
+    <t>1k4</t>
+  </si>
+  <si>
+    <t>1k3</t>
+  </si>
+  <si>
+    <t>1k2</t>
+  </si>
+  <si>
+    <t>1k1</t>
+  </si>
+  <si>
+    <t>A Block</t>
+  </si>
+  <si>
+    <t>B Block</t>
+  </si>
+  <si>
+    <t>C Block</t>
+  </si>
+  <si>
+    <t>D Block</t>
+  </si>
+  <si>
+    <t>5 Block</t>
+  </si>
+  <si>
+    <t>7 Block</t>
+  </si>
+  <si>
+    <t>Geometry Grey Corner</t>
+  </si>
+  <si>
+    <t>Geometry Grey Side</t>
+  </si>
+  <si>
+    <t>Geometry Slope2</t>
+  </si>
+  <si>
+    <t>Geometry Slope3</t>
+  </si>
+  <si>
+    <t>Geometry Slope3 Grey</t>
+  </si>
+  <si>
+    <t>L Block</t>
+  </si>
+  <si>
+    <t>X Block</t>
+  </si>
+  <si>
+    <t>PC Directional</t>
+  </si>
+  <si>
+    <t>Geometry Slope1</t>
   </si>
 </sst>
 </file>
@@ -8082,7 +8163,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -8149,7 +8230,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -8474,6 +8554,21 @@
         <row r="169">
           <cell r="A169" t="str">
             <v>1.4.10</v>
+          </cell>
+        </row>
+        <row r="171">
+          <cell r="A171" t="str">
+            <v>1.4.12</v>
+          </cell>
+        </row>
+        <row r="172">
+          <cell r="A172" t="str">
+            <v>1.4.13</v>
+          </cell>
+        </row>
+        <row r="173">
+          <cell r="A173" t="str">
+            <v>1.4.14</v>
           </cell>
         </row>
       </sheetData>
@@ -14284,10 +14379,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:S106"/>
+  <dimension ref="A1:S120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17037,55 +17132,58 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="42" t="s">
+    <row r="92" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="str">
+        <f>[1]Enums!$A$171</f>
+        <v>1.4.12</v>
+      </c>
+      <c r="B92" s="42" t="s">
         <v>2572</v>
       </c>
-      <c r="B92" s="43" t="s">
+      <c r="C92" s="42" t="s">
         <v>2573</v>
       </c>
-      <c r="C92" s="43" t="s">
+      <c r="D92" s="42" t="s">
+        <v>1963</v>
+      </c>
+      <c r="F92" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="H92" s="42">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="4" t="str">
+        <f>[1]Enums!$A$171</f>
+        <v>1.4.12</v>
+      </c>
+      <c r="B93" s="14" t="s">
         <v>2574</v>
       </c>
-      <c r="D92" s="43" t="s">
-        <v>1963</v>
-      </c>
-      <c r="F92" s="43" t="b">
+      <c r="C93" s="42" t="s">
+        <v>2575</v>
+      </c>
+      <c r="D93" s="42" t="s">
+        <v>2576</v>
+      </c>
+      <c r="F93" s="42" t="b">
         <v>0</v>
       </c>
-      <c r="H92" s="43">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="42" t="s">
-        <v>2572</v>
-      </c>
-      <c r="B93" s="14" t="s">
-        <v>2575</v>
-      </c>
-      <c r="C93" s="43" t="s">
-        <v>2576</v>
-      </c>
-      <c r="D93" s="43" t="s">
+      <c r="H93" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A94" s="4" t="str">
+        <f>[1]Enums!$A$171</f>
+        <v>1.4.12</v>
+      </c>
+      <c r="B94" s="26" t="s">
         <v>2577</v>
       </c>
-      <c r="F93" s="43" t="b">
-        <v>0</v>
-      </c>
-      <c r="H93" s="43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A94" s="27" t="s">
-        <v>2572</v>
-      </c>
-      <c r="B94" s="26" t="s">
+      <c r="C94" s="26" t="s">
         <v>2578</v>
-      </c>
-      <c r="C94" s="26" t="s">
-        <v>2579</v>
       </c>
       <c r="D94" s="26" t="s">
         <v>2552</v>
@@ -17098,14 +17196,15 @@
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A95" s="27" t="s">
-        <v>2572</v>
+      <c r="A95" s="4" t="str">
+        <f>[1]Enums!$A$171</f>
+        <v>1.4.12</v>
       </c>
       <c r="B95" s="13" t="s">
+        <v>2580</v>
+      </c>
+      <c r="C95" s="26" t="s">
         <v>2581</v>
-      </c>
-      <c r="C95" s="26" t="s">
-        <v>2582</v>
       </c>
       <c r="D95" s="26" t="s">
         <v>2552</v>
@@ -17118,14 +17217,15 @@
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A96" s="27" t="s">
-        <v>2572</v>
+      <c r="A96" s="4" t="str">
+        <f>[1]Enums!$A$171</f>
+        <v>1.4.12</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>2580</v>
+        <v>2579</v>
       </c>
       <c r="C96" s="26" t="s">
-        <v>2583</v>
+        <v>2582</v>
       </c>
       <c r="D96" s="26" t="s">
         <v>2552</v>
@@ -17138,14 +17238,15 @@
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A97" s="27" t="s">
-        <v>2572</v>
+      <c r="A97" s="4" t="str">
+        <f>[1]Enums!$A$171</f>
+        <v>1.4.12</v>
       </c>
       <c r="B97" s="26" t="s">
-        <v>2603</v>
+        <v>2601</v>
       </c>
       <c r="C97" s="26" t="s">
-        <v>2604</v>
+        <v>2602</v>
       </c>
       <c r="D97" s="26" t="s">
         <v>1963</v>
@@ -17158,14 +17259,15 @@
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A98" s="27" t="s">
-        <v>2572</v>
+      <c r="A98" s="4" t="str">
+        <f>[1]Enums!$A$171</f>
+        <v>1.4.12</v>
       </c>
       <c r="B98" s="26" t="s">
+        <v>2583</v>
+      </c>
+      <c r="C98" s="26" t="s">
         <v>2584</v>
-      </c>
-      <c r="C98" s="26" t="s">
-        <v>2585</v>
       </c>
       <c r="D98" s="26" t="s">
         <v>1963</v>
@@ -17178,17 +17280,18 @@
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A99" s="27" t="s">
-        <v>2572</v>
+      <c r="A99" s="4" t="str">
+        <f>[1]Enums!$A$171</f>
+        <v>1.4.12</v>
       </c>
       <c r="B99" s="26" t="s">
+        <v>2585</v>
+      </c>
+      <c r="C99" s="26" t="s">
         <v>2586</v>
       </c>
-      <c r="C99" s="26" t="s">
+      <c r="D99" s="26" t="s">
         <v>2587</v>
-      </c>
-      <c r="D99" s="26" t="s">
-        <v>2588</v>
       </c>
       <c r="F99" s="26" t="b">
         <v>0</v>
@@ -17197,7 +17300,7 @@
         <v>1</v>
       </c>
       <c r="J99" s="26" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
       <c r="K99" s="26">
         <v>1</v>
@@ -17216,17 +17319,18 @@
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A100" s="27" t="s">
+      <c r="A100" s="4" t="str">
+        <f>[1]Enums!$A$172</f>
+        <v>1.4.13</v>
+      </c>
+      <c r="B100" s="26" t="s">
+        <v>2589</v>
+      </c>
+      <c r="C100" s="26" t="s">
         <v>2590</v>
       </c>
-      <c r="B100" s="26" t="s">
-        <v>2591</v>
-      </c>
-      <c r="C100" s="26" t="s">
-        <v>2592</v>
-      </c>
       <c r="D100" s="26" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
       <c r="F100" s="26" t="b">
         <v>0</v>
@@ -17235,7 +17339,7 @@
         <v>1</v>
       </c>
       <c r="J100" s="26" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
       <c r="K100" s="26">
         <v>2</v>
@@ -17254,17 +17358,18 @@
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A101" s="27" t="s">
-        <v>2590</v>
+      <c r="A101" s="4" t="str">
+        <f>[1]Enums!$A$172</f>
+        <v>1.4.13</v>
       </c>
       <c r="B101" s="26" t="s">
-        <v>2593</v>
+        <v>2591</v>
       </c>
       <c r="C101" s="26" t="s">
-        <v>2594</v>
+        <v>2592</v>
       </c>
       <c r="D101" s="26" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
       <c r="F101" s="26" t="b">
         <v>0</v>
@@ -17273,7 +17378,7 @@
         <v>1</v>
       </c>
       <c r="J101" s="26" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
       <c r="K101" s="26">
         <v>1</v>
@@ -17292,17 +17397,18 @@
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A102" s="27" t="s">
-        <v>2590</v>
+      <c r="A102" s="4" t="str">
+        <f>[1]Enums!$A$172</f>
+        <v>1.4.13</v>
       </c>
       <c r="B102" s="26" t="s">
-        <v>2595</v>
+        <v>2593</v>
       </c>
       <c r="C102" s="26" t="s">
-        <v>2596</v>
+        <v>2594</v>
       </c>
       <c r="D102" s="26" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
       <c r="F102" s="26" t="b">
         <v>0</v>
@@ -17311,7 +17417,7 @@
         <v>1</v>
       </c>
       <c r="J102" s="26" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
       <c r="K102" s="26">
         <v>1.25</v>
@@ -17330,17 +17436,18 @@
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A103" s="27" t="s">
-        <v>2590</v>
+      <c r="A103" s="4" t="str">
+        <f>[1]Enums!$A$172</f>
+        <v>1.4.13</v>
       </c>
       <c r="B103" s="26" t="s">
-        <v>2597</v>
+        <v>2595</v>
       </c>
       <c r="C103" s="26" t="s">
-        <v>2598</v>
+        <v>2596</v>
       </c>
       <c r="D103" s="26" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
       <c r="F103" s="26" t="b">
         <v>0</v>
@@ -17349,7 +17456,7 @@
         <v>1</v>
       </c>
       <c r="J103" s="26" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
       <c r="K103" s="26">
         <v>0.85</v>
@@ -17368,17 +17475,18 @@
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A104" s="27" t="s">
-        <v>2590</v>
+      <c r="A104" s="4" t="str">
+        <f>[1]Enums!$A$172</f>
+        <v>1.4.13</v>
       </c>
       <c r="B104" s="26" t="s">
-        <v>2599</v>
+        <v>2597</v>
       </c>
       <c r="C104" s="26" t="s">
-        <v>2600</v>
+        <v>2598</v>
       </c>
       <c r="D104" s="26" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
       <c r="F104" s="26" t="b">
         <v>0</v>
@@ -17387,7 +17495,7 @@
         <v>1</v>
       </c>
       <c r="J104" s="26" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
       <c r="K104" s="26">
         <v>1</v>
@@ -17406,14 +17514,15 @@
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A105" s="27" t="s">
-        <v>2590</v>
+      <c r="A105" s="4" t="str">
+        <f>[1]Enums!$A$172</f>
+        <v>1.4.13</v>
       </c>
       <c r="B105" s="26" t="s">
-        <v>2601</v>
+        <v>2599</v>
       </c>
       <c r="C105" s="26" t="s">
-        <v>2602</v>
+        <v>2600</v>
       </c>
       <c r="D105" s="26" t="s">
         <v>1963</v>
@@ -17426,14 +17535,15 @@
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A106" s="27" t="s">
-        <v>2590</v>
+      <c r="A106" s="4" t="str">
+        <f>[1]Enums!$A$172</f>
+        <v>1.4.13</v>
       </c>
       <c r="B106" s="26" t="s">
-        <v>2605</v>
+        <v>2603</v>
       </c>
       <c r="C106" s="26" t="s">
-        <v>2606</v>
+        <v>2604</v>
       </c>
       <c r="D106" s="26" t="s">
         <v>1963</v>
@@ -17443,6 +17553,300 @@
       </c>
       <c r="H106" s="26">
         <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A107" s="4" t="str">
+        <f>[1]Enums!$A$173</f>
+        <v>1.4.14</v>
+      </c>
+      <c r="B107" s="13" t="s">
+        <v>2618</v>
+      </c>
+      <c r="C107" s="26" t="s">
+        <v>2619</v>
+      </c>
+      <c r="D107" s="26" t="s">
+        <v>2632</v>
+      </c>
+      <c r="F107" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H107" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A108" s="4" t="str">
+        <f>[1]Enums!$A$173</f>
+        <v>1.4.14</v>
+      </c>
+      <c r="B108" s="13" t="s">
+        <v>2617</v>
+      </c>
+      <c r="C108" s="26" t="s">
+        <v>2620</v>
+      </c>
+      <c r="D108" s="26" t="s">
+        <v>2632</v>
+      </c>
+      <c r="F108" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H108" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A109" s="4" t="str">
+        <f>[1]Enums!$A$173</f>
+        <v>1.4.14</v>
+      </c>
+      <c r="B109" s="13" t="s">
+        <v>2616</v>
+      </c>
+      <c r="C109" s="26" t="s">
+        <v>2621</v>
+      </c>
+      <c r="D109" s="26" t="s">
+        <v>2632</v>
+      </c>
+      <c r="F109" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H109" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A110" s="4" t="str">
+        <f>[1]Enums!$A$173</f>
+        <v>1.4.14</v>
+      </c>
+      <c r="B110" s="13" t="s">
+        <v>2615</v>
+      </c>
+      <c r="C110" s="26" t="s">
+        <v>2622</v>
+      </c>
+      <c r="D110" s="26" t="s">
+        <v>2632</v>
+      </c>
+      <c r="F110" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H110" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A111" s="4" t="str">
+        <f>[1]Enums!$A$173</f>
+        <v>1.4.14</v>
+      </c>
+      <c r="B111" s="13" t="s">
+        <v>2614</v>
+      </c>
+      <c r="C111" s="26" t="s">
+        <v>2630</v>
+      </c>
+      <c r="D111" s="26" t="s">
+        <v>2632</v>
+      </c>
+      <c r="F111" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H111" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A112" s="4" t="str">
+        <f>[1]Enums!$A$173</f>
+        <v>1.4.14</v>
+      </c>
+      <c r="B112" s="13" t="s">
+        <v>2613</v>
+      </c>
+      <c r="C112" s="26" t="s">
+        <v>2631</v>
+      </c>
+      <c r="D112" s="26" t="s">
+        <v>2632</v>
+      </c>
+      <c r="F112" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H112" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" s="4" t="str">
+        <f>[1]Enums!$A$173</f>
+        <v>1.4.14</v>
+      </c>
+      <c r="B113" s="13" t="s">
+        <v>2612</v>
+      </c>
+      <c r="C113" s="26" t="s">
+        <v>2623</v>
+      </c>
+      <c r="D113" s="26" t="s">
+        <v>2632</v>
+      </c>
+      <c r="F113" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H113" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" s="4" t="str">
+        <f>[1]Enums!$A$173</f>
+        <v>1.4.14</v>
+      </c>
+      <c r="B114" s="13" t="s">
+        <v>2611</v>
+      </c>
+      <c r="C114" s="26" t="s">
+        <v>2624</v>
+      </c>
+      <c r="D114" s="26" t="s">
+        <v>2632</v>
+      </c>
+      <c r="F114" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H114" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="4" t="str">
+        <f>[1]Enums!$A$173</f>
+        <v>1.4.14</v>
+      </c>
+      <c r="B115" s="13" t="s">
+        <v>2610</v>
+      </c>
+      <c r="C115" s="26" t="s">
+        <v>2625</v>
+      </c>
+      <c r="D115" s="26" t="s">
+        <v>2632</v>
+      </c>
+      <c r="F115" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H115" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" s="4" t="str">
+        <f>[1]Enums!$A$173</f>
+        <v>1.4.14</v>
+      </c>
+      <c r="B116" s="13" t="s">
+        <v>2609</v>
+      </c>
+      <c r="C116" s="26" t="s">
+        <v>2626</v>
+      </c>
+      <c r="D116" s="26" t="s">
+        <v>2632</v>
+      </c>
+      <c r="F116" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H116" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" s="4" t="str">
+        <f>[1]Enums!$A$173</f>
+        <v>1.4.14</v>
+      </c>
+      <c r="B117" s="13" t="s">
+        <v>2608</v>
+      </c>
+      <c r="C117" s="26" t="s">
+        <v>2633</v>
+      </c>
+      <c r="D117" s="26" t="s">
+        <v>2632</v>
+      </c>
+      <c r="F117" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H117" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" s="4" t="str">
+        <f>[1]Enums!$A$173</f>
+        <v>1.4.14</v>
+      </c>
+      <c r="B118" s="13" t="s">
+        <v>2607</v>
+      </c>
+      <c r="C118" s="26" t="s">
+        <v>2627</v>
+      </c>
+      <c r="D118" s="26" t="s">
+        <v>2632</v>
+      </c>
+      <c r="F118" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H118" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" s="4" t="str">
+        <f>[1]Enums!$A$173</f>
+        <v>1.4.14</v>
+      </c>
+      <c r="B119" s="13" t="s">
+        <v>2606</v>
+      </c>
+      <c r="C119" s="26" t="s">
+        <v>2628</v>
+      </c>
+      <c r="D119" s="26" t="s">
+        <v>2632</v>
+      </c>
+      <c r="F119" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H119" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120" s="4" t="str">
+        <f>[1]Enums!$A$173</f>
+        <v>1.4.14</v>
+      </c>
+      <c r="B120" s="13" t="s">
+        <v>2605</v>
+      </c>
+      <c r="C120" s="26" t="s">
+        <v>2629</v>
+      </c>
+      <c r="D120" s="26" t="s">
+        <v>2632</v>
+      </c>
+      <c r="F120" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H120" s="26">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tickmark and white background
</commit_message>
<xml_diff>
--- a/config/Polycraft Materials.xlsx
+++ b/config/Polycraft Materials.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2723" uniqueCount="2634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2729" uniqueCount="2638">
   <si>
     <t>Ore</t>
   </si>
@@ -7943,6 +7943,18 @@
   </si>
   <si>
     <t>Geometry Slope1</t>
+  </si>
+  <si>
+    <t>tickmark</t>
+  </si>
+  <si>
+    <t>whitebg</t>
+  </si>
+  <si>
+    <t>1kf</t>
+  </si>
+  <si>
+    <t>1kg</t>
   </si>
 </sst>
 </file>
@@ -14379,10 +14391,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:S120"/>
+  <dimension ref="A1:S122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="H122" sqref="A120:H122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17846,6 +17858,48 @@
         <v>0</v>
       </c>
       <c r="H120" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A121" s="4" t="str">
+        <f>[1]Enums!$A$173</f>
+        <v>1.4.14</v>
+      </c>
+      <c r="B121" s="13" t="s">
+        <v>2636</v>
+      </c>
+      <c r="C121" s="26" t="s">
+        <v>2634</v>
+      </c>
+      <c r="D121" s="26" t="s">
+        <v>2632</v>
+      </c>
+      <c r="F121" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H121" s="26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A122" s="4" t="str">
+        <f>[1]Enums!$A$173</f>
+        <v>1.4.14</v>
+      </c>
+      <c r="B122" s="13" t="s">
+        <v>2637</v>
+      </c>
+      <c r="C122" s="26" t="s">
+        <v>2635</v>
+      </c>
+      <c r="D122" s="26" t="s">
+        <v>2632</v>
+      </c>
+      <c r="F122" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H122" s="26">
         <v>64</v>
       </c>
     </row>

</xml_diff>